<commit_message>
Rumble Racing, Country Chase initial code
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$95</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -886,10 +886,10 @@
     <t xml:space="preserve">Fruitball Course</t>
   </si>
   <si>
-    <t xml:space="preserve">DisneyCourseA</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Racecourse A</t>
+    <t xml:space="preserve">DisneyCountryChase</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Country Chase</t>
   </si>
   <si>
     <t xml:space="preserve">DisneyRaceway</t>
@@ -2625,10 +2625,10 @@
   <dimension ref="A1:C24"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C2" activeCellId="1" sqref="H2:H213 C2"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.640625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -2920,11 +2920,11 @@
   </sheetPr>
   <dimension ref="A1:I212"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D57" activeCellId="1" sqref="H2:H213 D57"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E7" activeCellId="0" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -2958,7 +2958,7 @@
       </c>
       <c r="I1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1000)</f>
-        <v>0: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },1: { "worldId": 1, "name": "DepartureForecourtDay", "display": "Forecourt", "areaId": 1, "hideWorld": 0, },2: { "worldId": 1, "name": "DepartureGreatHall", "display": "Great Hall", "areaId": 2, "hideWorld": 0, },3: { "worldId": 1, "name": "VentusRoomDay", "display": "Ventus’s Room", "areaId": 3, "hideWorld": 0, },4: { "worldId": 1, "name": "VentusRoomNight", "display": "Ventus’s Room", "areaId": 4, "hideWorld": 0, },6: { "worldId": 1, "name": "DepartureMountainPath", "display": "Mountain Path", "areaId": 5, "hideWorld": 0, },7: { "worldId": 1, "name": "DepartureSummitNight", "display": "Summit", "areaId": 6, "hideWorld": 0, },8: { "worldId": 1, "name": "DepartureForecourtNight", "display": "Forecourt", "areaId": 7, "hideWorld": 0, },9: { "worldId": 1, "name": "DepartureForecourtRuins", "display": "Forecourt", "areaId": 8, "hideWorld": 0, },10: { "worldId": 1, "name": "DepartureGreatHallRuins", "display": "Great Hall", "areaId": 9, "hideWorld": 0, },11: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 10, "hideWorld": 0, },12: { "worldId": 1, "name": "ChamberOfWaking", "display": "Chamber of Waking", "areaId": 11, "hideWorld": 0, },13: { "worldId": 1, "name": "CastleOblivion", "display": "Castle Oblivion", "areaId": 12, "hideWorld": 0, },14: { "worldId": 1, "name": "CharacterSelect", "display": "Selecting a character…", "areaId": 13, "hideWorld": 1, },15: { "worldId": 1, "name": "DepartureForecourtRuins2", "display": "Forecourt", "areaId": 14, "hideWorld": 0, },16: { "worldId": 1, "name": "DepartureMountainPathRuins", "display": "Mountain Path", "areaId": 15, "hideWorld": 0, },17: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 16, "hideWorld": 0, },18: { "worldId": 2, "name": "DwarfMineEntrance", "display": "Mine Entrance", "areaId": 1, "hideWorld": 0, },19: { "worldId": 2, "name": "DwarfMine", "display": "The Mine", "areaId": 2, "hideWorld": 0, },20: { "worldId": 2, "name": "DwarfVault", "display": "Vault", "areaId": 3, "hideWorld": 0, },21: { "worldId": 2, "name": "DwarfMirrorChamber", "display": "Magic Mirror Chamber", "areaId": 4, "hideWorld": 0, },22: { "worldId": 2, "name": "DwarfWaterway", "display": "Underground Waterway", "areaId": 5, "hideWorld": 0, },23: { "worldId": 2, "name": "DwarfCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },24: { "worldId": 2, "name": "DwarfGlade", "display": "Flower Glade", "areaId": 7, "hideWorld": 0, },25: { "worldId": 2, "name": "DwarfWoods", "display": "Deep Woods", "areaId": 8, "hideWorld": 0, },26: { "worldId": 2, "name": "DwarfMirror", "display": "Inside the Magic Mirror", "areaId": 9, "hideWorld": 0, },27: { "worldId": 2, "name": "DwarfClearing", "display": "Cottage Clearing", "areaId": 10, "hideWorld": 0, },28: { "worldId": 2, "name": "DwarfCottage", "display": "The Cottage", "areaId": 11, "hideWorld": 0, },29: { "worldId": 2, "name": "DwarfMountainTrail", "display": "Mountain Trail", "areaId": 12, "hideWorld": 0, },30: { "worldId": 3, "name": "CastleHouse", "display": "Cinderella’s House", "areaId": 1, "hideWorld": 0, },31: { "worldId": 3, "name": "CastleMousehole", "display": "Mousehole", "areaId": 2, "hideWorld": 0, },32: { "worldId": 3, "name": "CastleWardrobe", "display": "Wardrobe Room", "areaId": 3, "hideWorld": 0, },33: { "worldId": 3, "name": "CastleEntrance", "display": "Entrance", "areaId": 4, "hideWorld": 0, },34: { "worldId": 3, "name": "CastleChateau", "display": "The Chateau", "areaId": 5, "hideWorld": 0, },35: { "worldId": 3, "name": "CastleForest", "display": "Forest", "areaId": 6, "hideWorld": 0, },36: { "worldId": 3, "name": "CastleCourtyard", "display": "Palace Courtyard", "areaId": 7, "hideWorld": 0, },37: { "worldId": 3, "name": "CastleCorridor", "display": "Corridor", "areaId": 8, "hideWorld": 0, },38: { "worldId": 3, "name": "CastleBallroom", "display": "Ballroom", "areaId": 9, "hideWorld": 0, },39: { "worldId": 3, "name": "CastleFoyer", "display": "Foyer", "areaId": 10, "hideWorld": 0, },40: { "worldId": 3, "name": "CastlePassage", "display": "Passage", "areaId": 11, "hideWorld": 0, },41: { "worldId": 3, "name": "CastleAntechamber", "display": "Antechamber", "areaId": 12, "hideWorld": 0, },42: { "worldId": 3, "name": "CastleWardrobe2", "display": "Wardrobe Room", "areaId": 13, "hideWorld": 0, },43: { "worldId": 3, "name": "CastleMousehole2", "display": "Mousehole", "areaId": 14, "hideWorld": 0, },44: { "worldId": 3, "name": "CastleWardrobe3", "display": "Wardrobe Room", "areaId": 15, "hideWorld": 0, },45: { "worldId": 4, "name": "EnchantedDungeonCell", "display": "Dungeon Cell", "areaId": 1, "hideWorld": 0, },46: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 2, "hideWorld": 0, },47: { "worldId": 4, "name": "EnchantedThrone", "display": "Maleficent’s Throne", "areaId": 3, "hideWorld": 0, },48: { "worldId": 4, "name": "EnchantedDungeon", "display": "Dungeon", "areaId": 4, "hideWorld": 0, },49: { "worldId": 4, "name": "EnchantedHall1", "display": "Hall", "areaId": 5, "hideWorld": 0, },50: { "worldId": 4, "name": "EnchantedMountain", "display": "Forbidden Mountain", "areaId": 6, "hideWorld": 0, },51: { "worldId": 4, "name": "EnchantedWaterside", "display": "Waterside", "areaId": 7, "hideWorld": 0, },52: { "worldId": 4, "name": "EnchantedClearing", "display": "Forest Clearing", "areaId": 8, "hideWorld": 0, },53: { "worldId": 4, "name": "EnchantedBridge", "display": "Bridge", "areaId": 9, "hideWorld": 0, },54: { "worldId": 4, "name": "EnchantedBridgeThorns", "display": "Bridge", "areaId": 10, "hideWorld": 0, },55: { "worldId": 4, "name": "EnchantedAudience1", "display": "Audience Chamber", "areaId": 11, "hideWorld": 0, },56: { "worldId": 4, "name": "EnchantedAudience2", "display": "Audience Chamber", "areaId": 12, "hideWorld": 0, },57: { "worldId": 4, "name": "EnchantedReserved", "display": "Somewhere in the World…", "areaId": 13, "hideWorld": 1, },58: { "worldId": 4, "name": "EnchantedHallway", "display": "Hallway", "areaId": 14, "hideWorld": 0, },59: { "worldId": 4, "name": "EnchantedAurora", "display": "Aurora’s Chamber", "areaId": 15, "hideWorld": 0, },60: { "worldId": 4, "name": "EnchantedTower", "display": "Tower Room", "areaId": 16, "hideWorld": 0, },61: { "worldId": 4, "name": "EnchantedHall2", "display": "Hall", "areaId": 17, "hideWorld": 0, },62: { "worldId": 4, "name": "EnchantedAurora2", "display": "Aurora’s Chamber", "areaId": 18, "hideWorld": 0, },63: { "worldId": 4, "name": "EnchantedHall3", "display": "Hall", "areaId": 19, "hideWorld": 0, },64: { "worldId": 4, "name": "EnchantedHall4", "display": "Hall", "areaId": 20, "hideWorld": 0, },65: { "worldId": 4, "name": "EnchantedHall5", "display": "Hall", "areaId": 21, "hideWorld": 0, },66: { "worldId": 4, "name": "EnchantedHall6", "display": "Hall", "areaId": 22, "hideWorld": 0, },67: { "worldId": 4, "name": "EnchantedHall7", "display": "Hall", "areaId": 23, "hideWorld": 0, },68: { "worldId": 4, "name": "EnchantedHall8", "display": "Hall", "areaId": 24, "hideWorld": 0, },69: { "worldId": 4, "name": "EnchantedHall9", "display": "Hall", "areaId": 25, "hideWorld": 0, },70: { "worldId": 4, "name": "EnchantedHall10", "display": "Hall", "areaId": 26, "hideWorld": 0, },71: { "worldId": 4, "name": "EnchantedHall11", "display": "Hall", "areaId": 27, "hideWorld": 0, },72: { "worldId": 4, "name": "EnchantedHall12", "display": "Hall", "areaId": 28, "hideWorld": 0, },73: { "worldId": 4, "name": "EnchantedHall13", "display": "Hall", "areaId": 29, "hideWorld": 0, },74: { "worldId": 4, "name": "EnchantedHall14", "display": "Hall", "areaId": 30, "hideWorld": 0, },75: { "worldId": 4, "name": "EnchantedHall15", "display": "Hall", "areaId": 31, "hideWorld": 0, },76: { "worldId": 4, "name": "EnchantedHall16", "display": "Hall", "areaId": 32, "hideWorld": 0, },77: { "worldId": 4, "name": "EnchantedHall17", "display": "Hall", "areaId": 33, "hideWorld": 0, },78: { "worldId": 4, "name": "EnchantedHall18", "display": "Hall", "areaId": 34, "hideWorld": 0, },79: { "worldId": 4, "name": "EnchantedHall19", "display": "Hall", "areaId": 35, "hideWorld": 0, },80: { "worldId": 4, "name": "EnchantedHall20", "display": "Hall", "areaId": 36, "hideWorld": 0, },81: { "worldId": 4, "name": "EnchantedHall21", "display": "Hall", "areaId": 37, "hideWorld": 0, },82: { "worldId": 4, "name": "EnchantedHall22", "display": "Hall", "areaId": 38, "hideWorld": 0, },83: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 39, "hideWorld": 0, },84: { "worldId": 5, "name": "MysteriousChamber", "display": "Sorcerer’s Chamber", "areaId": 1, "hideWorld": 0, },85: { "worldId": 5, "name": "MysteriousTower", "display": "Mysterious Tower", "areaId": 2, "hideWorld": 0, },86: { "worldId": 5, "name": "MysteriousEntrance", "display": "Tower Entrance", "areaId": 3, "hideWorld": 0, },87: { "worldId": 5, "name": "MysteriousChamber2", "display": "Sorcerer’s Chamber", "areaId": 4, "hideWorld": 0, },88: { "worldId": 6, "name": "RadiantOuterGardens", "display": "Outer Gardens", "areaId": 1, "hideWorld": 0, },89: { "worldId": 6, "name": "RadiantEntryway", "display": "Entryway", "areaId": 2, "hideWorld": 0, },90: { "worldId": 6, "name": "RadiantCentral", "display": "Central Square", "areaId": 3, "hideWorld": 0, },91: { "worldId": 6, "name": "RadiantAqueduct", "display": "Aqueduct", "areaId": 4, "hideWorld": 0, },92: { "worldId": 6, "name": "RadiantTown", "display": "Castle Town", "areaId": 5, "hideWorld": 0, },93: { "worldId": 6, "name": "RadiantReactor", "display": "Reactor", "areaId": 6, "hideWorld": 0, },94: { "worldId": 6, "name": "RadiantFountain", "display": "Fountain Court", "areaId": 7, "hideWorld": 0, },95: { "worldId": 6, "name": "RadiantMerlin", "display": "Merlin’s House", "areaId": 8, "hideWorld": 0, },96: { "worldId": 6, "name": "RadiantGardens", "display": "Gardens", "areaId": 9, "hideWorld": 0, },97: { "worldId": 6, "name": "RadiantDoors", "display": "Front Doors", "areaId": 10, "hideWorld": 0, },98: { "worldId": 6, "name": "RadiantPurification", "display": "Purification Facility", "areaId": 11, "hideWorld": 0, },99: { "worldId": 6, "name": "RadiantOuterGardens2", "display": "Outer Gardens", "areaId": 12, "hideWorld": 0, },100: { "worldId": 6, "name": "RadiantCentralDark", "display": "Central Square", "areaId": 13, "hideWorld": 0, },101: { "worldId": 6, "name": "RadiantCentralTerranort", "display": "Central Square", "areaId": 14, "hideWorld": 0, },102: { "worldId": 7, "name": "LouieCourt", "display": "Louie’s Ruins (Court)", "areaId": 1, "hideWorld": 0, },103: { "worldId": 7, "name": "LouiePath", "display": "Louie’s Ruins (Path)", "areaId": 2, "hideWorld": 0, },104: { "worldId": 7, "name": "Crossroad", "display": "Crossroad", "areaId": 3, "hideWorld": 0, },105: { "worldId": 7, "name": "UGRuinsEntrance", "display": "Underground Ruins (Entrance)", "areaId": 4, "hideWorld": 0, },106: { "worldId": 7, "name": "UGRuinsPassage1", "display": "Underground Ruins (Passage)", "areaId": 5, "hideWorld": 0, },107: { "worldId": 7, "name": "UGRuinsPassage2", "display": "Underground Ruins (Passage)", "areaId": 6, "hideWorld": 0, },108: { "worldId": 7, "name": "UGCourtyard", "display": "Underground Courtyard", "areaId": 7, "hideWorld": 0, },109: { "worldId": 7, "name": "JungleNearRuins", "display": "Jungle Near Ruins", "areaId": 8, "hideWorld": 0, },110: { "worldId": 7, "name": "Eminence", "display": "Eminence", "areaId": 9, "hideWorld": 0, },111: { "worldId": 7, "name": "Jungle", "display": "Jungle", "areaId": 10, "hideWorld": 0, },112: { "worldId": 7, "name": "River", "display": "Man-Village River", "areaId": 11, "hideWorld": 0, },113: { "worldId": 7, "name": "Bog", "display": "Bog", "areaId": 12, "hideWorld": 0, },114: { "worldId": 7, "name": "LanesBetween", "display": "The Lanes Between", "areaId": 50, "hideWorld": 0, },115: { "worldId": 7, "name": "Blank", "display": "Blank", "areaId": 51, "hideWorld": 0, },116: { "worldId": 7, "name": "Realm of Darkness", "display": "The Realm of Darkness", "areaId": 52, "hideWorld": 1, },117: { "worldId": 8, "name": "OlympusGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },118: { "worldId": 8, "name": "OlympusVestibule", "display": "Vestibule", "areaId": 2, "hideWorld": 0, },119: { "worldId": 8, "name": "OlympusWest", "display": "West Bracket", "areaId": 3, "hideWorld": 0, },120: { "worldId": 8, "name": "OlympusEast", "display": "East Bracket", "areaId": 4, "hideWorld": 0, },121: { "worldId": 8, "name": "OlympusTown", "display": "Town Near Thebes", "areaId": 5, "hideWorld": 0, },122: { "worldId": 8, "name": "OlympusEastNight", "display": "East Bracket", "areaId": 6, "hideWorld": 0, },123: { "worldId": 9, "name": "SpaceTuroBlock", "display": "Turo Prison Block", "areaId": 1, "hideWorld": 0, },124: { "worldId": 9, "name": "SpaceTuroTransporter", "display": "Turo Transporter", "areaId": 2, "hideWorld": 0, },125: { "worldId": 9, "name": "SpaceDurgonTransporter", "display": "Durgon Transporter", "areaId": 3, "hideWorld": 0, },126: { "worldId": 9, "name": "SpaceCorridor", "display": "Ship Corridor", "areaId": 4, "hideWorld": 0, },127: { "worldId": 9, "name": "SpaceControl", "display": "Control Room", "areaId": 5, "hideWorld": 0, },128: { "worldId": 9, "name": "SpacePod", "display": "Containment Pod", "areaId": 6, "hideWorld": 0, },129: { "worldId": 9, "name": "SpaceHub", "display": "Ship Hub", "areaId": 7, "hideWorld": 0, },130: { "worldId": 9, "name": "SpaceMachineryBay", "display": "Machinery Bay", "areaId": 8, "hideWorld": 0, },131: { "worldId": 9, "name": "SpaceLaunch", "display": "Launch Deck", "areaId": 9, "hideWorld": 0, },132: { "worldId": 9, "name": "SpaceExterior", "display": "Ship Exterior", "areaId": 10, "hideWorld": 0, },133: { "worldId": 9, "name": "SpaceOuter", "display": "Outer Space", "areaId": 11, "hideWorld": 0, },134: { "worldId": 9, "name": "SpaceCorridor2", "display": "Ship Corridor", "areaId": 12, "hideWorld": 0, },135: { "worldId": 9, "name": "SpaceLanesBetween", "display": "The Lanes Between", "areaId": 13, "hideWorld": 0, },136: { "worldId": 9, "name": "SpaceMachineryBayAccess", "display": "Machinery Bay Access", "areaId": 14, "hideWorld": 0, },137: { "worldId": 10, "name": "DestinyBeachDay", "display": "Island Beach", "areaId": 1, "hideWorld": 0, },138: { "worldId": 10, "name": "DestinyBeachSunset", "display": "Island Beach", "areaId": 2, "hideWorld": 0, },139: { "worldId": 10, "name": "DestinyBeachNight", "display": "Island Beach", "areaId": 3, "hideWorld": 0, },140: { "worldId": 10, "name": "DestinyMainIsland", "display": "Main Island Beach", "areaId": 4, "hideWorld": 0, },141: { "worldId": 11, "name": "NeverlandCove", "display": "Cove", "areaId": 1, "hideWorld": 0, },142: { "worldId": 11, "name": "NeverlandCliff", "display": "Cliff Path", "areaId": 2, "hideWorld": 0, },143: { "worldId": 11, "name": "NeverlandLagoon", "display": "Mermaid Lagoon", "areaId": 3, "hideWorld": 0, },144: { "worldId": 11, "name": "NeverlandSeacoast", "display": "Seacoast", "areaId": 4, "hideWorld": 0, },145: { "worldId": 11, "name": "NeverlandClearing", "display": "Jungle Clearing", "areaId": 5, "hideWorld": 0, },146: { "worldId": 11, "name": "NeverlandHideout", "display": "Peter’s Hideout", "areaId": 6, "hideWorld": 0, },147: { "worldId": 11, "name": "NeverlandGully", "display": "Gully", "areaId": 7, "hideWorld": 0, },148: { "worldId": 11, "name": "NeverlandCamp", "display": "Indian Camp", "areaId": 8, "hideWorld": 0, },149: { "worldId": 11, "name": "NeverlandBase", "display": "Rainbow Falls: Base", "areaId": 9, "hideWorld": 0, },150: { "worldId": 11, "name": "NeverlandAscent", "display": "Rainbow Falls: Ascent", "areaId": 10, "hideWorld": 0, },151: { "worldId": 11, "name": "NeverlandCrest", "display": "Rainbow Falls: Crest", "areaId": 11, "hideWorld": 0, },152: { "worldId": 11, "name": "NeverlandSkullEntrance", "display": "Skull Rock: Entrance", "areaId": 12, "hideWorld": 0, },153: { "worldId": 11, "name": "NeverlandSkullCavern", "display": "Skull Rock: Cavern", "areaId": 13, "hideWorld": 0, },154: { "worldId": 11, "name": "NeverlandSky", "display": "Night Sky", "areaId": 14, "hideWorld": 0, },155: { "worldId": 12, "name": "DisneyLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },156: { "worldId": 12, "name": "DisneyPlaza", "display": "Main Plaza", "areaId": 2, "hideWorld": 0, },157: { "worldId": 12, "name": "DisneyFruitballCourt", "display": "Fruitball Course", "areaId": 3, "hideWorld": 0, },158: { "worldId": 12, "name": "DisneyCourseA", "display": "Racecourse A", "areaId": 4, "hideWorld": 0, },159: { "worldId": 12, "name": "DisneyRaceway", "display": "Raceway", "areaId": 5, "hideWorld": 0, },160: { "worldId": 12, "name": "DisneyGizmo", "display": "Gizmo Gallery", "areaId": 6, "hideWorld": 0, },161: { "worldId": 12, "name": "DisneyRecRoom", "display": "Pete’s Rec Room", "areaId": 7, "hideWorld": 0, },162: { "worldId": 12, "name": "DisneyCourseB", "display": "Racecourse B", "areaId": 8, "hideWorld": 0, },163: { "worldId": 12, "name": "DisneyCourseC", "display": "Racecourse C", "areaId": 9, "hideWorld": 0, },164: { "worldId": 12, "name": "DisneyCourseD", "display": "Racecourse D", "areaId": 10, "hideWorld": 0, },165: { "worldId": 12, "name": "DisneyLanesBetween", "display": "The Lanes Between", "areaId": 11, "hideWorld": 0, },166: { "worldId": 12, "name": "DisneyRegistration", "display": "Raceway Registration", "areaId": 12, "hideWorld": 0, },167: { "worldId": 12, "name": "DisneyIceCream", "display": "Ice Cream", "areaId": 13, "hideWorld": 0, },168: { "worldId": 12, "name": "DisneyFruitball", "display": "Fruitball", "areaId": 14, "hideWorld": 0, },169: { "worldId": 12, "name": "DisneyCourseCastle", "display": "Race: Castle Course", "areaId": 15, "hideWorld": 0, },170: { "worldId": 13, "name": "GraveyardBadlands", "display": "Badlands", "areaId": 1, "hideWorld": 0, },171: { "worldId": 13, "name": "GraveyardWar", "display": "Seat of War", "areaId": 2, "hideWorld": 0, },172: { "worldId": 13, "name": "GraveyardTwister", "display": "Twister Trench", "areaId": 3, "hideWorld": 0, },173: { "worldId": 13, "name": "GraveyardEye1", "display": "Eye of the Storm", "areaId": 4, "hideWorld": 0, },174: { "worldId": 13, "name": "GraveyardEye2", "display": "Eye of the Storm", "areaId": 5, "hideWorld": 0, },175: { "worldId": 13, "name": "GraveyardEye3", "display": "Eye of the Storm", "areaId": 6, "hideWorld": 0, },176: { "worldId": 13, "name": "GraveyardFissure", "display": "Fissure", "areaId": 7, "hideWorld": 0, },177: { "worldId": 13, "name": "Graveyard1", "display": "Keyblade Graveyard", "areaId": 8, "hideWorld": 1, },178: { "worldId": 13, "name": "Graveyard2", "display": "Keyblade Graveyard", "areaId": 9, "hideWorld": 1, },179: { "worldId": 13, "name": "Graveyard3", "display": "Keyblade Graveyard", "areaId": 10, "hideWorld": 1, },180: { "worldId": 13, "name": "GraveyardCage", "display": "Will’s Cage", "areaId": 11, "hideWorld": 0, },181: { "worldId": 13, "name": "Graveyard4", "display": "Keyblade Graveyard", "areaId": 12, "hideWorld": 1, },182: { "worldId": 13, "name": "VentusHeart1", "display": "Ventus’s Heart", "areaId": 50, "hideWorld": 0, },183: { "worldId": 13, "name": "VentusHeart2", "display": "Ventus’s Heart", "areaId": 51, "hideWorld": 0, },184: { "worldId": 13, "name": "VentusHeart3", "display": "Ventus’s Heart", "areaId": 52, "hideWorld": 0, },185: { "worldId": 13, "name": "SoraHeart", "display": "Sora’s Heart", "areaId": 53, "hideWorld": 0, },186: { "worldId": 13, "name": "TerraHeart", "display": "Terra’s Heart", "areaId": 54, "hideWorld": 0, },187: { "worldId": 13, "name": "Graveyard5", "display": "Keyblade Graveyard", "areaId": 55, "hideWorld": 0, },188: { "worldId": 13, "name": "GraveyardBadlands2", "display": "Badlands", "areaId": 56, "hideWorld": 0, },189: { "worldId": 15, "name": "MirageHub", "display": "Hub", "areaId": 1, "hideWorld": 0, },190: { "worldId": 15, "name": "MirageColiseum", "display": "Coliseum", "areaId": 2, "hideWorld": 0, },191: { "worldId": 15, "name": "MirageArena1", "display": "Arena", "areaId": 3, "hideWorld": 0, },192: { "worldId": 15, "name": "MirageBadlands", "display": "Badlands", "areaId": 4, "hideWorld": 0, },193: { "worldId": 15, "name": "MiragePinball", "display": "Pinball", "areaId": 5, "hideWorld": 0, },194: { "worldId": 15, "name": "MirageShipHub", "display": "Ship Hub", "areaId": 6, "hideWorld": 0, },195: { "worldId": 15, "name": "MirageMousehole", "display": "Mousehole", "areaId": 7, "hideWorld": 0, },196: { "worldId": 15, "name": "MirageForest", "display": "Forest", "areaId": 8, "hideWorld": 0, },197: { "worldId": 15, "name": "MirageSkull", "display": "Skull Rock", "areaId": 9, "hideWorld": 0, },198: { "worldId": 15, "name": "MirageChamber", "display": "Audience Chamber", "areaId": 10, "hideWorld": 0, },199: { "worldId": 15, "name": "MirageForecourt", "display": "Forecourt", "areaId": 11, "hideWorld": 0, },200: { "worldId": 15, "name": "MirageSummit", "display": "Summit", "areaId": 12, "hideWorld": 0, },201: { "worldId": 15, "name": "MirageDeck", "display": "Launch Deck", "areaId": 13, "hideWorld": 0, },202: { "worldId": 15, "name": "MirageExterior", "display": "Ship Exterior", "areaId": 14, "hideWorld": 0, },203: { "worldId": 15, "name": "MirageArena2", "display": "Arena", "areaId": 15, "hideWorld": 0, },204: { "worldId": 16, "name": "CommandDeparture", "display": "The Land of Departure Command Board", "areaId": 1, "hideWorld": 1, },205: { "worldId": 16, "name": "CommandCinderella", "display": "Cinderella Command Board", "areaId": 3, "hideWorld": 1, },206: { "worldId": 16, "name": "CommandSitch", "display": "Lilo and Stitch Command Board", "areaId": 9, "hideWorld": 1, },207: { "worldId": 16, "name": "CommandPan", "display": "Peter Pan Command Board", "areaId": 11, "hideWorld": 1, },208: { "worldId": 16, "name": "CommandDisney", "display": "Disney Castle Command Board", "areaId": 12, "hideWorld": 1, },209: { "worldId": 16, "name": "CommandPooh", "display": "Winnie the Pooh Command Board", "areaId": 18, "hideWorld": 1, },210: { "worldId": 16, "name": "CommandPan2", "display": "Peter Pan Command Board", "areaId": 19, "hideWorld": 1, },211: { "worldId": 17, "name": "WorldMap", "display": "World Map", "areaId": 1, "hideWorld": 1, },</v>
+        <v>0: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },1: { "worldId": 1, "name": "DepartureForecourtDay", "display": "Forecourt", "areaId": 1, "hideWorld": 0, },2: { "worldId": 1, "name": "DepartureGreatHall", "display": "Great Hall", "areaId": 2, "hideWorld": 0, },3: { "worldId": 1, "name": "VentusRoomDay", "display": "Ventus’s Room", "areaId": 3, "hideWorld": 0, },4: { "worldId": 1, "name": "VentusRoomNight", "display": "Ventus’s Room", "areaId": 4, "hideWorld": 0, },6: { "worldId": 1, "name": "DepartureMountainPath", "display": "Mountain Path", "areaId": 5, "hideWorld": 0, },7: { "worldId": 1, "name": "DepartureSummitNight", "display": "Summit", "areaId": 6, "hideWorld": 0, },8: { "worldId": 1, "name": "DepartureForecourtNight", "display": "Forecourt", "areaId": 7, "hideWorld": 0, },9: { "worldId": 1, "name": "DepartureForecourtRuins", "display": "Forecourt", "areaId": 8, "hideWorld": 0, },10: { "worldId": 1, "name": "DepartureGreatHallRuins", "display": "Great Hall", "areaId": 9, "hideWorld": 0, },11: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 10, "hideWorld": 0, },12: { "worldId": 1, "name": "ChamberOfWaking", "display": "Chamber of Waking", "areaId": 11, "hideWorld": 0, },13: { "worldId": 1, "name": "CastleOblivion", "display": "Castle Oblivion", "areaId": 12, "hideWorld": 0, },14: { "worldId": 1, "name": "CharacterSelect", "display": "Selecting a character…", "areaId": 13, "hideWorld": 1, },15: { "worldId": 1, "name": "DepartureForecourtRuins2", "display": "Forecourt", "areaId": 14, "hideWorld": 0, },16: { "worldId": 1, "name": "DepartureMountainPathRuins", "display": "Mountain Path", "areaId": 15, "hideWorld": 0, },17: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 16, "hideWorld": 0, },18: { "worldId": 2, "name": "DwarfMineEntrance", "display": "Mine Entrance", "areaId": 1, "hideWorld": 0, },19: { "worldId": 2, "name": "DwarfMine", "display": "The Mine", "areaId": 2, "hideWorld": 0, },20: { "worldId": 2, "name": "DwarfVault", "display": "Vault", "areaId": 3, "hideWorld": 0, },21: { "worldId": 2, "name": "DwarfMirrorChamber", "display": "Magic Mirror Chamber", "areaId": 4, "hideWorld": 0, },22: { "worldId": 2, "name": "DwarfWaterway", "display": "Underground Waterway", "areaId": 5, "hideWorld": 0, },23: { "worldId": 2, "name": "DwarfCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },24: { "worldId": 2, "name": "DwarfGlade", "display": "Flower Glade", "areaId": 7, "hideWorld": 0, },25: { "worldId": 2, "name": "DwarfWoods", "display": "Deep Woods", "areaId": 8, "hideWorld": 0, },26: { "worldId": 2, "name": "DwarfMirror", "display": "Inside the Magic Mirror", "areaId": 9, "hideWorld": 0, },27: { "worldId": 2, "name": "DwarfClearing", "display": "Cottage Clearing", "areaId": 10, "hideWorld": 0, },28: { "worldId": 2, "name": "DwarfCottage", "display": "The Cottage", "areaId": 11, "hideWorld": 0, },29: { "worldId": 2, "name": "DwarfMountainTrail", "display": "Mountain Trail", "areaId": 12, "hideWorld": 0, },30: { "worldId": 3, "name": "CastleHouse", "display": "Cinderella’s House", "areaId": 1, "hideWorld": 0, },31: { "worldId": 3, "name": "CastleMousehole", "display": "Mousehole", "areaId": 2, "hideWorld": 0, },32: { "worldId": 3, "name": "CastleWardrobe", "display": "Wardrobe Room", "areaId": 3, "hideWorld": 0, },33: { "worldId": 3, "name": "CastleEntrance", "display": "Entrance", "areaId": 4, "hideWorld": 0, },34: { "worldId": 3, "name": "CastleChateau", "display": "The Chateau", "areaId": 5, "hideWorld": 0, },35: { "worldId": 3, "name": "CastleForest", "display": "Forest", "areaId": 6, "hideWorld": 0, },36: { "worldId": 3, "name": "CastleCourtyard", "display": "Palace Courtyard", "areaId": 7, "hideWorld": 0, },37: { "worldId": 3, "name": "CastleCorridor", "display": "Corridor", "areaId": 8, "hideWorld": 0, },38: { "worldId": 3, "name": "CastleBallroom", "display": "Ballroom", "areaId": 9, "hideWorld": 0, },39: { "worldId": 3, "name": "CastleFoyer", "display": "Foyer", "areaId": 10, "hideWorld": 0, },40: { "worldId": 3, "name": "CastlePassage", "display": "Passage", "areaId": 11, "hideWorld": 0, },41: { "worldId": 3, "name": "CastleAntechamber", "display": "Antechamber", "areaId": 12, "hideWorld": 0, },42: { "worldId": 3, "name": "CastleWardrobe2", "display": "Wardrobe Room", "areaId": 13, "hideWorld": 0, },43: { "worldId": 3, "name": "CastleMousehole2", "display": "Mousehole", "areaId": 14, "hideWorld": 0, },44: { "worldId": 3, "name": "CastleWardrobe3", "display": "Wardrobe Room", "areaId": 15, "hideWorld": 0, },45: { "worldId": 4, "name": "EnchantedDungeonCell", "display": "Dungeon Cell", "areaId": 1, "hideWorld": 0, },46: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 2, "hideWorld": 0, },47: { "worldId": 4, "name": "EnchantedThrone", "display": "Maleficent’s Throne", "areaId": 3, "hideWorld": 0, },48: { "worldId": 4, "name": "EnchantedDungeon", "display": "Dungeon", "areaId": 4, "hideWorld": 0, },49: { "worldId": 4, "name": "EnchantedHall1", "display": "Hall", "areaId": 5, "hideWorld": 0, },50: { "worldId": 4, "name": "EnchantedMountain", "display": "Forbidden Mountain", "areaId": 6, "hideWorld": 0, },51: { "worldId": 4, "name": "EnchantedWaterside", "display": "Waterside", "areaId": 7, "hideWorld": 0, },52: { "worldId": 4, "name": "EnchantedClearing", "display": "Forest Clearing", "areaId": 8, "hideWorld": 0, },53: { "worldId": 4, "name": "EnchantedBridge", "display": "Bridge", "areaId": 9, "hideWorld": 0, },54: { "worldId": 4, "name": "EnchantedBridgeThorns", "display": "Bridge", "areaId": 10, "hideWorld": 0, },55: { "worldId": 4, "name": "EnchantedAudience1", "display": "Audience Chamber", "areaId": 11, "hideWorld": 0, },56: { "worldId": 4, "name": "EnchantedAudience2", "display": "Audience Chamber", "areaId": 12, "hideWorld": 0, },57: { "worldId": 4, "name": "EnchantedReserved", "display": "Somewhere in the World…", "areaId": 13, "hideWorld": 1, },58: { "worldId": 4, "name": "EnchantedHallway", "display": "Hallway", "areaId": 14, "hideWorld": 0, },59: { "worldId": 4, "name": "EnchantedAurora", "display": "Aurora’s Chamber", "areaId": 15, "hideWorld": 0, },60: { "worldId": 4, "name": "EnchantedTower", "display": "Tower Room", "areaId": 16, "hideWorld": 0, },61: { "worldId": 4, "name": "EnchantedHall2", "display": "Hall", "areaId": 17, "hideWorld": 0, },62: { "worldId": 4, "name": "EnchantedAurora2", "display": "Aurora’s Chamber", "areaId": 18, "hideWorld": 0, },63: { "worldId": 4, "name": "EnchantedHall3", "display": "Hall", "areaId": 19, "hideWorld": 0, },64: { "worldId": 4, "name": "EnchantedHall4", "display": "Hall", "areaId": 20, "hideWorld": 0, },65: { "worldId": 4, "name": "EnchantedHall5", "display": "Hall", "areaId": 21, "hideWorld": 0, },66: { "worldId": 4, "name": "EnchantedHall6", "display": "Hall", "areaId": 22, "hideWorld": 0, },67: { "worldId": 4, "name": "EnchantedHall7", "display": "Hall", "areaId": 23, "hideWorld": 0, },68: { "worldId": 4, "name": "EnchantedHall8", "display": "Hall", "areaId": 24, "hideWorld": 0, },69: { "worldId": 4, "name": "EnchantedHall9", "display": "Hall", "areaId": 25, "hideWorld": 0, },70: { "worldId": 4, "name": "EnchantedHall10", "display": "Hall", "areaId": 26, "hideWorld": 0, },71: { "worldId": 4, "name": "EnchantedHall11", "display": "Hall", "areaId": 27, "hideWorld": 0, },72: { "worldId": 4, "name": "EnchantedHall12", "display": "Hall", "areaId": 28, "hideWorld": 0, },73: { "worldId": 4, "name": "EnchantedHall13", "display": "Hall", "areaId": 29, "hideWorld": 0, },74: { "worldId": 4, "name": "EnchantedHall14", "display": "Hall", "areaId": 30, "hideWorld": 0, },75: { "worldId": 4, "name": "EnchantedHall15", "display": "Hall", "areaId": 31, "hideWorld": 0, },76: { "worldId": 4, "name": "EnchantedHall16", "display": "Hall", "areaId": 32, "hideWorld": 0, },77: { "worldId": 4, "name": "EnchantedHall17", "display": "Hall", "areaId": 33, "hideWorld": 0, },78: { "worldId": 4, "name": "EnchantedHall18", "display": "Hall", "areaId": 34, "hideWorld": 0, },79: { "worldId": 4, "name": "EnchantedHall19", "display": "Hall", "areaId": 35, "hideWorld": 0, },80: { "worldId": 4, "name": "EnchantedHall20", "display": "Hall", "areaId": 36, "hideWorld": 0, },81: { "worldId": 4, "name": "EnchantedHall21", "display": "Hall", "areaId": 37, "hideWorld": 0, },82: { "worldId": 4, "name": "EnchantedHall22", "display": "Hall", "areaId": 38, "hideWorld": 0, },83: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 39, "hideWorld": 0, },84: { "worldId": 5, "name": "MysteriousChamber", "display": "Sorcerer’s Chamber", "areaId": 1, "hideWorld": 0, },85: { "worldId": 5, "name": "MysteriousTower", "display": "Mysterious Tower", "areaId": 2, "hideWorld": 0, },86: { "worldId": 5, "name": "MysteriousEntrance", "display": "Tower Entrance", "areaId": 3, "hideWorld": 0, },87: { "worldId": 5, "name": "MysteriousChamber2", "display": "Sorcerer’s Chamber", "areaId": 4, "hideWorld": 0, },88: { "worldId": 6, "name": "RadiantOuterGardens", "display": "Outer Gardens", "areaId": 1, "hideWorld": 0, },89: { "worldId": 6, "name": "RadiantEntryway", "display": "Entryway", "areaId": 2, "hideWorld": 0, },90: { "worldId": 6, "name": "RadiantCentral", "display": "Central Square", "areaId": 3, "hideWorld": 0, },91: { "worldId": 6, "name": "RadiantAqueduct", "display": "Aqueduct", "areaId": 4, "hideWorld": 0, },92: { "worldId": 6, "name": "RadiantTown", "display": "Castle Town", "areaId": 5, "hideWorld": 0, },93: { "worldId": 6, "name": "RadiantReactor", "display": "Reactor", "areaId": 6, "hideWorld": 0, },94: { "worldId": 6, "name": "RadiantFountain", "display": "Fountain Court", "areaId": 7, "hideWorld": 0, },95: { "worldId": 6, "name": "RadiantMerlin", "display": "Merlin’s House", "areaId": 8, "hideWorld": 0, },96: { "worldId": 6, "name": "RadiantGardens", "display": "Gardens", "areaId": 9, "hideWorld": 0, },97: { "worldId": 6, "name": "RadiantDoors", "display": "Front Doors", "areaId": 10, "hideWorld": 0, },98: { "worldId": 6, "name": "RadiantPurification", "display": "Purification Facility", "areaId": 11, "hideWorld": 0, },99: { "worldId": 6, "name": "RadiantOuterGardens2", "display": "Outer Gardens", "areaId": 12, "hideWorld": 0, },100: { "worldId": 6, "name": "RadiantCentralDark", "display": "Central Square", "areaId": 13, "hideWorld": 0, },101: { "worldId": 6, "name": "RadiantCentralTerranort", "display": "Central Square", "areaId": 14, "hideWorld": 0, },102: { "worldId": 7, "name": "LouieCourt", "display": "Louie’s Ruins (Court)", "areaId": 1, "hideWorld": 0, },103: { "worldId": 7, "name": "LouiePath", "display": "Louie’s Ruins (Path)", "areaId": 2, "hideWorld": 0, },104: { "worldId": 7, "name": "Crossroad", "display": "Crossroad", "areaId": 3, "hideWorld": 0, },105: { "worldId": 7, "name": "UGRuinsEntrance", "display": "Underground Ruins (Entrance)", "areaId": 4, "hideWorld": 0, },106: { "worldId": 7, "name": "UGRuinsPassage1", "display": "Underground Ruins (Passage)", "areaId": 5, "hideWorld": 0, },107: { "worldId": 7, "name": "UGRuinsPassage2", "display": "Underground Ruins (Passage)", "areaId": 6, "hideWorld": 0, },108: { "worldId": 7, "name": "UGCourtyard", "display": "Underground Courtyard", "areaId": 7, "hideWorld": 0, },109: { "worldId": 7, "name": "JungleNearRuins", "display": "Jungle Near Ruins", "areaId": 8, "hideWorld": 0, },110: { "worldId": 7, "name": "Eminence", "display": "Eminence", "areaId": 9, "hideWorld": 0, },111: { "worldId": 7, "name": "Jungle", "display": "Jungle", "areaId": 10, "hideWorld": 0, },112: { "worldId": 7, "name": "River", "display": "Man-Village River", "areaId": 11, "hideWorld": 0, },113: { "worldId": 7, "name": "Bog", "display": "Bog", "areaId": 12, "hideWorld": 0, },114: { "worldId": 7, "name": "LanesBetween", "display": "The Lanes Between", "areaId": 50, "hideWorld": 0, },115: { "worldId": 7, "name": "Blank", "display": "Blank", "areaId": 51, "hideWorld": 0, },116: { "worldId": 7, "name": "Realm of Darkness", "display": "The Realm of Darkness", "areaId": 52, "hideWorld": 1, },117: { "worldId": 8, "name": "OlympusGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },118: { "worldId": 8, "name": "OlympusVestibule", "display": "Vestibule", "areaId": 2, "hideWorld": 0, },119: { "worldId": 8, "name": "OlympusWest", "display": "West Bracket", "areaId": 3, "hideWorld": 0, },120: { "worldId": 8, "name": "OlympusEast", "display": "East Bracket", "areaId": 4, "hideWorld": 0, },121: { "worldId": 8, "name": "OlympusTown", "display": "Town Near Thebes", "areaId": 5, "hideWorld": 0, },122: { "worldId": 8, "name": "OlympusEastNight", "display": "East Bracket", "areaId": 6, "hideWorld": 0, },123: { "worldId": 9, "name": "SpaceTuroBlock", "display": "Turo Prison Block", "areaId": 1, "hideWorld": 0, },124: { "worldId": 9, "name": "SpaceTuroTransporter", "display": "Turo Transporter", "areaId": 2, "hideWorld": 0, },125: { "worldId": 9, "name": "SpaceDurgonTransporter", "display": "Durgon Transporter", "areaId": 3, "hideWorld": 0, },126: { "worldId": 9, "name": "SpaceCorridor", "display": "Ship Corridor", "areaId": 4, "hideWorld": 0, },127: { "worldId": 9, "name": "SpaceControl", "display": "Control Room", "areaId": 5, "hideWorld": 0, },128: { "worldId": 9, "name": "SpacePod", "display": "Containment Pod", "areaId": 6, "hideWorld": 0, },129: { "worldId": 9, "name": "SpaceHub", "display": "Ship Hub", "areaId": 7, "hideWorld": 0, },130: { "worldId": 9, "name": "SpaceMachineryBay", "display": "Machinery Bay", "areaId": 8, "hideWorld": 0, },131: { "worldId": 9, "name": "SpaceLaunch", "display": "Launch Deck", "areaId": 9, "hideWorld": 0, },132: { "worldId": 9, "name": "SpaceExterior", "display": "Ship Exterior", "areaId": 10, "hideWorld": 0, },133: { "worldId": 9, "name": "SpaceOuter", "display": "Outer Space", "areaId": 11, "hideWorld": 0, },134: { "worldId": 9, "name": "SpaceCorridor2", "display": "Ship Corridor", "areaId": 12, "hideWorld": 0, },135: { "worldId": 9, "name": "SpaceLanesBetween", "display": "The Lanes Between", "areaId": 13, "hideWorld": 0, },136: { "worldId": 9, "name": "SpaceMachineryBayAccess", "display": "Machinery Bay Access", "areaId": 14, "hideWorld": 0, },137: { "worldId": 10, "name": "DestinyBeachDay", "display": "Island Beach", "areaId": 1, "hideWorld": 0, },138: { "worldId": 10, "name": "DestinyBeachSunset", "display": "Island Beach", "areaId": 2, "hideWorld": 0, },139: { "worldId": 10, "name": "DestinyBeachNight", "display": "Island Beach", "areaId": 3, "hideWorld": 0, },140: { "worldId": 10, "name": "DestinyMainIsland", "display": "Main Island Beach", "areaId": 4, "hideWorld": 0, },141: { "worldId": 11, "name": "NeverlandCove", "display": "Cove", "areaId": 1, "hideWorld": 0, },142: { "worldId": 11, "name": "NeverlandCliff", "display": "Cliff Path", "areaId": 2, "hideWorld": 0, },143: { "worldId": 11, "name": "NeverlandLagoon", "display": "Mermaid Lagoon", "areaId": 3, "hideWorld": 0, },144: { "worldId": 11, "name": "NeverlandSeacoast", "display": "Seacoast", "areaId": 4, "hideWorld": 0, },145: { "worldId": 11, "name": "NeverlandClearing", "display": "Jungle Clearing", "areaId": 5, "hideWorld": 0, },146: { "worldId": 11, "name": "NeverlandHideout", "display": "Peter’s Hideout", "areaId": 6, "hideWorld": 0, },147: { "worldId": 11, "name": "NeverlandGully", "display": "Gully", "areaId": 7, "hideWorld": 0, },148: { "worldId": 11, "name": "NeverlandCamp", "display": "Indian Camp", "areaId": 8, "hideWorld": 0, },149: { "worldId": 11, "name": "NeverlandBase", "display": "Rainbow Falls: Base", "areaId": 9, "hideWorld": 0, },150: { "worldId": 11, "name": "NeverlandAscent", "display": "Rainbow Falls: Ascent", "areaId": 10, "hideWorld": 0, },151: { "worldId": 11, "name": "NeverlandCrest", "display": "Rainbow Falls: Crest", "areaId": 11, "hideWorld": 0, },152: { "worldId": 11, "name": "NeverlandSkullEntrance", "display": "Skull Rock: Entrance", "areaId": 12, "hideWorld": 0, },153: { "worldId": 11, "name": "NeverlandSkullCavern", "display": "Skull Rock: Cavern", "areaId": 13, "hideWorld": 0, },154: { "worldId": 11, "name": "NeverlandSky", "display": "Night Sky", "areaId": 14, "hideWorld": 0, },155: { "worldId": 12, "name": "DisneyLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },156: { "worldId": 12, "name": "DisneyPlaza", "display": "Main Plaza", "areaId": 2, "hideWorld": 0, },157: { "worldId": 12, "name": "DisneyFruitballCourt", "display": "Fruitball Course", "areaId": 3, "hideWorld": 0, },158: { "worldId": 12, "name": "DisneyCountryChase", "display": "Country Chase", "areaId": 4, "hideWorld": 0, },159: { "worldId": 12, "name": "DisneyRaceway", "display": "Raceway", "areaId": 5, "hideWorld": 0, },160: { "worldId": 12, "name": "DisneyGizmo", "display": "Gizmo Gallery", "areaId": 6, "hideWorld": 0, },161: { "worldId": 12, "name": "DisneyRecRoom", "display": "Pete’s Rec Room", "areaId": 7, "hideWorld": 0, },162: { "worldId": 12, "name": "DisneyCourseB", "display": "Racecourse B", "areaId": 8, "hideWorld": 0, },163: { "worldId": 12, "name": "DisneyCourseC", "display": "Racecourse C", "areaId": 9, "hideWorld": 0, },164: { "worldId": 12, "name": "DisneyCourseD", "display": "Racecourse D", "areaId": 10, "hideWorld": 0, },165: { "worldId": 12, "name": "DisneyLanesBetween", "display": "The Lanes Between", "areaId": 11, "hideWorld": 0, },166: { "worldId": 12, "name": "DisneyRegistration", "display": "Raceway Registration", "areaId": 12, "hideWorld": 0, },167: { "worldId": 12, "name": "DisneyIceCream", "display": "Ice Cream", "areaId": 13, "hideWorld": 0, },168: { "worldId": 12, "name": "DisneyFruitball", "display": "Fruitball", "areaId": 14, "hideWorld": 0, },169: { "worldId": 12, "name": "DisneyCourseCastle", "display": "Race: Castle Course", "areaId": 15, "hideWorld": 0, },170: { "worldId": 13, "name": "GraveyardBadlands", "display": "Badlands", "areaId": 1, "hideWorld": 0, },171: { "worldId": 13, "name": "GraveyardWar", "display": "Seat of War", "areaId": 2, "hideWorld": 0, },172: { "worldId": 13, "name": "GraveyardTwister", "display": "Twister Trench", "areaId": 3, "hideWorld": 0, },173: { "worldId": 13, "name": "GraveyardEye1", "display": "Eye of the Storm", "areaId": 4, "hideWorld": 0, },174: { "worldId": 13, "name": "GraveyardEye2", "display": "Eye of the Storm", "areaId": 5, "hideWorld": 0, },175: { "worldId": 13, "name": "GraveyardEye3", "display": "Eye of the Storm", "areaId": 6, "hideWorld": 0, },176: { "worldId": 13, "name": "GraveyardFissure", "display": "Fissure", "areaId": 7, "hideWorld": 0, },177: { "worldId": 13, "name": "Graveyard1", "display": "Keyblade Graveyard", "areaId": 8, "hideWorld": 1, },178: { "worldId": 13, "name": "Graveyard2", "display": "Keyblade Graveyard", "areaId": 9, "hideWorld": 1, },179: { "worldId": 13, "name": "Graveyard3", "display": "Keyblade Graveyard", "areaId": 10, "hideWorld": 1, },180: { "worldId": 13, "name": "GraveyardCage", "display": "Will’s Cage", "areaId": 11, "hideWorld": 0, },181: { "worldId": 13, "name": "Graveyard4", "display": "Keyblade Graveyard", "areaId": 12, "hideWorld": 1, },182: { "worldId": 13, "name": "VentusHeart1", "display": "Ventus’s Heart", "areaId": 50, "hideWorld": 0, },183: { "worldId": 13, "name": "VentusHeart2", "display": "Ventus’s Heart", "areaId": 51, "hideWorld": 0, },184: { "worldId": 13, "name": "VentusHeart3", "display": "Ventus’s Heart", "areaId": 52, "hideWorld": 0, },185: { "worldId": 13, "name": "SoraHeart", "display": "Sora’s Heart", "areaId": 53, "hideWorld": 0, },186: { "worldId": 13, "name": "TerraHeart", "display": "Terra’s Heart", "areaId": 54, "hideWorld": 0, },187: { "worldId": 13, "name": "Graveyard5", "display": "Keyblade Graveyard", "areaId": 55, "hideWorld": 0, },188: { "worldId": 13, "name": "GraveyardBadlands2", "display": "Badlands", "areaId": 56, "hideWorld": 0, },189: { "worldId": 15, "name": "MirageHub", "display": "Hub", "areaId": 1, "hideWorld": 0, },190: { "worldId": 15, "name": "MirageColiseum", "display": "Coliseum", "areaId": 2, "hideWorld": 0, },191: { "worldId": 15, "name": "MirageArena1", "display": "Arena", "areaId": 3, "hideWorld": 0, },192: { "worldId": 15, "name": "MirageBadlands", "display": "Badlands", "areaId": 4, "hideWorld": 0, },193: { "worldId": 15, "name": "MiragePinball", "display": "Pinball", "areaId": 5, "hideWorld": 0, },194: { "worldId": 15, "name": "MirageShipHub", "display": "Ship Hub", "areaId": 6, "hideWorld": 0, },195: { "worldId": 15, "name": "MirageMousehole", "display": "Mousehole", "areaId": 7, "hideWorld": 0, },196: { "worldId": 15, "name": "MirageForest", "display": "Forest", "areaId": 8, "hideWorld": 0, },197: { "worldId": 15, "name": "MirageSkull", "display": "Skull Rock", "areaId": 9, "hideWorld": 0, },198: { "worldId": 15, "name": "MirageChamber", "display": "Audience Chamber", "areaId": 10, "hideWorld": 0, },199: { "worldId": 15, "name": "MirageForecourt", "display": "Forecourt", "areaId": 11, "hideWorld": 0, },200: { "worldId": 15, "name": "MirageSummit", "display": "Summit", "areaId": 12, "hideWorld": 0, },201: { "worldId": 15, "name": "MirageDeck", "display": "Launch Deck", "areaId": 13, "hideWorld": 0, },202: { "worldId": 15, "name": "MirageExterior", "display": "Ship Exterior", "areaId": 14, "hideWorld": 0, },203: { "worldId": 15, "name": "MirageArena2", "display": "Arena", "areaId": 15, "hideWorld": 0, },204: { "worldId": 16, "name": "CommandDeparture", "display": "The Land of Departure Command Board", "areaId": 1, "hideWorld": 1, },205: { "worldId": 16, "name": "CommandCinderella", "display": "Cinderella Command Board", "areaId": 3, "hideWorld": 1, },206: { "worldId": 16, "name": "CommandSitch", "display": "Lilo and Stitch Command Board", "areaId": 9, "hideWorld": 1, },207: { "worldId": 16, "name": "CommandPan", "display": "Peter Pan Command Board", "areaId": 11, "hideWorld": 1, },208: { "worldId": 16, "name": "CommandDisney", "display": "Disney Castle Command Board", "areaId": 12, "hideWorld": 1, },209: { "worldId": 16, "name": "CommandPooh", "display": "Winnie the Pooh Command Board", "areaId": 18, "hideWorld": 1, },210: { "worldId": 16, "name": "CommandPan2", "display": "Peter Pan Command Board", "areaId": 19, "hideWorld": 1, },211: { "worldId": 17, "name": "WorldMap", "display": "World Map", "areaId": 1, "hideWorld": 1, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6750,7 +6750,7 @@
       </c>
       <c r="G159" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A159,": { ""worldId"": ",C159,", ""name"": """,D159,""", ""display"": """,E159,""", ""areaId"": ",B159,", ""hideWorld"": ",F159,", },")</f>
-        <v>158: { "worldId": 12, "name": "DisneyCourseA", "display": "Racecourse A", "areaId": 4, "hideWorld": 0, },</v>
+        <v>158: { "worldId": 12, "name": "DisneyCountryChase", "display": "Country Chase", "areaId": 4, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8043,11 +8043,11 @@
   </sheetPr>
   <dimension ref="A1:J213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A191" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2:H213"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A191" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H2" activeCellId="0" sqref="H2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -13404,7 +13404,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C95"/>
+  <autoFilter ref="C1:C95"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Finalized Rumble Racing challenge achievements and leaderboards
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$95</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$95</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$95</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -916,16 +916,16 @@
     <t xml:space="preserve">Disney Drive</t>
   </si>
   <si>
-    <t xml:space="preserve">DisneyCourseC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Racecourse C</t>
-  </si>
-  <si>
-    <t xml:space="preserve">DisneyCourseD</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Racecourse D</t>
+    <t xml:space="preserve">DisneySpree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Grand Spree</t>
+  </si>
+  <si>
+    <t xml:space="preserve">DisneyCastle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Castle Circuit</t>
   </si>
   <si>
     <t xml:space="preserve">DisneyLanesBetween</t>
@@ -2631,7 +2631,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.66796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.6875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -2923,11 +2923,11 @@
   </sheetPr>
   <dimension ref="A1:I212"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A184" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E164" activeCellId="0" sqref="E164"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A151" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="E166" activeCellId="0" sqref="E166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.2734375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.2890625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -2961,7 +2961,7 @@
       </c>
       <c r="I1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1000)</f>
-        <v>0: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },1: { "worldId": 1, "name": "DepartureForecourtDay", "display": "Forecourt", "areaId": 1, "hideWorld": 0, },2: { "worldId": 1, "name": "DepartureGreatHall", "display": "Great Hall", "areaId": 2, "hideWorld": 0, },3: { "worldId": 1, "name": "VentusRoomDay", "display": "Ventus’s Room", "areaId": 3, "hideWorld": 0, },4: { "worldId": 1, "name": "VentusRoomNight", "display": "Ventus’s Room", "areaId": 4, "hideWorld": 0, },6: { "worldId": 1, "name": "DepartureMountainPath", "display": "Mountain Path", "areaId": 5, "hideWorld": 0, },7: { "worldId": 1, "name": "DepartureSummitNight", "display": "Summit", "areaId": 6, "hideWorld": 0, },8: { "worldId": 1, "name": "DepartureForecourtNight", "display": "Forecourt", "areaId": 7, "hideWorld": 0, },9: { "worldId": 1, "name": "DepartureForecourtRuins", "display": "Forecourt", "areaId": 8, "hideWorld": 0, },10: { "worldId": 1, "name": "DepartureGreatHallRuins", "display": "Great Hall", "areaId": 9, "hideWorld": 0, },11: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 10, "hideWorld": 0, },12: { "worldId": 1, "name": "ChamberOfWaking", "display": "Chamber of Waking", "areaId": 11, "hideWorld": 0, },13: { "worldId": 1, "name": "CastleOblivion", "display": "Castle Oblivion", "areaId": 12, "hideWorld": 0, },14: { "worldId": 1, "name": "CharacterSelect", "display": "Selecting a character…", "areaId": 13, "hideWorld": 1, },15: { "worldId": 1, "name": "DepartureForecourtRuins2", "display": "Forecourt", "areaId": 14, "hideWorld": 0, },16: { "worldId": 1, "name": "DepartureMountainPathRuins", "display": "Mountain Path", "areaId": 15, "hideWorld": 0, },17: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 16, "hideWorld": 0, },18: { "worldId": 2, "name": "DwarfMineEntrance", "display": "Mine Entrance", "areaId": 1, "hideWorld": 0, },19: { "worldId": 2, "name": "DwarfMine", "display": "The Mine", "areaId": 2, "hideWorld": 0, },20: { "worldId": 2, "name": "DwarfVault", "display": "Vault", "areaId": 3, "hideWorld": 0, },21: { "worldId": 2, "name": "DwarfMirrorChamber", "display": "Magic Mirror Chamber", "areaId": 4, "hideWorld": 0, },22: { "worldId": 2, "name": "DwarfWaterway", "display": "Underground Waterway", "areaId": 5, "hideWorld": 0, },23: { "worldId": 2, "name": "DwarfCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },24: { "worldId": 2, "name": "DwarfGlade", "display": "Flower Glade", "areaId": 7, "hideWorld": 0, },25: { "worldId": 2, "name": "DwarfWoods", "display": "Deep Woods", "areaId": 8, "hideWorld": 0, },26: { "worldId": 2, "name": "DwarfMirror", "display": "Inside the Magic Mirror", "areaId": 9, "hideWorld": 0, },27: { "worldId": 2, "name": "DwarfClearing", "display": "Cottage Clearing", "areaId": 10, "hideWorld": 0, },28: { "worldId": 2, "name": "DwarfCottage", "display": "The Cottage", "areaId": 11, "hideWorld": 0, },29: { "worldId": 2, "name": "DwarfMountainTrail", "display": "Mountain Trail", "areaId": 12, "hideWorld": 0, },30: { "worldId": 3, "name": "CastleHouse", "display": "Cinderella’s House", "areaId": 1, "hideWorld": 0, },31: { "worldId": 3, "name": "CastleMousehole", "display": "Mousehole", "areaId": 2, "hideWorld": 0, },32: { "worldId": 3, "name": "CastleWardrobe", "display": "Wardrobe Room", "areaId": 3, "hideWorld": 0, },33: { "worldId": 3, "name": "CastleEntrance", "display": "Entrance", "areaId": 4, "hideWorld": 0, },34: { "worldId": 3, "name": "CastleChateau", "display": "The Chateau", "areaId": 5, "hideWorld": 0, },35: { "worldId": 3, "name": "CastleForest", "display": "Forest", "areaId": 6, "hideWorld": 0, },36: { "worldId": 3, "name": "CastleCourtyard", "display": "Palace Courtyard", "areaId": 7, "hideWorld": 0, },37: { "worldId": 3, "name": "CastleCorridor", "display": "Corridor", "areaId": 8, "hideWorld": 0, },38: { "worldId": 3, "name": "CastleBallroom", "display": "Ballroom", "areaId": 9, "hideWorld": 0, },39: { "worldId": 3, "name": "CastleFoyer", "display": "Foyer", "areaId": 10, "hideWorld": 0, },40: { "worldId": 3, "name": "CastlePassage", "display": "Passage", "areaId": 11, "hideWorld": 0, },41: { "worldId": 3, "name": "CastleAntechamber", "display": "Antechamber", "areaId": 12, "hideWorld": 0, },42: { "worldId": 3, "name": "CastleWardrobe2", "display": "Wardrobe Room", "areaId": 13, "hideWorld": 0, },43: { "worldId": 3, "name": "CastleMousehole2", "display": "Mousehole", "areaId": 14, "hideWorld": 0, },44: { "worldId": 3, "name": "CastleWardrobe3", "display": "Wardrobe Room", "areaId": 15, "hideWorld": 0, },45: { "worldId": 4, "name": "EnchantedDungeonCell", "display": "Dungeon Cell", "areaId": 1, "hideWorld": 0, },46: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 2, "hideWorld": 0, },47: { "worldId": 4, "name": "EnchantedThrone", "display": "Maleficent’s Throne", "areaId": 3, "hideWorld": 0, },48: { "worldId": 4, "name": "EnchantedDungeon", "display": "Dungeon", "areaId": 4, "hideWorld": 0, },49: { "worldId": 4, "name": "EnchantedHall1", "display": "Hall", "areaId": 5, "hideWorld": 0, },50: { "worldId": 4, "name": "EnchantedMountain", "display": "Forbidden Mountain", "areaId": 6, "hideWorld": 0, },51: { "worldId": 4, "name": "EnchantedWaterside", "display": "Waterside", "areaId": 7, "hideWorld": 0, },52: { "worldId": 4, "name": "EnchantedClearing", "display": "Forest Clearing", "areaId": 8, "hideWorld": 0, },53: { "worldId": 4, "name": "EnchantedBridge", "display": "Bridge", "areaId": 9, "hideWorld": 0, },54: { "worldId": 4, "name": "EnchantedBridgeThorns", "display": "Bridge", "areaId": 10, "hideWorld": 0, },55: { "worldId": 4, "name": "EnchantedAudience1", "display": "Audience Chamber", "areaId": 11, "hideWorld": 0, },56: { "worldId": 4, "name": "EnchantedAudience2", "display": "Audience Chamber", "areaId": 12, "hideWorld": 0, },57: { "worldId": 4, "name": "EnchantedReserved", "display": "Somewhere in the World…", "areaId": 13, "hideWorld": 1, },58: { "worldId": 4, "name": "EnchantedHallway", "display": "Hallway", "areaId": 14, "hideWorld": 0, },59: { "worldId": 4, "name": "EnchantedAurora", "display": "Aurora’s Chamber", "areaId": 15, "hideWorld": 0, },60: { "worldId": 4, "name": "EnchantedTower", "display": "Tower Room", "areaId": 16, "hideWorld": 0, },61: { "worldId": 4, "name": "EnchantedHall2", "display": "Hall", "areaId": 17, "hideWorld": 0, },62: { "worldId": 4, "name": "EnchantedAurora2", "display": "Aurora’s Chamber", "areaId": 18, "hideWorld": 0, },63: { "worldId": 4, "name": "EnchantedHall3", "display": "Hall", "areaId": 19, "hideWorld": 0, },64: { "worldId": 4, "name": "EnchantedHall4", "display": "Hall", "areaId": 20, "hideWorld": 0, },65: { "worldId": 4, "name": "EnchantedHall5", "display": "Hall", "areaId": 21, "hideWorld": 0, },66: { "worldId": 4, "name": "EnchantedHall6", "display": "Hall", "areaId": 22, "hideWorld": 0, },67: { "worldId": 4, "name": "EnchantedHall7", "display": "Hall", "areaId": 23, "hideWorld": 0, },68: { "worldId": 4, "name": "EnchantedHall8", "display": "Hall", "areaId": 24, "hideWorld": 0, },69: { "worldId": 4, "name": "EnchantedHall9", "display": "Hall", "areaId": 25, "hideWorld": 0, },70: { "worldId": 4, "name": "EnchantedHall10", "display": "Hall", "areaId": 26, "hideWorld": 0, },71: { "worldId": 4, "name": "EnchantedHall11", "display": "Hall", "areaId": 27, "hideWorld": 0, },72: { "worldId": 4, "name": "EnchantedHall12", "display": "Hall", "areaId": 28, "hideWorld": 0, },73: { "worldId": 4, "name": "EnchantedHall13", "display": "Hall", "areaId": 29, "hideWorld": 0, },74: { "worldId": 4, "name": "EnchantedHall14", "display": "Hall", "areaId": 30, "hideWorld": 0, },75: { "worldId": 4, "name": "EnchantedHall15", "display": "Hall", "areaId": 31, "hideWorld": 0, },76: { "worldId": 4, "name": "EnchantedHall16", "display": "Hall", "areaId": 32, "hideWorld": 0, },77: { "worldId": 4, "name": "EnchantedHall17", "display": "Hall", "areaId": 33, "hideWorld": 0, },78: { "worldId": 4, "name": "EnchantedHall18", "display": "Hall", "areaId": 34, "hideWorld": 0, },79: { "worldId": 4, "name": "EnchantedHall19", "display": "Hall", "areaId": 35, "hideWorld": 0, },80: { "worldId": 4, "name": "EnchantedHall20", "display": "Hall", "areaId": 36, "hideWorld": 0, },81: { "worldId": 4, "name": "EnchantedHall21", "display": "Hall", "areaId": 37, "hideWorld": 0, },82: { "worldId": 4, "name": "EnchantedHall22", "display": "Hall", "areaId": 38, "hideWorld": 0, },83: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 39, "hideWorld": 0, },84: { "worldId": 5, "name": "MysteriousChamber", "display": "Sorcerer’s Chamber", "areaId": 1, "hideWorld": 0, },85: { "worldId": 5, "name": "MysteriousTower", "display": "Mysterious Tower", "areaId": 2, "hideWorld": 0, },86: { "worldId": 5, "name": "MysteriousEntrance", "display": "Tower Entrance", "areaId": 3, "hideWorld": 0, },87: { "worldId": 5, "name": "MysteriousChamber2", "display": "Sorcerer’s Chamber", "areaId": 4, "hideWorld": 0, },88: { "worldId": 6, "name": "RadiantOuterGardens", "display": "Outer Gardens", "areaId": 1, "hideWorld": 0, },89: { "worldId": 6, "name": "RadiantEntryway", "display": "Entryway", "areaId": 2, "hideWorld": 0, },90: { "worldId": 6, "name": "RadiantCentral", "display": "Central Square", "areaId": 3, "hideWorld": 0, },91: { "worldId": 6, "name": "RadiantAqueduct", "display": "Aqueduct", "areaId": 4, "hideWorld": 0, },92: { "worldId": 6, "name": "RadiantTown", "display": "Castle Town", "areaId": 5, "hideWorld": 0, },93: { "worldId": 6, "name": "RadiantReactor", "display": "Reactor", "areaId": 6, "hideWorld": 0, },94: { "worldId": 6, "name": "RadiantFountain", "display": "Fountain Court", "areaId": 7, "hideWorld": 0, },95: { "worldId": 6, "name": "RadiantMerlin", "display": "Merlin’s House", "areaId": 8, "hideWorld": 0, },96: { "worldId": 6, "name": "RadiantGardens", "display": "Gardens", "areaId": 9, "hideWorld": 0, },97: { "worldId": 6, "name": "RadiantDoors", "display": "Front Doors", "areaId": 10, "hideWorld": 0, },98: { "worldId": 6, "name": "RadiantPurification", "display": "Purification Facility", "areaId": 11, "hideWorld": 0, },99: { "worldId": 6, "name": "RadiantOuterGardens2", "display": "Outer Gardens", "areaId": 12, "hideWorld": 0, },100: { "worldId": 6, "name": "RadiantCentralDark", "display": "Central Square", "areaId": 13, "hideWorld": 0, },101: { "worldId": 6, "name": "RadiantCentralTerranort", "display": "Central Square", "areaId": 14, "hideWorld": 0, },102: { "worldId": 7, "name": "LouieCourt", "display": "Louie’s Ruins (Court)", "areaId": 1, "hideWorld": 0, },103: { "worldId": 7, "name": "LouiePath", "display": "Louie’s Ruins (Path)", "areaId": 2, "hideWorld": 0, },104: { "worldId": 7, "name": "Crossroad", "display": "Crossroad", "areaId": 3, "hideWorld": 0, },105: { "worldId": 7, "name": "UGRuinsEntrance", "display": "Underground Ruins (Entrance)", "areaId": 4, "hideWorld": 0, },106: { "worldId": 7, "name": "UGRuinsPassage1", "display": "Underground Ruins (Passage)", "areaId": 5, "hideWorld": 0, },107: { "worldId": 7, "name": "UGRuinsPassage2", "display": "Underground Ruins (Passage)", "areaId": 6, "hideWorld": 0, },108: { "worldId": 7, "name": "UGCourtyard", "display": "Underground Courtyard", "areaId": 7, "hideWorld": 0, },109: { "worldId": 7, "name": "JungleNearRuins", "display": "Jungle Near Ruins", "areaId": 8, "hideWorld": 0, },110: { "worldId": 7, "name": "Eminence", "display": "Eminence", "areaId": 9, "hideWorld": 0, },111: { "worldId": 7, "name": "Jungle", "display": "Jungle", "areaId": 10, "hideWorld": 0, },112: { "worldId": 7, "name": "River", "display": "Man-Village River", "areaId": 11, "hideWorld": 0, },113: { "worldId": 7, "name": "Bog", "display": "Bog", "areaId": 12, "hideWorld": 0, },114: { "worldId": 7, "name": "LanesBetween", "display": "The Lanes Between", "areaId": 50, "hideWorld": 0, },115: { "worldId": 7, "name": "Blank", "display": "Blank", "areaId": 51, "hideWorld": 0, },116: { "worldId": 7, "name": "Realm of Darkness", "display": "The Realm of Darkness", "areaId": 52, "hideWorld": 1, },117: { "worldId": 8, "name": "OlympusGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },118: { "worldId": 8, "name": "OlympusVestibule", "display": "Vestibule", "areaId": 2, "hideWorld": 0, },119: { "worldId": 8, "name": "OlympusWest", "display": "West Bracket", "areaId": 3, "hideWorld": 0, },120: { "worldId": 8, "name": "OlympusEast", "display": "East Bracket", "areaId": 4, "hideWorld": 0, },121: { "worldId": 8, "name": "OlympusTown", "display": "Town Near Thebes", "areaId": 5, "hideWorld": 0, },122: { "worldId": 8, "name": "OlympusEastNight", "display": "East Bracket", "areaId": 6, "hideWorld": 0, },123: { "worldId": 9, "name": "SpaceTuroBlock", "display": "Turo Prison Block", "areaId": 1, "hideWorld": 0, },124: { "worldId": 9, "name": "SpaceTuroTransporter", "display": "Turo Transporter", "areaId": 2, "hideWorld": 0, },125: { "worldId": 9, "name": "SpaceDurgonTransporter", "display": "Durgon Transporter", "areaId": 3, "hideWorld": 0, },126: { "worldId": 9, "name": "SpaceCorridor", "display": "Ship Corridor", "areaId": 4, "hideWorld": 0, },127: { "worldId": 9, "name": "SpaceControl", "display": "Control Room", "areaId": 5, "hideWorld": 0, },128: { "worldId": 9, "name": "SpacePod", "display": "Containment Pod", "areaId": 6, "hideWorld": 0, },129: { "worldId": 9, "name": "SpaceHub", "display": "Ship Hub", "areaId": 7, "hideWorld": 0, },130: { "worldId": 9, "name": "SpaceMachineryBay", "display": "Machinery Bay", "areaId": 8, "hideWorld": 0, },131: { "worldId": 9, "name": "SpaceLaunch", "display": "Launch Deck", "areaId": 9, "hideWorld": 0, },132: { "worldId": 9, "name": "SpaceExterior", "display": "Ship Exterior", "areaId": 10, "hideWorld": 0, },133: { "worldId": 9, "name": "SpaceOuter", "display": "Outer Space", "areaId": 11, "hideWorld": 0, },134: { "worldId": 9, "name": "SpaceCorridor2", "display": "Ship Corridor", "areaId": 12, "hideWorld": 0, },135: { "worldId": 9, "name": "SpaceLanesBetween", "display": "The Lanes Between", "areaId": 13, "hideWorld": 0, },136: { "worldId": 9, "name": "SpaceMachineryBayAccess", "display": "Machinery Bay Access", "areaId": 14, "hideWorld": 0, },137: { "worldId": 10, "name": "DestinyBeachDay", "display": "Island Beach", "areaId": 1, "hideWorld": 0, },138: { "worldId": 10, "name": "DestinyBeachSunset", "display": "Island Beach", "areaId": 2, "hideWorld": 0, },139: { "worldId": 10, "name": "DestinyBeachNight", "display": "Island Beach", "areaId": 3, "hideWorld": 0, },140: { "worldId": 10, "name": "DestinyMainIsland", "display": "Main Island Beach", "areaId": 4, "hideWorld": 0, },141: { "worldId": 11, "name": "NeverlandCove", "display": "Cove", "areaId": 1, "hideWorld": 0, },142: { "worldId": 11, "name": "NeverlandCliff", "display": "Cliff Path", "areaId": 2, "hideWorld": 0, },143: { "worldId": 11, "name": "NeverlandLagoon", "display": "Mermaid Lagoon", "areaId": 3, "hideWorld": 0, },144: { "worldId": 11, "name": "NeverlandSeacoast", "display": "Seacoast", "areaId": 4, "hideWorld": 0, },145: { "worldId": 11, "name": "NeverlandClearing", "display": "Jungle Clearing", "areaId": 5, "hideWorld": 0, },146: { "worldId": 11, "name": "NeverlandHideout", "display": "Peter’s Hideout", "areaId": 6, "hideWorld": 0, },147: { "worldId": 11, "name": "NeverlandGully", "display": "Gully", "areaId": 7, "hideWorld": 0, },148: { "worldId": 11, "name": "NeverlandCamp", "display": "Indian Camp", "areaId": 8, "hideWorld": 0, },149: { "worldId": 11, "name": "NeverlandBase", "display": "Rainbow Falls: Base", "areaId": 9, "hideWorld": 0, },150: { "worldId": 11, "name": "NeverlandAscent", "display": "Rainbow Falls: Ascent", "areaId": 10, "hideWorld": 0, },151: { "worldId": 11, "name": "NeverlandCrest", "display": "Rainbow Falls: Crest", "areaId": 11, "hideWorld": 0, },152: { "worldId": 11, "name": "NeverlandSkullEntrance", "display": "Skull Rock: Entrance", "areaId": 12, "hideWorld": 0, },153: { "worldId": 11, "name": "NeverlandSkullCavern", "display": "Skull Rock: Cavern", "areaId": 13, "hideWorld": 0, },154: { "worldId": 11, "name": "NeverlandSky", "display": "Night Sky", "areaId": 14, "hideWorld": 0, },155: { "worldId": 12, "name": "DisneyLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },156: { "worldId": 12, "name": "DisneyPlaza", "display": "Main Plaza", "areaId": 2, "hideWorld": 0, },157: { "worldId": 12, "name": "DisneyFruitballCourt", "display": "Fruitball Course", "areaId": 3, "hideWorld": 0, },158: { "worldId": 12, "name": "DisneyCountryChase", "display": "Country Chase", "areaId": 4, "hideWorld": 0, },159: { "worldId": 12, "name": "DisneyRaceway", "display": "Raceway", "areaId": 5, "hideWorld": 0, },160: { "worldId": 12, "name": "DisneyGizmo", "display": "Gizmo Gallery", "areaId": 6, "hideWorld": 0, },161: { "worldId": 12, "name": "DisneyRecRoom", "display": "Pete’s Rec Room", "areaId": 7, "hideWorld": 0, },162: { "worldId": 12, "name": "DisneyDrive", "display": "Disney Drive", "areaId": 8, "hideWorld": 0, },163: { "worldId": 12, "name": "DisneyCourseC", "display": "Racecourse C", "areaId": 9, "hideWorld": 0, },164: { "worldId": 12, "name": "DisneyCourseD", "display": "Racecourse D", "areaId": 10, "hideWorld": 0, },165: { "worldId": 12, "name": "DisneyLanesBetween", "display": "The Lanes Between", "areaId": 11, "hideWorld": 0, },166: { "worldId": 12, "name": "DisneyRegistration", "display": "Raceway Registration", "areaId": 12, "hideWorld": 0, },167: { "worldId": 12, "name": "DisneyIceCream", "display": "Ice Cream", "areaId": 13, "hideWorld": 0, },168: { "worldId": 12, "name": "DisneyFruitball", "display": "Fruitball", "areaId": 14, "hideWorld": 0, },169: { "worldId": 12, "name": "DisneyCourseCastle", "display": "Race: Castle Course", "areaId": 15, "hideWorld": 0, },170: { "worldId": 13, "name": "GraveyardBadlands", "display": "Badlands", "areaId": 1, "hideWorld": 0, },171: { "worldId": 13, "name": "GraveyardWar", "display": "Seat of War", "areaId": 2, "hideWorld": 0, },172: { "worldId": 13, "name": "GraveyardTwister", "display": "Twister Trench", "areaId": 3, "hideWorld": 0, },173: { "worldId": 13, "name": "GraveyardEye1", "display": "Eye of the Storm", "areaId": 4, "hideWorld": 0, },174: { "worldId": 13, "name": "GraveyardEye2", "display": "Eye of the Storm", "areaId": 5, "hideWorld": 0, },175: { "worldId": 13, "name": "GraveyardEye3", "display": "Eye of the Storm", "areaId": 6, "hideWorld": 0, },176: { "worldId": 13, "name": "GraveyardFissure", "display": "Fissure", "areaId": 7, "hideWorld": 0, },177: { "worldId": 13, "name": "Graveyard1", "display": "Keyblade Graveyard", "areaId": 8, "hideWorld": 1, },178: { "worldId": 13, "name": "Graveyard2", "display": "Keyblade Graveyard", "areaId": 9, "hideWorld": 1, },179: { "worldId": 13, "name": "Graveyard3", "display": "Keyblade Graveyard", "areaId": 10, "hideWorld": 1, },180: { "worldId": 13, "name": "GraveyardCage", "display": "Will’s Cage", "areaId": 11, "hideWorld": 0, },181: { "worldId": 13, "name": "Graveyard4", "display": "Keyblade Graveyard", "areaId": 12, "hideWorld": 1, },182: { "worldId": 13, "name": "VentusHeart1", "display": "Ventus’s Heart", "areaId": 50, "hideWorld": 0, },183: { "worldId": 13, "name": "VentusHeart2", "display": "Ventus’s Heart", "areaId": 51, "hideWorld": 0, },184: { "worldId": 13, "name": "VentusHeart3", "display": "Ventus’s Heart", "areaId": 52, "hideWorld": 0, },185: { "worldId": 13, "name": "SoraHeart", "display": "Sora’s Heart", "areaId": 53, "hideWorld": 0, },186: { "worldId": 13, "name": "TerraHeart", "display": "Terra’s Heart", "areaId": 54, "hideWorld": 0, },187: { "worldId": 13, "name": "Graveyard5", "display": "Keyblade Graveyard", "areaId": 55, "hideWorld": 0, },188: { "worldId": 13, "name": "GraveyardBadlands2", "display": "Badlands", "areaId": 56, "hideWorld": 0, },189: { "worldId": 15, "name": "MirageHub", "display": "Hub", "areaId": 1, "hideWorld": 0, },190: { "worldId": 15, "name": "MirageColiseum", "display": "Coliseum", "areaId": 2, "hideWorld": 0, },191: { "worldId": 15, "name": "MirageArena1", "display": "Arena", "areaId": 3, "hideWorld": 0, },192: { "worldId": 15, "name": "MirageBadlands", "display": "Badlands", "areaId": 4, "hideWorld": 0, },193: { "worldId": 15, "name": "MiragePinball", "display": "Pinball", "areaId": 5, "hideWorld": 0, },194: { "worldId": 15, "name": "MirageShipHub", "display": "Ship Hub", "areaId": 6, "hideWorld": 0, },195: { "worldId": 15, "name": "MirageMousehole", "display": "Mousehole", "areaId": 7, "hideWorld": 0, },196: { "worldId": 15, "name": "MirageForest", "display": "Forest", "areaId": 8, "hideWorld": 0, },197: { "worldId": 15, "name": "MirageSkull", "display": "Skull Rock", "areaId": 9, "hideWorld": 0, },198: { "worldId": 15, "name": "MirageChamber", "display": "Audience Chamber", "areaId": 10, "hideWorld": 0, },199: { "worldId": 15, "name": "MirageForecourt", "display": "Forecourt", "areaId": 11, "hideWorld": 0, },200: { "worldId": 15, "name": "MirageSummit", "display": "Summit", "areaId": 12, "hideWorld": 0, },201: { "worldId": 15, "name": "MirageDeck", "display": "Launch Deck", "areaId": 13, "hideWorld": 0, },202: { "worldId": 15, "name": "MirageExterior", "display": "Ship Exterior", "areaId": 14, "hideWorld": 0, },203: { "worldId": 15, "name": "MirageArena2", "display": "Arena", "areaId": 15, "hideWorld": 0, },204: { "worldId": 16, "name": "CommandDeparture", "display": "The Land of Departure Command Board", "areaId": 1, "hideWorld": 1, },205: { "worldId": 16, "name": "CommandCinderella", "display": "Cinderella Command Board", "areaId": 3, "hideWorld": 1, },206: { "worldId": 16, "name": "CommandSitch", "display": "Lilo and Stitch Command Board", "areaId": 9, "hideWorld": 1, },207: { "worldId": 16, "name": "CommandPan", "display": "Peter Pan Command Board", "areaId": 11, "hideWorld": 1, },208: { "worldId": 16, "name": "CommandDisney", "display": "Disney Castle Command Board", "areaId": 12, "hideWorld": 1, },209: { "worldId": 16, "name": "CommandPooh", "display": "Winnie the Pooh Command Board", "areaId": 18, "hideWorld": 1, },210: { "worldId": 16, "name": "CommandPan2", "display": "Peter Pan Command Board", "areaId": 19, "hideWorld": 1, },211: { "worldId": 17, "name": "WorldMap", "display": "World Map", "areaId": 1, "hideWorld": 1, },</v>
+        <v>0: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },1: { "worldId": 1, "name": "DepartureForecourtDay", "display": "Forecourt", "areaId": 1, "hideWorld": 0, },2: { "worldId": 1, "name": "DepartureGreatHall", "display": "Great Hall", "areaId": 2, "hideWorld": 0, },3: { "worldId": 1, "name": "VentusRoomDay", "display": "Ventus’s Room", "areaId": 3, "hideWorld": 0, },4: { "worldId": 1, "name": "VentusRoomNight", "display": "Ventus’s Room", "areaId": 4, "hideWorld": 0, },6: { "worldId": 1, "name": "DepartureMountainPath", "display": "Mountain Path", "areaId": 5, "hideWorld": 0, },7: { "worldId": 1, "name": "DepartureSummitNight", "display": "Summit", "areaId": 6, "hideWorld": 0, },8: { "worldId": 1, "name": "DepartureForecourtNight", "display": "Forecourt", "areaId": 7, "hideWorld": 0, },9: { "worldId": 1, "name": "DepartureForecourtRuins", "display": "Forecourt", "areaId": 8, "hideWorld": 0, },10: { "worldId": 1, "name": "DepartureGreatHallRuins", "display": "Great Hall", "areaId": 9, "hideWorld": 0, },11: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 10, "hideWorld": 0, },12: { "worldId": 1, "name": "ChamberOfWaking", "display": "Chamber of Waking", "areaId": 11, "hideWorld": 0, },13: { "worldId": 1, "name": "CastleOblivion", "display": "Castle Oblivion", "areaId": 12, "hideWorld": 0, },14: { "worldId": 1, "name": "CharacterSelect", "display": "Selecting a character…", "areaId": 13, "hideWorld": 1, },15: { "worldId": 1, "name": "DepartureForecourtRuins2", "display": "Forecourt", "areaId": 14, "hideWorld": 0, },16: { "worldId": 1, "name": "DepartureMountainPathRuins", "display": "Mountain Path", "areaId": 15, "hideWorld": 0, },17: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 16, "hideWorld": 0, },18: { "worldId": 2, "name": "DwarfMineEntrance", "display": "Mine Entrance", "areaId": 1, "hideWorld": 0, },19: { "worldId": 2, "name": "DwarfMine", "display": "The Mine", "areaId": 2, "hideWorld": 0, },20: { "worldId": 2, "name": "DwarfVault", "display": "Vault", "areaId": 3, "hideWorld": 0, },21: { "worldId": 2, "name": "DwarfMirrorChamber", "display": "Magic Mirror Chamber", "areaId": 4, "hideWorld": 0, },22: { "worldId": 2, "name": "DwarfWaterway", "display": "Underground Waterway", "areaId": 5, "hideWorld": 0, },23: { "worldId": 2, "name": "DwarfCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },24: { "worldId": 2, "name": "DwarfGlade", "display": "Flower Glade", "areaId": 7, "hideWorld": 0, },25: { "worldId": 2, "name": "DwarfWoods", "display": "Deep Woods", "areaId": 8, "hideWorld": 0, },26: { "worldId": 2, "name": "DwarfMirror", "display": "Inside the Magic Mirror", "areaId": 9, "hideWorld": 0, },27: { "worldId": 2, "name": "DwarfClearing", "display": "Cottage Clearing", "areaId": 10, "hideWorld": 0, },28: { "worldId": 2, "name": "DwarfCottage", "display": "The Cottage", "areaId": 11, "hideWorld": 0, },29: { "worldId": 2, "name": "DwarfMountainTrail", "display": "Mountain Trail", "areaId": 12, "hideWorld": 0, },30: { "worldId": 3, "name": "CastleHouse", "display": "Cinderella’s House", "areaId": 1, "hideWorld": 0, },31: { "worldId": 3, "name": "CastleMousehole", "display": "Mousehole", "areaId": 2, "hideWorld": 0, },32: { "worldId": 3, "name": "CastleWardrobe", "display": "Wardrobe Room", "areaId": 3, "hideWorld": 0, },33: { "worldId": 3, "name": "CastleEntrance", "display": "Entrance", "areaId": 4, "hideWorld": 0, },34: { "worldId": 3, "name": "CastleChateau", "display": "The Chateau", "areaId": 5, "hideWorld": 0, },35: { "worldId": 3, "name": "CastleForest", "display": "Forest", "areaId": 6, "hideWorld": 0, },36: { "worldId": 3, "name": "CastleCourtyard", "display": "Palace Courtyard", "areaId": 7, "hideWorld": 0, },37: { "worldId": 3, "name": "CastleCorridor", "display": "Corridor", "areaId": 8, "hideWorld": 0, },38: { "worldId": 3, "name": "CastleBallroom", "display": "Ballroom", "areaId": 9, "hideWorld": 0, },39: { "worldId": 3, "name": "CastleFoyer", "display": "Foyer", "areaId": 10, "hideWorld": 0, },40: { "worldId": 3, "name": "CastlePassage", "display": "Passage", "areaId": 11, "hideWorld": 0, },41: { "worldId": 3, "name": "CastleAntechamber", "display": "Antechamber", "areaId": 12, "hideWorld": 0, },42: { "worldId": 3, "name": "CastleWardrobe2", "display": "Wardrobe Room", "areaId": 13, "hideWorld": 0, },43: { "worldId": 3, "name": "CastleMousehole2", "display": "Mousehole", "areaId": 14, "hideWorld": 0, },44: { "worldId": 3, "name": "CastleWardrobe3", "display": "Wardrobe Room", "areaId": 15, "hideWorld": 0, },45: { "worldId": 4, "name": "EnchantedDungeonCell", "display": "Dungeon Cell", "areaId": 1, "hideWorld": 0, },46: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 2, "hideWorld": 0, },47: { "worldId": 4, "name": "EnchantedThrone", "display": "Maleficent’s Throne", "areaId": 3, "hideWorld": 0, },48: { "worldId": 4, "name": "EnchantedDungeon", "display": "Dungeon", "areaId": 4, "hideWorld": 0, },49: { "worldId": 4, "name": "EnchantedHall1", "display": "Hall", "areaId": 5, "hideWorld": 0, },50: { "worldId": 4, "name": "EnchantedMountain", "display": "Forbidden Mountain", "areaId": 6, "hideWorld": 0, },51: { "worldId": 4, "name": "EnchantedWaterside", "display": "Waterside", "areaId": 7, "hideWorld": 0, },52: { "worldId": 4, "name": "EnchantedClearing", "display": "Forest Clearing", "areaId": 8, "hideWorld": 0, },53: { "worldId": 4, "name": "EnchantedBridge", "display": "Bridge", "areaId": 9, "hideWorld": 0, },54: { "worldId": 4, "name": "EnchantedBridgeThorns", "display": "Bridge", "areaId": 10, "hideWorld": 0, },55: { "worldId": 4, "name": "EnchantedAudience1", "display": "Audience Chamber", "areaId": 11, "hideWorld": 0, },56: { "worldId": 4, "name": "EnchantedAudience2", "display": "Audience Chamber", "areaId": 12, "hideWorld": 0, },57: { "worldId": 4, "name": "EnchantedReserved", "display": "Somewhere in the World…", "areaId": 13, "hideWorld": 1, },58: { "worldId": 4, "name": "EnchantedHallway", "display": "Hallway", "areaId": 14, "hideWorld": 0, },59: { "worldId": 4, "name": "EnchantedAurora", "display": "Aurora’s Chamber", "areaId": 15, "hideWorld": 0, },60: { "worldId": 4, "name": "EnchantedTower", "display": "Tower Room", "areaId": 16, "hideWorld": 0, },61: { "worldId": 4, "name": "EnchantedHall2", "display": "Hall", "areaId": 17, "hideWorld": 0, },62: { "worldId": 4, "name": "EnchantedAurora2", "display": "Aurora’s Chamber", "areaId": 18, "hideWorld": 0, },63: { "worldId": 4, "name": "EnchantedHall3", "display": "Hall", "areaId": 19, "hideWorld": 0, },64: { "worldId": 4, "name": "EnchantedHall4", "display": "Hall", "areaId": 20, "hideWorld": 0, },65: { "worldId": 4, "name": "EnchantedHall5", "display": "Hall", "areaId": 21, "hideWorld": 0, },66: { "worldId": 4, "name": "EnchantedHall6", "display": "Hall", "areaId": 22, "hideWorld": 0, },67: { "worldId": 4, "name": "EnchantedHall7", "display": "Hall", "areaId": 23, "hideWorld": 0, },68: { "worldId": 4, "name": "EnchantedHall8", "display": "Hall", "areaId": 24, "hideWorld": 0, },69: { "worldId": 4, "name": "EnchantedHall9", "display": "Hall", "areaId": 25, "hideWorld": 0, },70: { "worldId": 4, "name": "EnchantedHall10", "display": "Hall", "areaId": 26, "hideWorld": 0, },71: { "worldId": 4, "name": "EnchantedHall11", "display": "Hall", "areaId": 27, "hideWorld": 0, },72: { "worldId": 4, "name": "EnchantedHall12", "display": "Hall", "areaId": 28, "hideWorld": 0, },73: { "worldId": 4, "name": "EnchantedHall13", "display": "Hall", "areaId": 29, "hideWorld": 0, },74: { "worldId": 4, "name": "EnchantedHall14", "display": "Hall", "areaId": 30, "hideWorld": 0, },75: { "worldId": 4, "name": "EnchantedHall15", "display": "Hall", "areaId": 31, "hideWorld": 0, },76: { "worldId": 4, "name": "EnchantedHall16", "display": "Hall", "areaId": 32, "hideWorld": 0, },77: { "worldId": 4, "name": "EnchantedHall17", "display": "Hall", "areaId": 33, "hideWorld": 0, },78: { "worldId": 4, "name": "EnchantedHall18", "display": "Hall", "areaId": 34, "hideWorld": 0, },79: { "worldId": 4, "name": "EnchantedHall19", "display": "Hall", "areaId": 35, "hideWorld": 0, },80: { "worldId": 4, "name": "EnchantedHall20", "display": "Hall", "areaId": 36, "hideWorld": 0, },81: { "worldId": 4, "name": "EnchantedHall21", "display": "Hall", "areaId": 37, "hideWorld": 0, },82: { "worldId": 4, "name": "EnchantedHall22", "display": "Hall", "areaId": 38, "hideWorld": 0, },83: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 39, "hideWorld": 0, },84: { "worldId": 5, "name": "MysteriousChamber", "display": "Sorcerer’s Chamber", "areaId": 1, "hideWorld": 0, },85: { "worldId": 5, "name": "MysteriousTower", "display": "Mysterious Tower", "areaId": 2, "hideWorld": 0, },86: { "worldId": 5, "name": "MysteriousEntrance", "display": "Tower Entrance", "areaId": 3, "hideWorld": 0, },87: { "worldId": 5, "name": "MysteriousChamber2", "display": "Sorcerer’s Chamber", "areaId": 4, "hideWorld": 0, },88: { "worldId": 6, "name": "RadiantOuterGardens", "display": "Outer Gardens", "areaId": 1, "hideWorld": 0, },89: { "worldId": 6, "name": "RadiantEntryway", "display": "Entryway", "areaId": 2, "hideWorld": 0, },90: { "worldId": 6, "name": "RadiantCentral", "display": "Central Square", "areaId": 3, "hideWorld": 0, },91: { "worldId": 6, "name": "RadiantAqueduct", "display": "Aqueduct", "areaId": 4, "hideWorld": 0, },92: { "worldId": 6, "name": "RadiantTown", "display": "Castle Town", "areaId": 5, "hideWorld": 0, },93: { "worldId": 6, "name": "RadiantReactor", "display": "Reactor", "areaId": 6, "hideWorld": 0, },94: { "worldId": 6, "name": "RadiantFountain", "display": "Fountain Court", "areaId": 7, "hideWorld": 0, },95: { "worldId": 6, "name": "RadiantMerlin", "display": "Merlin’s House", "areaId": 8, "hideWorld": 0, },96: { "worldId": 6, "name": "RadiantGardens", "display": "Gardens", "areaId": 9, "hideWorld": 0, },97: { "worldId": 6, "name": "RadiantDoors", "display": "Front Doors", "areaId": 10, "hideWorld": 0, },98: { "worldId": 6, "name": "RadiantPurification", "display": "Purification Facility", "areaId": 11, "hideWorld": 0, },99: { "worldId": 6, "name": "RadiantOuterGardens2", "display": "Outer Gardens", "areaId": 12, "hideWorld": 0, },100: { "worldId": 6, "name": "RadiantCentralDark", "display": "Central Square", "areaId": 13, "hideWorld": 0, },101: { "worldId": 6, "name": "RadiantCentralTerranort", "display": "Central Square", "areaId": 14, "hideWorld": 0, },102: { "worldId": 7, "name": "LouieCourt", "display": "Louie’s Ruins (Court)", "areaId": 1, "hideWorld": 0, },103: { "worldId": 7, "name": "LouiePath", "display": "Louie’s Ruins (Path)", "areaId": 2, "hideWorld": 0, },104: { "worldId": 7, "name": "Crossroad", "display": "Crossroad", "areaId": 3, "hideWorld": 0, },105: { "worldId": 7, "name": "UGRuinsEntrance", "display": "Underground Ruins (Entrance)", "areaId": 4, "hideWorld": 0, },106: { "worldId": 7, "name": "UGRuinsPassage1", "display": "Underground Ruins (Passage)", "areaId": 5, "hideWorld": 0, },107: { "worldId": 7, "name": "UGRuinsPassage2", "display": "Underground Ruins (Passage)", "areaId": 6, "hideWorld": 0, },108: { "worldId": 7, "name": "UGCourtyard", "display": "Underground Courtyard", "areaId": 7, "hideWorld": 0, },109: { "worldId": 7, "name": "JungleNearRuins", "display": "Jungle Near Ruins", "areaId": 8, "hideWorld": 0, },110: { "worldId": 7, "name": "Eminence", "display": "Eminence", "areaId": 9, "hideWorld": 0, },111: { "worldId": 7, "name": "Jungle", "display": "Jungle", "areaId": 10, "hideWorld": 0, },112: { "worldId": 7, "name": "River", "display": "Man-Village River", "areaId": 11, "hideWorld": 0, },113: { "worldId": 7, "name": "Bog", "display": "Bog", "areaId": 12, "hideWorld": 0, },114: { "worldId": 7, "name": "LanesBetween", "display": "The Lanes Between", "areaId": 50, "hideWorld": 0, },115: { "worldId": 7, "name": "Blank", "display": "Blank", "areaId": 51, "hideWorld": 0, },116: { "worldId": 7, "name": "Realm of Darkness", "display": "The Realm of Darkness", "areaId": 52, "hideWorld": 1, },117: { "worldId": 8, "name": "OlympusGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },118: { "worldId": 8, "name": "OlympusVestibule", "display": "Vestibule", "areaId": 2, "hideWorld": 0, },119: { "worldId": 8, "name": "OlympusWest", "display": "West Bracket", "areaId": 3, "hideWorld": 0, },120: { "worldId": 8, "name": "OlympusEast", "display": "East Bracket", "areaId": 4, "hideWorld": 0, },121: { "worldId": 8, "name": "OlympusTown", "display": "Town Near Thebes", "areaId": 5, "hideWorld": 0, },122: { "worldId": 8, "name": "OlympusEastNight", "display": "East Bracket", "areaId": 6, "hideWorld": 0, },123: { "worldId": 9, "name": "SpaceTuroBlock", "display": "Turo Prison Block", "areaId": 1, "hideWorld": 0, },124: { "worldId": 9, "name": "SpaceTuroTransporter", "display": "Turo Transporter", "areaId": 2, "hideWorld": 0, },125: { "worldId": 9, "name": "SpaceDurgonTransporter", "display": "Durgon Transporter", "areaId": 3, "hideWorld": 0, },126: { "worldId": 9, "name": "SpaceCorridor", "display": "Ship Corridor", "areaId": 4, "hideWorld": 0, },127: { "worldId": 9, "name": "SpaceControl", "display": "Control Room", "areaId": 5, "hideWorld": 0, },128: { "worldId": 9, "name": "SpacePod", "display": "Containment Pod", "areaId": 6, "hideWorld": 0, },129: { "worldId": 9, "name": "SpaceHub", "display": "Ship Hub", "areaId": 7, "hideWorld": 0, },130: { "worldId": 9, "name": "SpaceMachineryBay", "display": "Machinery Bay", "areaId": 8, "hideWorld": 0, },131: { "worldId": 9, "name": "SpaceLaunch", "display": "Launch Deck", "areaId": 9, "hideWorld": 0, },132: { "worldId": 9, "name": "SpaceExterior", "display": "Ship Exterior", "areaId": 10, "hideWorld": 0, },133: { "worldId": 9, "name": "SpaceOuter", "display": "Outer Space", "areaId": 11, "hideWorld": 0, },134: { "worldId": 9, "name": "SpaceCorridor2", "display": "Ship Corridor", "areaId": 12, "hideWorld": 0, },135: { "worldId": 9, "name": "SpaceLanesBetween", "display": "The Lanes Between", "areaId": 13, "hideWorld": 0, },136: { "worldId": 9, "name": "SpaceMachineryBayAccess", "display": "Machinery Bay Access", "areaId": 14, "hideWorld": 0, },137: { "worldId": 10, "name": "DestinyBeachDay", "display": "Island Beach", "areaId": 1, "hideWorld": 0, },138: { "worldId": 10, "name": "DestinyBeachSunset", "display": "Island Beach", "areaId": 2, "hideWorld": 0, },139: { "worldId": 10, "name": "DestinyBeachNight", "display": "Island Beach", "areaId": 3, "hideWorld": 0, },140: { "worldId": 10, "name": "DestinyMainIsland", "display": "Main Island Beach", "areaId": 4, "hideWorld": 0, },141: { "worldId": 11, "name": "NeverlandCove", "display": "Cove", "areaId": 1, "hideWorld": 0, },142: { "worldId": 11, "name": "NeverlandCliff", "display": "Cliff Path", "areaId": 2, "hideWorld": 0, },143: { "worldId": 11, "name": "NeverlandLagoon", "display": "Mermaid Lagoon", "areaId": 3, "hideWorld": 0, },144: { "worldId": 11, "name": "NeverlandSeacoast", "display": "Seacoast", "areaId": 4, "hideWorld": 0, },145: { "worldId": 11, "name": "NeverlandClearing", "display": "Jungle Clearing", "areaId": 5, "hideWorld": 0, },146: { "worldId": 11, "name": "NeverlandHideout", "display": "Peter’s Hideout", "areaId": 6, "hideWorld": 0, },147: { "worldId": 11, "name": "NeverlandGully", "display": "Gully", "areaId": 7, "hideWorld": 0, },148: { "worldId": 11, "name": "NeverlandCamp", "display": "Indian Camp", "areaId": 8, "hideWorld": 0, },149: { "worldId": 11, "name": "NeverlandBase", "display": "Rainbow Falls: Base", "areaId": 9, "hideWorld": 0, },150: { "worldId": 11, "name": "NeverlandAscent", "display": "Rainbow Falls: Ascent", "areaId": 10, "hideWorld": 0, },151: { "worldId": 11, "name": "NeverlandCrest", "display": "Rainbow Falls: Crest", "areaId": 11, "hideWorld": 0, },152: { "worldId": 11, "name": "NeverlandSkullEntrance", "display": "Skull Rock: Entrance", "areaId": 12, "hideWorld": 0, },153: { "worldId": 11, "name": "NeverlandSkullCavern", "display": "Skull Rock: Cavern", "areaId": 13, "hideWorld": 0, },154: { "worldId": 11, "name": "NeverlandSky", "display": "Night Sky", "areaId": 14, "hideWorld": 0, },155: { "worldId": 12, "name": "DisneyLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },156: { "worldId": 12, "name": "DisneyPlaza", "display": "Main Plaza", "areaId": 2, "hideWorld": 0, },157: { "worldId": 12, "name": "DisneyFruitballCourt", "display": "Fruitball Course", "areaId": 3, "hideWorld": 0, },158: { "worldId": 12, "name": "DisneyCountryChase", "display": "Country Chase", "areaId": 4, "hideWorld": 0, },159: { "worldId": 12, "name": "DisneyRaceway", "display": "Raceway", "areaId": 5, "hideWorld": 0, },160: { "worldId": 12, "name": "DisneyGizmo", "display": "Gizmo Gallery", "areaId": 6, "hideWorld": 0, },161: { "worldId": 12, "name": "DisneyRecRoom", "display": "Pete’s Rec Room", "areaId": 7, "hideWorld": 0, },162: { "worldId": 12, "name": "DisneyDrive", "display": "Disney Drive", "areaId": 8, "hideWorld": 0, },163: { "worldId": 12, "name": "DisneySpree", "display": "Grand Spree", "areaId": 9, "hideWorld": 0, },164: { "worldId": 12, "name": "DisneyCastle", "display": "Castle Circuit", "areaId": 10, "hideWorld": 0, },165: { "worldId": 12, "name": "DisneyLanesBetween", "display": "The Lanes Between", "areaId": 11, "hideWorld": 0, },166: { "worldId": 12, "name": "DisneyRegistration", "display": "Raceway Registration", "areaId": 12, "hideWorld": 0, },167: { "worldId": 12, "name": "DisneyIceCream", "display": "Ice Cream", "areaId": 13, "hideWorld": 0, },168: { "worldId": 12, "name": "DisneyFruitball", "display": "Fruitball", "areaId": 14, "hideWorld": 0, },169: { "worldId": 12, "name": "DisneyCourseCastle", "display": "Race: Castle Course", "areaId": 15, "hideWorld": 0, },170: { "worldId": 13, "name": "GraveyardBadlands", "display": "Badlands", "areaId": 1, "hideWorld": 0, },171: { "worldId": 13, "name": "GraveyardWar", "display": "Seat of War", "areaId": 2, "hideWorld": 0, },172: { "worldId": 13, "name": "GraveyardTwister", "display": "Twister Trench", "areaId": 3, "hideWorld": 0, },173: { "worldId": 13, "name": "GraveyardEye1", "display": "Eye of the Storm", "areaId": 4, "hideWorld": 0, },174: { "worldId": 13, "name": "GraveyardEye2", "display": "Eye of the Storm", "areaId": 5, "hideWorld": 0, },175: { "worldId": 13, "name": "GraveyardEye3", "display": "Eye of the Storm", "areaId": 6, "hideWorld": 0, },176: { "worldId": 13, "name": "GraveyardFissure", "display": "Fissure", "areaId": 7, "hideWorld": 0, },177: { "worldId": 13, "name": "Graveyard1", "display": "Keyblade Graveyard", "areaId": 8, "hideWorld": 1, },178: { "worldId": 13, "name": "Graveyard2", "display": "Keyblade Graveyard", "areaId": 9, "hideWorld": 1, },179: { "worldId": 13, "name": "Graveyard3", "display": "Keyblade Graveyard", "areaId": 10, "hideWorld": 1, },180: { "worldId": 13, "name": "GraveyardCage", "display": "Will’s Cage", "areaId": 11, "hideWorld": 0, },181: { "worldId": 13, "name": "Graveyard4", "display": "Keyblade Graveyard", "areaId": 12, "hideWorld": 1, },182: { "worldId": 13, "name": "VentusHeart1", "display": "Ventus’s Heart", "areaId": 50, "hideWorld": 0, },183: { "worldId": 13, "name": "VentusHeart2", "display": "Ventus’s Heart", "areaId": 51, "hideWorld": 0, },184: { "worldId": 13, "name": "VentusHeart3", "display": "Ventus’s Heart", "areaId": 52, "hideWorld": 0, },185: { "worldId": 13, "name": "SoraHeart", "display": "Sora’s Heart", "areaId": 53, "hideWorld": 0, },186: { "worldId": 13, "name": "TerraHeart", "display": "Terra’s Heart", "areaId": 54, "hideWorld": 0, },187: { "worldId": 13, "name": "Graveyard5", "display": "Keyblade Graveyard", "areaId": 55, "hideWorld": 0, },188: { "worldId": 13, "name": "GraveyardBadlands2", "display": "Badlands", "areaId": 56, "hideWorld": 0, },189: { "worldId": 15, "name": "MirageHub", "display": "Hub", "areaId": 1, "hideWorld": 0, },190: { "worldId": 15, "name": "MirageColiseum", "display": "Coliseum", "areaId": 2, "hideWorld": 0, },191: { "worldId": 15, "name": "MirageArena1", "display": "Arena", "areaId": 3, "hideWorld": 0, },192: { "worldId": 15, "name": "MirageBadlands", "display": "Badlands", "areaId": 4, "hideWorld": 0, },193: { "worldId": 15, "name": "MiragePinball", "display": "Pinball", "areaId": 5, "hideWorld": 0, },194: { "worldId": 15, "name": "MirageShipHub", "display": "Ship Hub", "areaId": 6, "hideWorld": 0, },195: { "worldId": 15, "name": "MirageMousehole", "display": "Mousehole", "areaId": 7, "hideWorld": 0, },196: { "worldId": 15, "name": "MirageForest", "display": "Forest", "areaId": 8, "hideWorld": 0, },197: { "worldId": 15, "name": "MirageSkull", "display": "Skull Rock", "areaId": 9, "hideWorld": 0, },198: { "worldId": 15, "name": "MirageChamber", "display": "Audience Chamber", "areaId": 10, "hideWorld": 0, },199: { "worldId": 15, "name": "MirageForecourt", "display": "Forecourt", "areaId": 11, "hideWorld": 0, },200: { "worldId": 15, "name": "MirageSummit", "display": "Summit", "areaId": 12, "hideWorld": 0, },201: { "worldId": 15, "name": "MirageDeck", "display": "Launch Deck", "areaId": 13, "hideWorld": 0, },202: { "worldId": 15, "name": "MirageExterior", "display": "Ship Exterior", "areaId": 14, "hideWorld": 0, },203: { "worldId": 15, "name": "MirageArena2", "display": "Arena", "areaId": 15, "hideWorld": 0, },204: { "worldId": 16, "name": "CommandDeparture", "display": "The Land of Departure Command Board", "areaId": 1, "hideWorld": 1, },205: { "worldId": 16, "name": "CommandCinderella", "display": "Cinderella Command Board", "areaId": 3, "hideWorld": 1, },206: { "worldId": 16, "name": "CommandSitch", "display": "Lilo and Stitch Command Board", "areaId": 9, "hideWorld": 1, },207: { "worldId": 16, "name": "CommandPan", "display": "Peter Pan Command Board", "areaId": 11, "hideWorld": 1, },208: { "worldId": 16, "name": "CommandDisney", "display": "Disney Castle Command Board", "areaId": 12, "hideWorld": 1, },209: { "worldId": 16, "name": "CommandPooh", "display": "Winnie the Pooh Command Board", "areaId": 18, "hideWorld": 1, },210: { "worldId": 16, "name": "CommandPan2", "display": "Peter Pan Command Board", "areaId": 19, "hideWorld": 1, },211: { "worldId": 17, "name": "WorldMap", "display": "World Map", "areaId": 1, "hideWorld": 1, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6873,7 +6873,7 @@
       </c>
       <c r="G164" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A164,": { ""worldId"": ",C164,", ""name"": """,D164,""", ""display"": """,E164,""", ""areaId"": ",B164,", ""hideWorld"": ",F164,", },")</f>
-        <v>163: { "worldId": 12, "name": "DisneyCourseC", "display": "Racecourse C", "areaId": 9, "hideWorld": 0, },</v>
+        <v>163: { "worldId": 12, "name": "DisneySpree", "display": "Grand Spree", "areaId": 9, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6897,7 +6897,7 @@
       </c>
       <c r="G165" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A165,": { ""worldId"": ",C165,", ""name"": """,D165,""", ""display"": """,E165,""", ""areaId"": ",B165,", ""hideWorld"": ",F165,", },")</f>
-        <v>164: { "worldId": 12, "name": "DisneyCourseD", "display": "Racecourse D", "areaId": 10, "hideWorld": 0, },</v>
+        <v>164: { "worldId": 12, "name": "DisneyCastle", "display": "Castle Circuit", "areaId": 10, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8046,11 +8046,11 @@
   </sheetPr>
   <dimension ref="A1:K213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I213" activeCellId="0" sqref="I213"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A199" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A214" activeCellId="0" sqref="A214"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.94140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.95703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -14046,7 +14046,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C95"/>
+  <autoFilter ref="A1:C95"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added more Unversed Mission achievements
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -2242,31 +2242,31 @@
     <t xml:space="preserve">0xf2</t>
   </si>
   <si>
-    <t xml:space="preserve">Illusion L</t>
+    <t xml:space="preserve">Illusion-L</t>
   </si>
   <si>
     <t xml:space="preserve">0xf3</t>
   </si>
   <si>
-    <t xml:space="preserve">Illusion R</t>
+    <t xml:space="preserve">Illusion-F</t>
   </si>
   <si>
     <t xml:space="preserve">0xf4</t>
   </si>
   <si>
-    <t xml:space="preserve">Illusion S</t>
+    <t xml:space="preserve">Illusion-V</t>
   </si>
   <si>
     <t xml:space="preserve">0xf5</t>
   </si>
   <si>
-    <t xml:space="preserve">Illusion P</t>
+    <t xml:space="preserve">Illusion-R</t>
   </si>
   <si>
     <t xml:space="preserve">0xf6</t>
   </si>
   <si>
-    <t xml:space="preserve">Illusion D</t>
+    <t xml:space="preserve">Illusion-B</t>
   </si>
   <si>
     <t xml:space="preserve">0xf7</t>
@@ -2730,7 +2730,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.82421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3022,11 +3022,11 @@
   </sheetPr>
   <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="I219" activeCellId="0" sqref="I219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8169,13 +8169,13 @@
   </sheetPr>
   <dimension ref="A1:N226"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K15" activeCellId="0" sqref="K15"/>
+      <selection pane="bottomLeft" activeCell="C170" activeCellId="0" sqref="C170"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -8228,7 +8228,7 @@
       </c>
       <c r="N1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L2:L1013)</f>
-        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion L", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion R", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion S", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion P", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion D", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },</v>
+        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14443,10 +14443,10 @@
         <v>738</v>
       </c>
       <c r="C167" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="D167" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="E167" s="0" t="n">
         <v>2</v>
@@ -14468,7 +14468,7 @@
       </c>
       <c r="L167" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A167,": { ""id"": ",A167,", ""name"": """,B167,""", ""category"": """,C167,""", ""slots"": ",E167,", ""type"": """,G167,""", ""tier"": ",I167,", ""healsHp"": ",J167,", ""equippableBattleCommand"": ",K167,", ""supercategory"": """,D167,""", ""element"": """,F167,""" },")</f>
-        <v>0xf2: { "id": 0xf2, "name": "Illusion L", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },</v>
+        <v>0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14479,10 +14479,10 @@
         <v>740</v>
       </c>
       <c r="C168" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="D168" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="E168" s="0" t="n">
         <v>2</v>
@@ -14504,7 +14504,7 @@
       </c>
       <c r="L168" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A168,": { ""id"": ",A168,", ""name"": """,B168,""", ""category"": """,C168,""", ""slots"": ",E168,", ""type"": """,G168,""", ""tier"": ",I168,", ""healsHp"": ",J168,", ""equippableBattleCommand"": ",K168,", ""supercategory"": """,D168,""", ""element"": """,F168,""" },")</f>
-        <v>0xf3: { "id": 0xf3, "name": "Illusion R", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },</v>
+        <v>0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14515,10 +14515,10 @@
         <v>742</v>
       </c>
       <c r="C169" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="D169" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="E169" s="0" t="n">
         <v>2</v>
@@ -14540,7 +14540,7 @@
       </c>
       <c r="L169" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A169,": { ""id"": ",A169,", ""name"": """,B169,""", ""category"": """,C169,""", ""slots"": ",E169,", ""type"": """,G169,""", ""tier"": ",I169,", ""healsHp"": ",J169,", ""equippableBattleCommand"": ",K169,", ""supercategory"": """,D169,""", ""element"": """,F169,""" },")</f>
-        <v>0xf4: { "id": 0xf4, "name": "Illusion S", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },</v>
+        <v>0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14551,10 +14551,10 @@
         <v>744</v>
       </c>
       <c r="C170" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="D170" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="E170" s="0" t="n">
         <v>2</v>
@@ -14576,7 +14576,7 @@
       </c>
       <c r="L170" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A170,": { ""id"": ",A170,", ""name"": """,B170,""", ""category"": """,C170,""", ""slots"": ",E170,", ""type"": """,G170,""", ""tier"": ",I170,", ""healsHp"": ",J170,", ""equippableBattleCommand"": ",K170,", ""supercategory"": """,D170,""", ""element"": """,F170,""" },")</f>
-        <v>0xf5: { "id": 0xf5, "name": "Illusion P", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },</v>
+        <v>0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -14587,10 +14587,10 @@
         <v>746</v>
       </c>
       <c r="C171" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="D171" s="0" t="s">
-        <v>712</v>
+        <v>674</v>
       </c>
       <c r="E171" s="0" t="n">
         <v>2</v>
@@ -14612,7 +14612,7 @@
       </c>
       <c r="L171" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A171,": { ""id"": ",A171,", ""name"": """,B171,""", ""category"": """,C171,""", ""slots"": ",E171,", ""type"": """,G171,""", ""tier"": ",I171,", ""healsHp"": ",J171,", ""equippableBattleCommand"": ",K171,", ""supercategory"": """,D171,""", ""element"": """,F171,""" },")</f>
-        <v>0xf6: { "id": 0xf6, "name": "Illusion D", "category": "D-Link", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },</v>
+        <v>0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16596,7 +16596,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C108"/>
+  <autoFilter ref="C1:C108"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added achievements for Ven's story up to the end of the Dwarf Woodlands
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1816" uniqueCount="861">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="864">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -2609,6 +2609,15 @@
   </si>
   <si>
     <t xml:space="preserve">Multivortex</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x13c</t>
+  </si>
+  <si>
+    <t xml:space="preserve">White Calm</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Situational</t>
   </si>
 </sst>
 </file>
@@ -2730,7 +2739,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.83984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3026,7 +3035,7 @@
       <selection pane="topLeft" activeCell="I219" activeCellId="0" sqref="I219"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.43359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8167,15 +8176,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N226"/>
+  <dimension ref="A1:N227"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A149" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="C170" activeCellId="0" sqref="C170"/>
+      <selection pane="bottomLeft" activeCell="K229" activeCellId="0" sqref="K229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -8228,7 +8237,7 @@
       </c>
       <c r="N1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L2:L1013)</f>
-        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },</v>
+        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16595,8 +16604,47 @@
         <v>0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },</v>
       </c>
     </row>
+    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A227" s="0" t="s">
+        <v>861</v>
+      </c>
+      <c r="B227" s="0" t="s">
+        <v>862</v>
+      </c>
+      <c r="C227" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="D227" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="E227" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F227" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="G227" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="H227" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I227" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J227" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K227" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L227" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A227,": { ""id"": ",A227,", ""name"": """,B227,""", ""category"": """,C227,""", ""slots"": ",E227,", ""type"": """,G227,""", ""tier"": ",I227,", ""healsHp"": ",J227,", ""equippableBattleCommand"": ",K227,", ""supercategory"": """,D227,""", ""element"": """,F227,""" },")</f>
+        <v>0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:C108"/>
+  <autoFilter ref="A1:C108"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added achievements for Ven up until the end of the Castle of Dreams
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -250,10 +250,10 @@
     <t xml:space="preserve">Mountain Trail</t>
   </si>
   <si>
-    <t xml:space="preserve">CastleHouse</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Cinderella’s House</t>
+    <t xml:space="preserve">CastleRoom</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Cinderella’s Room</t>
   </si>
   <si>
     <t xml:space="preserve">CastleMousehole</t>
@@ -2739,7 +2739,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.859375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3031,11 +3031,11 @@
   </sheetPr>
   <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A195" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I219" activeCellId="0" sqref="I219"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -3069,7 +3069,7 @@
       </c>
       <c r="I1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(G2:G1000)</f>
-        <v>0: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },1: { "worldId": 1, "name": "DepartureForecourtDay", "display": "Forecourt", "areaId": 1, "hideWorld": 0, },2: { "worldId": 1, "name": "DepartureGreatHall", "display": "Great Hall", "areaId": 2, "hideWorld": 0, },3: { "worldId": 1, "name": "VentusRoomDay", "display": "Ventus’s Room", "areaId": 3, "hideWorld": 0, },4: { "worldId": 1, "name": "VentusRoomNight", "display": "Ventus’s Room", "areaId": 4, "hideWorld": 0, },6: { "worldId": 1, "name": "DepartureMountainPath", "display": "Mountain Path", "areaId": 5, "hideWorld": 0, },7: { "worldId": 1, "name": "DepartureSummitNight", "display": "Summit", "areaId": 6, "hideWorld": 0, },8: { "worldId": 1, "name": "DepartureForecourtNight", "display": "Forecourt", "areaId": 7, "hideWorld": 0, },9: { "worldId": 1, "name": "DepartureForecourtRuins", "display": "Forecourt", "areaId": 8, "hideWorld": 0, },10: { "worldId": 1, "name": "DepartureGreatHallRuins", "display": "Great Hall", "areaId": 9, "hideWorld": 0, },11: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 10, "hideWorld": 0, },12: { "worldId": 1, "name": "ChamberOfWaking", "display": "Chamber of Waking", "areaId": 11, "hideWorld": 0, },13: { "worldId": 1, "name": "CastleOblivion", "display": "Castle Oblivion", "areaId": 12, "hideWorld": 0, },14: { "worldId": 1, "name": "CharacterSelect", "display": "Selecting a character…", "areaId": 13, "hideWorld": 1, },15: { "worldId": 1, "name": "DepartureForecourtRuins2", "display": "Forecourt", "areaId": 14, "hideWorld": 0, },16: { "worldId": 1, "name": "DepartureMountainPathRuins", "display": "Mountain Path", "areaId": 15, "hideWorld": 0, },17: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 16, "hideWorld": 0, },18: { "worldId": 2, "name": "DwarfMineEntrance", "display": "Mine Entrance", "areaId": 1, "hideWorld": 0, },19: { "worldId": 2, "name": "DwarfMine", "display": "The Mine", "areaId": 2, "hideWorld": 0, },20: { "worldId": 2, "name": "DwarfVault", "display": "Vault", "areaId": 3, "hideWorld": 0, },21: { "worldId": 2, "name": "DwarfMirrorChamber", "display": "Magic Mirror Chamber", "areaId": 4, "hideWorld": 0, },22: { "worldId": 2, "name": "DwarfWaterway", "display": "Underground Waterway", "areaId": 5, "hideWorld": 0, },23: { "worldId": 2, "name": "DwarfCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },24: { "worldId": 2, "name": "DwarfGlade", "display": "Flower Glade", "areaId": 7, "hideWorld": 0, },25: { "worldId": 2, "name": "DwarfWoods", "display": "Deep Woods", "areaId": 8, "hideWorld": 0, },26: { "worldId": 2, "name": "DwarfMirror", "display": "Inside the Magic Mirror", "areaId": 9, "hideWorld": 0, },27: { "worldId": 2, "name": "DwarfClearing", "display": "Cottage Clearing", "areaId": 10, "hideWorld": 0, },28: { "worldId": 2, "name": "DwarfCottage", "display": "The Cottage", "areaId": 11, "hideWorld": 0, },29: { "worldId": 2, "name": "DwarfMountainTrail", "display": "Mountain Trail", "areaId": 12, "hideWorld": 0, },30: { "worldId": 3, "name": "CastleHouse", "display": "Cinderella’s House", "areaId": 1, "hideWorld": 0, },31: { "worldId": 3, "name": "CastleMousehole", "display": "Mousehole", "areaId": 2, "hideWorld": 0, },32: { "worldId": 3, "name": "CastleWardrobe", "display": "Wardrobe Room", "areaId": 3, "hideWorld": 0, },33: { "worldId": 3, "name": "CastleEntrance", "display": "Entrance", "areaId": 4, "hideWorld": 0, },34: { "worldId": 3, "name": "CastleChateau", "display": "The Chateau", "areaId": 5, "hideWorld": 0, },35: { "worldId": 3, "name": "CastleForest", "display": "Forest", "areaId": 6, "hideWorld": 0, },36: { "worldId": 3, "name": "CastleCourtyard", "display": "Palace Courtyard", "areaId": 7, "hideWorld": 0, },37: { "worldId": 3, "name": "CastleCorridor", "display": "Corridor", "areaId": 8, "hideWorld": 0, },38: { "worldId": 3, "name": "CastleBallroom", "display": "Ballroom", "areaId": 9, "hideWorld": 0, },39: { "worldId": 3, "name": "CastleFoyer", "display": "Foyer", "areaId": 10, "hideWorld": 0, },40: { "worldId": 3, "name": "CastlePassage", "display": "Passage", "areaId": 11, "hideWorld": 0, },41: { "worldId": 3, "name": "CastleAntechamber", "display": "Antechamber", "areaId": 12, "hideWorld": 0, },42: { "worldId": 3, "name": "CastleWardrobe2", "display": "Wardrobe Room", "areaId": 13, "hideWorld": 0, },43: { "worldId": 3, "name": "CastleMousehole2", "display": "Mousehole", "areaId": 14, "hideWorld": 0, },44: { "worldId": 3, "name": "CastleWardrobe3", "display": "Wardrobe Room", "areaId": 15, "hideWorld": 0, },45: { "worldId": 4, "name": "EnchantedDungeonCell", "display": "Dungeon Cell", "areaId": 1, "hideWorld": 0, },46: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 2, "hideWorld": 0, },47: { "worldId": 4, "name": "EnchantedThrone", "display": "Maleficent’s Throne", "areaId": 3, "hideWorld": 0, },48: { "worldId": 4, "name": "EnchantedDungeon", "display": "Dungeon", "areaId": 4, "hideWorld": 0, },49: { "worldId": 4, "name": "EnchantedHall1", "display": "Hall", "areaId": 5, "hideWorld": 0, },50: { "worldId": 4, "name": "EnchantedMountain", "display": "Forbidden Mountain", "areaId": 6, "hideWorld": 0, },51: { "worldId": 4, "name": "EnchantedWaterside", "display": "Waterside", "areaId": 7, "hideWorld": 0, },52: { "worldId": 4, "name": "EnchantedClearing", "display": "Forest Clearing", "areaId": 8, "hideWorld": 0, },53: { "worldId": 4, "name": "EnchantedBridge", "display": "Bridge", "areaId": 9, "hideWorld": 0, },54: { "worldId": 4, "name": "EnchantedBridgeThorns", "display": "Bridge", "areaId": 10, "hideWorld": 0, },55: { "worldId": 4, "name": "EnchantedAudience1", "display": "Audience Chamber", "areaId": 11, "hideWorld": 0, },56: { "worldId": 4, "name": "EnchantedAudience2", "display": "Audience Chamber", "areaId": 12, "hideWorld": 0, },57: { "worldId": 4, "name": "EnchantedReserved", "display": "Somewhere in the World…", "areaId": 13, "hideWorld": 1, },58: { "worldId": 4, "name": "EnchantedHallway", "display": "Hallway", "areaId": 14, "hideWorld": 0, },59: { "worldId": 4, "name": "EnchantedAurora", "display": "Aurora’s Chamber", "areaId": 15, "hideWorld": 0, },60: { "worldId": 4, "name": "EnchantedTower", "display": "Tower Room", "areaId": 16, "hideWorld": 0, },61: { "worldId": 4, "name": "EnchantedHall2", "display": "Hall", "areaId": 17, "hideWorld": 0, },62: { "worldId": 4, "name": "EnchantedAurora2", "display": "Aurora’s Chamber", "areaId": 18, "hideWorld": 0, },63: { "worldId": 4, "name": "EnchantedHall3", "display": "Hall", "areaId": 19, "hideWorld": 0, },64: { "worldId": 4, "name": "EnchantedHall4", "display": "Hall", "areaId": 20, "hideWorld": 0, },65: { "worldId": 4, "name": "EnchantedHall5", "display": "Hall", "areaId": 21, "hideWorld": 0, },66: { "worldId": 4, "name": "EnchantedHall6", "display": "Hall", "areaId": 22, "hideWorld": 0, },67: { "worldId": 4, "name": "EnchantedHall7", "display": "Hall", "areaId": 23, "hideWorld": 0, },68: { "worldId": 4, "name": "EnchantedHall8", "display": "Hall", "areaId": 24, "hideWorld": 0, },69: { "worldId": 4, "name": "EnchantedHall9", "display": "Hall", "areaId": 25, "hideWorld": 0, },70: { "worldId": 4, "name": "EnchantedHall10", "display": "Hall", "areaId": 26, "hideWorld": 0, },71: { "worldId": 4, "name": "EnchantedHall11", "display": "Hall", "areaId": 27, "hideWorld": 0, },72: { "worldId": 4, "name": "EnchantedHall12", "display": "Hall", "areaId": 28, "hideWorld": 0, },73: { "worldId": 4, "name": "EnchantedHall13", "display": "Hall", "areaId": 29, "hideWorld": 0, },74: { "worldId": 4, "name": "EnchantedHall14", "display": "Hall", "areaId": 30, "hideWorld": 0, },75: { "worldId": 4, "name": "EnchantedHall15", "display": "Hall", "areaId": 31, "hideWorld": 0, },76: { "worldId": 4, "name": "EnchantedHall16", "display": "Hall", "areaId": 32, "hideWorld": 0, },77: { "worldId": 4, "name": "EnchantedHall17", "display": "Hall", "areaId": 33, "hideWorld": 0, },78: { "worldId": 4, "name": "EnchantedHall18", "display": "Hall", "areaId": 34, "hideWorld": 0, },79: { "worldId": 4, "name": "EnchantedHall19", "display": "Hall", "areaId": 35, "hideWorld": 0, },80: { "worldId": 4, "name": "EnchantedHall20", "display": "Hall", "areaId": 36, "hideWorld": 0, },81: { "worldId": 4, "name": "EnchantedHall21", "display": "Hall", "areaId": 37, "hideWorld": 0, },82: { "worldId": 4, "name": "EnchantedHall22", "display": "Hall", "areaId": 38, "hideWorld": 0, },83: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 39, "hideWorld": 0, },84: { "worldId": 5, "name": "MysteriousChamber", "display": "Sorcerer’s Chamber", "areaId": 1, "hideWorld": 0, },85: { "worldId": 5, "name": "MysteriousTower", "display": "Mysterious Tower", "areaId": 2, "hideWorld": 0, },86: { "worldId": 5, "name": "MysteriousEntrance", "display": "Tower Entrance", "areaId": 3, "hideWorld": 0, },87: { "worldId": 5, "name": "MysteriousChamber2", "display": "Sorcerer’s Chamber", "areaId": 4, "hideWorld": 0, },88: { "worldId": 6, "name": "RadiantOuterGardens", "display": "Outer Gardens", "areaId": 1, "hideWorld": 0, },89: { "worldId": 6, "name": "RadiantEntryway", "display": "Entryway", "areaId": 2, "hideWorld": 0, },90: { "worldId": 6, "name": "RadiantCentral", "display": "Central Square", "areaId": 3, "hideWorld": 0, },91: { "worldId": 6, "name": "RadiantAqueduct", "display": "Aqueduct", "areaId": 4, "hideWorld": 0, },92: { "worldId": 6, "name": "RadiantTown", "display": "Castle Town", "areaId": 5, "hideWorld": 0, },93: { "worldId": 6, "name": "RadiantReactor", "display": "Reactor", "areaId": 6, "hideWorld": 0, },94: { "worldId": 6, "name": "RadiantFountain", "display": "Fountain Court", "areaId": 7, "hideWorld": 0, },95: { "worldId": 6, "name": "RadiantMerlin", "display": "Merlin’s House", "areaId": 8, "hideWorld": 0, },96: { "worldId": 6, "name": "RadiantGardens", "display": "Gardens", "areaId": 9, "hideWorld": 0, },97: { "worldId": 6, "name": "RadiantDoors", "display": "Front Doors", "areaId": 10, "hideWorld": 0, },98: { "worldId": 6, "name": "RadiantPurification", "display": "Purification Facility", "areaId": 11, "hideWorld": 0, },99: { "worldId": 6, "name": "RadiantOuterGardens2", "display": "Outer Gardens", "areaId": 12, "hideWorld": 0, },100: { "worldId": 6, "name": "RadiantCentralDark", "display": "Central Square", "areaId": 13, "hideWorld": 0, },101: { "worldId": 6, "name": "RadiantCentralTerranort", "display": "Central Square", "areaId": 14, "hideWorld": 0, },102: { "worldId": 7, "name": "LouieCourt", "display": "Louie’s Ruins (Court)", "areaId": 1, "hideWorld": 0, },103: { "worldId": 7, "name": "LouiePath", "display": "Louie’s Ruins (Path)", "areaId": 2, "hideWorld": 0, },104: { "worldId": 7, "name": "Crossroad", "display": "Crossroad", "areaId": 3, "hideWorld": 0, },105: { "worldId": 7, "name": "UGRuinsEntrance", "display": "Underground Ruins (Entrance)", "areaId": 4, "hideWorld": 0, },106: { "worldId": 7, "name": "UGRuinsPassage1", "display": "Underground Ruins (Passage)", "areaId": 5, "hideWorld": 0, },107: { "worldId": 7, "name": "UGRuinsPassage2", "display": "Underground Ruins (Passage)", "areaId": 6, "hideWorld": 0, },108: { "worldId": 7, "name": "UGCourtyard", "display": "Underground Courtyard", "areaId": 7, "hideWorld": 0, },109: { "worldId": 7, "name": "JungleNearRuins", "display": "Jungle Near Ruins", "areaId": 8, "hideWorld": 0, },110: { "worldId": 7, "name": "Eminence", "display": "Eminence", "areaId": 9, "hideWorld": 0, },111: { "worldId": 7, "name": "Jungle", "display": "Jungle", "areaId": 10, "hideWorld": 0, },112: { "worldId": 7, "name": "River", "display": "Man-Village River", "areaId": 11, "hideWorld": 0, },113: { "worldId": 7, "name": "Bog", "display": "Bog", "areaId": 12, "hideWorld": 0, },114: { "worldId": 7, "name": "LanesBetween", "display": "The Lanes Between", "areaId": 50, "hideWorld": 0, },115: { "worldId": 7, "name": "Blank", "display": "Blank", "areaId": 51, "hideWorld": 0, },116: { "worldId": 7, "name": "Realm of Darkness", "display": "The Realm of Darkness", "areaId": 52, "hideWorld": 1, },117: { "worldId": 8, "name": "OlympusGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },118: { "worldId": 8, "name": "OlympusVestibule", "display": "Vestibule", "areaId": 2, "hideWorld": 0, },119: { "worldId": 8, "name": "OlympusWest", "display": "West Bracket", "areaId": 3, "hideWorld": 0, },120: { "worldId": 8, "name": "OlympusEast", "display": "East Bracket", "areaId": 4, "hideWorld": 0, },121: { "worldId": 8, "name": "OlympusTown", "display": "Town Near Thebes", "areaId": 5, "hideWorld": 0, },122: { "worldId": 8, "name": "OlympusEastNight", "display": "East Bracket", "areaId": 6, "hideWorld": 0, },123: { "worldId": 9, "name": "SpaceTuroBlock", "display": "Turo Prison Block", "areaId": 1, "hideWorld": 0, },124: { "worldId": 9, "name": "SpaceTuroTransporter", "display": "Turo Transporter", "areaId": 2, "hideWorld": 0, },125: { "worldId": 9, "name": "SpaceDurgonTransporter", "display": "Durgon Transporter", "areaId": 3, "hideWorld": 0, },126: { "worldId": 9, "name": "SpaceCorridor", "display": "Ship Corridor", "areaId": 4, "hideWorld": 0, },127: { "worldId": 9, "name": "SpaceControl", "display": "Control Room", "areaId": 5, "hideWorld": 0, },128: { "worldId": 9, "name": "SpacePod", "display": "Containment Pod", "areaId": 6, "hideWorld": 0, },129: { "worldId": 9, "name": "SpaceHub", "display": "Ship Hub", "areaId": 7, "hideWorld": 0, },130: { "worldId": 9, "name": "SpaceMachineryBay", "display": "Machinery Bay", "areaId": 8, "hideWorld": 0, },131: { "worldId": 9, "name": "SpaceLaunch", "display": "Launch Deck", "areaId": 9, "hideWorld": 0, },132: { "worldId": 9, "name": "SpaceExterior", "display": "Ship Exterior", "areaId": 10, "hideWorld": 0, },133: { "worldId": 9, "name": "SpaceOuter", "display": "Outer Space", "areaId": 11, "hideWorld": 0, },134: { "worldId": 9, "name": "SpaceCorridor2", "display": "Ship Corridor", "areaId": 12, "hideWorld": 0, },135: { "worldId": 9, "name": "SpaceLanesBetween", "display": "The Lanes Between", "areaId": 13, "hideWorld": 0, },136: { "worldId": 9, "name": "SpaceMachineryBayAccess", "display": "Machinery Bay Access", "areaId": 14, "hideWorld": 0, },137: { "worldId": 10, "name": "DestinyBeachDay", "display": "Island Beach", "areaId": 1, "hideWorld": 0, },138: { "worldId": 10, "name": "DestinyBeachSunset", "display": "Island Beach", "areaId": 2, "hideWorld": 0, },139: { "worldId": 10, "name": "DestinyBeachNight", "display": "Island Beach", "areaId": 3, "hideWorld": 0, },140: { "worldId": 10, "name": "DestinyMainIsland", "display": "Main Island Beach", "areaId": 4, "hideWorld": 0, },141: { "worldId": 11, "name": "NeverlandCove", "display": "Cove", "areaId": 1, "hideWorld": 0, },142: { "worldId": 11, "name": "NeverlandCliff", "display": "Cliff Path", "areaId": 2, "hideWorld": 0, },143: { "worldId": 11, "name": "NeverlandLagoon", "display": "Mermaid Lagoon", "areaId": 3, "hideWorld": 0, },144: { "worldId": 11, "name": "NeverlandSeacoast", "display": "Seacoast", "areaId": 4, "hideWorld": 0, },145: { "worldId": 11, "name": "NeverlandClearing", "display": "Jungle Clearing", "areaId": 5, "hideWorld": 0, },146: { "worldId": 11, "name": "NeverlandHideout", "display": "Peter’s Hideout", "areaId": 6, "hideWorld": 0, },147: { "worldId": 11, "name": "NeverlandGully", "display": "Gully", "areaId": 7, "hideWorld": 0, },148: { "worldId": 11, "name": "NeverlandCamp", "display": "Indian Camp", "areaId": 8, "hideWorld": 0, },149: { "worldId": 11, "name": "NeverlandBase", "display": "Rainbow Falls: Base", "areaId": 9, "hideWorld": 0, },150: { "worldId": 11, "name": "NeverlandAscent", "display": "Rainbow Falls: Ascent", "areaId": 10, "hideWorld": 0, },151: { "worldId": 11, "name": "NeverlandCrest", "display": "Rainbow Falls: Crest", "areaId": 11, "hideWorld": 0, },152: { "worldId": 11, "name": "NeverlandSkullEntrance", "display": "Skull Rock: Entrance", "areaId": 12, "hideWorld": 0, },153: { "worldId": 11, "name": "NeverlandSkullCavern", "display": "Skull Rock: Cavern", "areaId": 13, "hideWorld": 0, },154: { "worldId": 11, "name": "NeverlandSky", "display": "Night Sky", "areaId": 14, "hideWorld": 0, },155: { "worldId": 12, "name": "DisneyLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },156: { "worldId": 12, "name": "DisneyPlaza", "display": "Main Plaza", "areaId": 2, "hideWorld": 0, },157: { "worldId": 12, "name": "DisneyFruitballCourt", "display": "Fruitball Course", "areaId": 3, "hideWorld": 0, },158: { "worldId": 12, "name": "DisneyCountryChase", "display": "Country Chase", "areaId": 4, "hideWorld": 0, },159: { "worldId": 12, "name": "DisneyRaceway", "display": "Raceway", "areaId": 5, "hideWorld": 0, },160: { "worldId": 12, "name": "DisneyGizmo", "display": "Gizmo Gallery", "areaId": 6, "hideWorld": 0, },161: { "worldId": 12, "name": "DisneyRecRoom", "display": "Pete’s Rec Room", "areaId": 7, "hideWorld": 0, },162: { "worldId": 12, "name": "DisneyDrive", "display": "Disney Drive", "areaId": 8, "hideWorld": 0, },163: { "worldId": 12, "name": "DisneySpree", "display": "Grand Spree", "areaId": 9, "hideWorld": 0, },164: { "worldId": 12, "name": "DisneyCastle", "display": "Castle Circuit", "areaId": 10, "hideWorld": 0, },165: { "worldId": 12, "name": "DisneyLanesBetween", "display": "The Lanes Between", "areaId": 11, "hideWorld": 0, },166: { "worldId": 12, "name": "DisneyRegistration", "display": "Raceway Registration", "areaId": 12, "hideWorld": 0, },167: { "worldId": 12, "name": "DisneyIceCream", "display": "Ice Cream", "areaId": 13, "hideWorld": 0, },168: { "worldId": 12, "name": "DisneyFruitball", "display": "Fruitball", "areaId": 14, "hideWorld": 0, },169: { "worldId": 12, "name": "DisneyCourseCastle", "display": "Race: Castle Course", "areaId": 15, "hideWorld": 0, },170: { "worldId": 13, "name": "GraveyardBadlands", "display": "Badlands", "areaId": 1, "hideWorld": 0, },171: { "worldId": 13, "name": "GraveyardWar", "display": "Seat of War", "areaId": 2, "hideWorld": 0, },172: { "worldId": 13, "name": "GraveyardTwister", "display": "Twister Trench", "areaId": 3, "hideWorld": 0, },173: { "worldId": 13, "name": "GraveyardEye1", "display": "Eye of the Storm", "areaId": 4, "hideWorld": 0, },174: { "worldId": 13, "name": "GraveyardEye2", "display": "Eye of the Storm", "areaId": 5, "hideWorld": 0, },175: { "worldId": 13, "name": "GraveyardEye3", "display": "Eye of the Storm", "areaId": 6, "hideWorld": 0, },176: { "worldId": 13, "name": "GraveyardFissure", "display": "Fissure", "areaId": 7, "hideWorld": 0, },177: { "worldId": 13, "name": "Graveyard1", "display": "Keyblade Graveyard", "areaId": 8, "hideWorld": 1, },178: { "worldId": 13, "name": "Graveyard2", "display": "Keyblade Graveyard", "areaId": 9, "hideWorld": 1, },179: { "worldId": 13, "name": "Graveyard3", "display": "Keyblade Graveyard", "areaId": 10, "hideWorld": 1, },180: { "worldId": 13, "name": "GraveyardCage", "display": "Will’s Cage", "areaId": 11, "hideWorld": 0, },181: { "worldId": 13, "name": "Graveyard4", "display": "Keyblade Graveyard", "areaId": 12, "hideWorld": 1, },182: { "worldId": 13, "name": "VentusHeart1", "display": "Ventus’s Heart", "areaId": 50, "hideWorld": 0, },183: { "worldId": 13, "name": "VentusHeart2", "display": "Ventus’s Heart", "areaId": 51, "hideWorld": 0, },184: { "worldId": 13, "name": "VentusHeart3", "display": "Ventus’s Heart", "areaId": 52, "hideWorld": 0, },185: { "worldId": 13, "name": "SoraHeart", "display": "Sora’s Heart", "areaId": 53, "hideWorld": 0, },186: { "worldId": 13, "name": "TerraHeart", "display": "Terra’s Heart", "areaId": 54, "hideWorld": 0, },187: { "worldId": 13, "name": "Graveyard5", "display": "Keyblade Graveyard", "areaId": 55, "hideWorld": 0, },188: { "worldId": 13, "name": "GraveyardBadlands2", "display": "Badlands", "areaId": 56, "hideWorld": 0, },189: { "worldId": 15, "name": "MirageHub", "display": "Hub", "areaId": 1, "hideWorld": 0, },190: { "worldId": 15, "name": "MirageColiseum", "display": "Coliseum", "areaId": 2, "hideWorld": 0, },191: { "worldId": 15, "name": "MirageArena1", "display": "Arena", "areaId": 3, "hideWorld": 0, },192: { "worldId": 15, "name": "MirageBadlands", "display": "Badlands", "areaId": 4, "hideWorld": 0, },193: { "worldId": 15, "name": "MiragePinball", "display": "Pinball", "areaId": 5, "hideWorld": 0, },194: { "worldId": 15, "name": "MirageShipHub", "display": "Ship Hub", "areaId": 6, "hideWorld": 0, },195: { "worldId": 15, "name": "MirageMousehole", "display": "Mousehole", "areaId": 7, "hideWorld": 0, },196: { "worldId": 15, "name": "MirageForest", "display": "Forest", "areaId": 8, "hideWorld": 0, },197: { "worldId": 15, "name": "MirageSkull", "display": "Skull Rock", "areaId": 9, "hideWorld": 0, },198: { "worldId": 15, "name": "MirageChamber", "display": "Audience Chamber", "areaId": 10, "hideWorld": 0, },199: { "worldId": 15, "name": "MirageForecourt", "display": "Forecourt", "areaId": 11, "hideWorld": 0, },200: { "worldId": 15, "name": "MirageSummit", "display": "Summit", "areaId": 12, "hideWorld": 0, },201: { "worldId": 15, "name": "MirageDeck", "display": "Launch Deck", "areaId": 13, "hideWorld": 0, },202: { "worldId": 15, "name": "MirageExterior", "display": "Ship Exterior", "areaId": 14, "hideWorld": 0, },203: { "worldId": 15, "name": "MirageArena2", "display": "Arena", "areaId": 15, "hideWorld": 0, },204: { "worldId": 16, "name": "CommandDeparture", "display": "The Land of Departure Command Board", "areaId": 1, "hideWorld": 1, },205: { "worldId": 16, "name": "CommandCinderella", "display": "Cinderella Command Board", "areaId": 3, "hideWorld": 1, },206: { "worldId": 16, "name": "CommandSitch", "display": "Lilo and Stitch Command Board", "areaId": 9, "hideWorld": 1, },207: { "worldId": 16, "name": "CommandPan", "display": "Peter Pan Command Board", "areaId": 11, "hideWorld": 1, },208: { "worldId": 16, "name": "CommandDisney", "display": "Disney Castle Command Board", "areaId": 12, "hideWorld": 1, },209: { "worldId": 16, "name": "CommandPooh", "display": "Winnie the Pooh Command Board", "areaId": 18, "hideWorld": 1, },210: { "worldId": 16, "name": "CommandPan2", "display": "Peter Pan Command Board", "areaId": 19, "hideWorld": 1, },211: { "worldId": 17, "name": "WorldMap", "display": "World Map", "areaId": 1, "hideWorld": 1, },212: { "worldId": 15, "name": "MirageMonstro", "display": "Prankster’s Paradise", "areaId": 17, "hideWorld": 0, },</v>
+        <v>0: { "worldId": 255, "name": "Title", "display": "On the title screen…", "areaId": 255, "hideWorld": 1, },1: { "worldId": 1, "name": "DepartureForecourtDay", "display": "Forecourt", "areaId": 1, "hideWorld": 0, },2: { "worldId": 1, "name": "DepartureGreatHall", "display": "Great Hall", "areaId": 2, "hideWorld": 0, },3: { "worldId": 1, "name": "VentusRoomDay", "display": "Ventus’s Room", "areaId": 3, "hideWorld": 0, },4: { "worldId": 1, "name": "VentusRoomNight", "display": "Ventus’s Room", "areaId": 4, "hideWorld": 0, },6: { "worldId": 1, "name": "DepartureMountainPath", "display": "Mountain Path", "areaId": 5, "hideWorld": 0, },7: { "worldId": 1, "name": "DepartureSummitNight", "display": "Summit", "areaId": 6, "hideWorld": 0, },8: { "worldId": 1, "name": "DepartureForecourtNight", "display": "Forecourt", "areaId": 7, "hideWorld": 0, },9: { "worldId": 1, "name": "DepartureForecourtRuins", "display": "Forecourt", "areaId": 8, "hideWorld": 0, },10: { "worldId": 1, "name": "DepartureGreatHallRuins", "display": "Great Hall", "areaId": 9, "hideWorld": 0, },11: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 10, "hideWorld": 0, },12: { "worldId": 1, "name": "ChamberOfWaking", "display": "Chamber of Waking", "areaId": 11, "hideWorld": 0, },13: { "worldId": 1, "name": "CastleOblivion", "display": "Castle Oblivion", "areaId": 12, "hideWorld": 0, },14: { "worldId": 1, "name": "CharacterSelect", "display": "Selecting a character…", "areaId": 13, "hideWorld": 1, },15: { "worldId": 1, "name": "DepartureForecourtRuins2", "display": "Forecourt", "areaId": 14, "hideWorld": 0, },16: { "worldId": 1, "name": "DepartureMountainPathRuins", "display": "Mountain Path", "areaId": 15, "hideWorld": 0, },17: { "worldId": 1, "name": "DepartureSummitRuins", "display": "Summit", "areaId": 16, "hideWorld": 0, },18: { "worldId": 2, "name": "DwarfMineEntrance", "display": "Mine Entrance", "areaId": 1, "hideWorld": 0, },19: { "worldId": 2, "name": "DwarfMine", "display": "The Mine", "areaId": 2, "hideWorld": 0, },20: { "worldId": 2, "name": "DwarfVault", "display": "Vault", "areaId": 3, "hideWorld": 0, },21: { "worldId": 2, "name": "DwarfMirrorChamber", "display": "Magic Mirror Chamber", "areaId": 4, "hideWorld": 0, },22: { "worldId": 2, "name": "DwarfWaterway", "display": "Underground Waterway", "areaId": 5, "hideWorld": 0, },23: { "worldId": 2, "name": "DwarfCourtyard", "display": "Courtyard", "areaId": 6, "hideWorld": 0, },24: { "worldId": 2, "name": "DwarfGlade", "display": "Flower Glade", "areaId": 7, "hideWorld": 0, },25: { "worldId": 2, "name": "DwarfWoods", "display": "Deep Woods", "areaId": 8, "hideWorld": 0, },26: { "worldId": 2, "name": "DwarfMirror", "display": "Inside the Magic Mirror", "areaId": 9, "hideWorld": 0, },27: { "worldId": 2, "name": "DwarfClearing", "display": "Cottage Clearing", "areaId": 10, "hideWorld": 0, },28: { "worldId": 2, "name": "DwarfCottage", "display": "The Cottage", "areaId": 11, "hideWorld": 0, },29: { "worldId": 2, "name": "DwarfMountainTrail", "display": "Mountain Trail", "areaId": 12, "hideWorld": 0, },30: { "worldId": 3, "name": "CastleRoom", "display": "Cinderella’s Room", "areaId": 1, "hideWorld": 0, },31: { "worldId": 3, "name": "CastleMousehole", "display": "Mousehole", "areaId": 2, "hideWorld": 0, },32: { "worldId": 3, "name": "CastleWardrobe", "display": "Wardrobe Room", "areaId": 3, "hideWorld": 0, },33: { "worldId": 3, "name": "CastleEntrance", "display": "Entrance", "areaId": 4, "hideWorld": 0, },34: { "worldId": 3, "name": "CastleChateau", "display": "The Chateau", "areaId": 5, "hideWorld": 0, },35: { "worldId": 3, "name": "CastleForest", "display": "Forest", "areaId": 6, "hideWorld": 0, },36: { "worldId": 3, "name": "CastleCourtyard", "display": "Palace Courtyard", "areaId": 7, "hideWorld": 0, },37: { "worldId": 3, "name": "CastleCorridor", "display": "Corridor", "areaId": 8, "hideWorld": 0, },38: { "worldId": 3, "name": "CastleBallroom", "display": "Ballroom", "areaId": 9, "hideWorld": 0, },39: { "worldId": 3, "name": "CastleFoyer", "display": "Foyer", "areaId": 10, "hideWorld": 0, },40: { "worldId": 3, "name": "CastlePassage", "display": "Passage", "areaId": 11, "hideWorld": 0, },41: { "worldId": 3, "name": "CastleAntechamber", "display": "Antechamber", "areaId": 12, "hideWorld": 0, },42: { "worldId": 3, "name": "CastleWardrobe2", "display": "Wardrobe Room", "areaId": 13, "hideWorld": 0, },43: { "worldId": 3, "name": "CastleMousehole2", "display": "Mousehole", "areaId": 14, "hideWorld": 0, },44: { "worldId": 3, "name": "CastleWardrobe3", "display": "Wardrobe Room", "areaId": 15, "hideWorld": 0, },45: { "worldId": 4, "name": "EnchantedDungeonCell", "display": "Dungeon Cell", "areaId": 1, "hideWorld": 0, },46: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 2, "hideWorld": 0, },47: { "worldId": 4, "name": "EnchantedThrone", "display": "Maleficent’s Throne", "areaId": 3, "hideWorld": 0, },48: { "worldId": 4, "name": "EnchantedDungeon", "display": "Dungeon", "areaId": 4, "hideWorld": 0, },49: { "worldId": 4, "name": "EnchantedHall1", "display": "Hall", "areaId": 5, "hideWorld": 0, },50: { "worldId": 4, "name": "EnchantedMountain", "display": "Forbidden Mountain", "areaId": 6, "hideWorld": 0, },51: { "worldId": 4, "name": "EnchantedWaterside", "display": "Waterside", "areaId": 7, "hideWorld": 0, },52: { "worldId": 4, "name": "EnchantedClearing", "display": "Forest Clearing", "areaId": 8, "hideWorld": 0, },53: { "worldId": 4, "name": "EnchantedBridge", "display": "Bridge", "areaId": 9, "hideWorld": 0, },54: { "worldId": 4, "name": "EnchantedBridgeThorns", "display": "Bridge", "areaId": 10, "hideWorld": 0, },55: { "worldId": 4, "name": "EnchantedAudience1", "display": "Audience Chamber", "areaId": 11, "hideWorld": 0, },56: { "worldId": 4, "name": "EnchantedAudience2", "display": "Audience Chamber", "areaId": 12, "hideWorld": 0, },57: { "worldId": 4, "name": "EnchantedReserved", "display": "Somewhere in the World…", "areaId": 13, "hideWorld": 1, },58: { "worldId": 4, "name": "EnchantedHallway", "display": "Hallway", "areaId": 14, "hideWorld": 0, },59: { "worldId": 4, "name": "EnchantedAurora", "display": "Aurora’s Chamber", "areaId": 15, "hideWorld": 0, },60: { "worldId": 4, "name": "EnchantedTower", "display": "Tower Room", "areaId": 16, "hideWorld": 0, },61: { "worldId": 4, "name": "EnchantedHall2", "display": "Hall", "areaId": 17, "hideWorld": 0, },62: { "worldId": 4, "name": "EnchantedAurora2", "display": "Aurora’s Chamber", "areaId": 18, "hideWorld": 0, },63: { "worldId": 4, "name": "EnchantedHall3", "display": "Hall", "areaId": 19, "hideWorld": 0, },64: { "worldId": 4, "name": "EnchantedHall4", "display": "Hall", "areaId": 20, "hideWorld": 0, },65: { "worldId": 4, "name": "EnchantedHall5", "display": "Hall", "areaId": 21, "hideWorld": 0, },66: { "worldId": 4, "name": "EnchantedHall6", "display": "Hall", "areaId": 22, "hideWorld": 0, },67: { "worldId": 4, "name": "EnchantedHall7", "display": "Hall", "areaId": 23, "hideWorld": 0, },68: { "worldId": 4, "name": "EnchantedHall8", "display": "Hall", "areaId": 24, "hideWorld": 0, },69: { "worldId": 4, "name": "EnchantedHall9", "display": "Hall", "areaId": 25, "hideWorld": 0, },70: { "worldId": 4, "name": "EnchantedHall10", "display": "Hall", "areaId": 26, "hideWorld": 0, },71: { "worldId": 4, "name": "EnchantedHall11", "display": "Hall", "areaId": 27, "hideWorld": 0, },72: { "worldId": 4, "name": "EnchantedHall12", "display": "Hall", "areaId": 28, "hideWorld": 0, },73: { "worldId": 4, "name": "EnchantedHall13", "display": "Hall", "areaId": 29, "hideWorld": 0, },74: { "worldId": 4, "name": "EnchantedHall14", "display": "Hall", "areaId": 30, "hideWorld": 0, },75: { "worldId": 4, "name": "EnchantedHall15", "display": "Hall", "areaId": 31, "hideWorld": 0, },76: { "worldId": 4, "name": "EnchantedHall16", "display": "Hall", "areaId": 32, "hideWorld": 0, },77: { "worldId": 4, "name": "EnchantedHall17", "display": "Hall", "areaId": 33, "hideWorld": 0, },78: { "worldId": 4, "name": "EnchantedHall18", "display": "Hall", "areaId": 34, "hideWorld": 0, },79: { "worldId": 4, "name": "EnchantedHall19", "display": "Hall", "areaId": 35, "hideWorld": 0, },80: { "worldId": 4, "name": "EnchantedHall20", "display": "Hall", "areaId": 36, "hideWorld": 0, },81: { "worldId": 4, "name": "EnchantedHall21", "display": "Hall", "areaId": 37, "hideWorld": 0, },82: { "worldId": 4, "name": "EnchantedHall22", "display": "Hall", "areaId": 38, "hideWorld": 0, },83: { "worldId": 4, "name": "EnchantedGates", "display": "Gates", "areaId": 39, "hideWorld": 0, },84: { "worldId": 5, "name": "MysteriousChamber", "display": "Sorcerer’s Chamber", "areaId": 1, "hideWorld": 0, },85: { "worldId": 5, "name": "MysteriousTower", "display": "Mysterious Tower", "areaId": 2, "hideWorld": 0, },86: { "worldId": 5, "name": "MysteriousEntrance", "display": "Tower Entrance", "areaId": 3, "hideWorld": 0, },87: { "worldId": 5, "name": "MysteriousChamber2", "display": "Sorcerer’s Chamber", "areaId": 4, "hideWorld": 0, },88: { "worldId": 6, "name": "RadiantOuterGardens", "display": "Outer Gardens", "areaId": 1, "hideWorld": 0, },89: { "worldId": 6, "name": "RadiantEntryway", "display": "Entryway", "areaId": 2, "hideWorld": 0, },90: { "worldId": 6, "name": "RadiantCentral", "display": "Central Square", "areaId": 3, "hideWorld": 0, },91: { "worldId": 6, "name": "RadiantAqueduct", "display": "Aqueduct", "areaId": 4, "hideWorld": 0, },92: { "worldId": 6, "name": "RadiantTown", "display": "Castle Town", "areaId": 5, "hideWorld": 0, },93: { "worldId": 6, "name": "RadiantReactor", "display": "Reactor", "areaId": 6, "hideWorld": 0, },94: { "worldId": 6, "name": "RadiantFountain", "display": "Fountain Court", "areaId": 7, "hideWorld": 0, },95: { "worldId": 6, "name": "RadiantMerlin", "display": "Merlin’s House", "areaId": 8, "hideWorld": 0, },96: { "worldId": 6, "name": "RadiantGardens", "display": "Gardens", "areaId": 9, "hideWorld": 0, },97: { "worldId": 6, "name": "RadiantDoors", "display": "Front Doors", "areaId": 10, "hideWorld": 0, },98: { "worldId": 6, "name": "RadiantPurification", "display": "Purification Facility", "areaId": 11, "hideWorld": 0, },99: { "worldId": 6, "name": "RadiantOuterGardens2", "display": "Outer Gardens", "areaId": 12, "hideWorld": 0, },100: { "worldId": 6, "name": "RadiantCentralDark", "display": "Central Square", "areaId": 13, "hideWorld": 0, },101: { "worldId": 6, "name": "RadiantCentralTerranort", "display": "Central Square", "areaId": 14, "hideWorld": 0, },102: { "worldId": 7, "name": "LouieCourt", "display": "Louie’s Ruins (Court)", "areaId": 1, "hideWorld": 0, },103: { "worldId": 7, "name": "LouiePath", "display": "Louie’s Ruins (Path)", "areaId": 2, "hideWorld": 0, },104: { "worldId": 7, "name": "Crossroad", "display": "Crossroad", "areaId": 3, "hideWorld": 0, },105: { "worldId": 7, "name": "UGRuinsEntrance", "display": "Underground Ruins (Entrance)", "areaId": 4, "hideWorld": 0, },106: { "worldId": 7, "name": "UGRuinsPassage1", "display": "Underground Ruins (Passage)", "areaId": 5, "hideWorld": 0, },107: { "worldId": 7, "name": "UGRuinsPassage2", "display": "Underground Ruins (Passage)", "areaId": 6, "hideWorld": 0, },108: { "worldId": 7, "name": "UGCourtyard", "display": "Underground Courtyard", "areaId": 7, "hideWorld": 0, },109: { "worldId": 7, "name": "JungleNearRuins", "display": "Jungle Near Ruins", "areaId": 8, "hideWorld": 0, },110: { "worldId": 7, "name": "Eminence", "display": "Eminence", "areaId": 9, "hideWorld": 0, },111: { "worldId": 7, "name": "Jungle", "display": "Jungle", "areaId": 10, "hideWorld": 0, },112: { "worldId": 7, "name": "River", "display": "Man-Village River", "areaId": 11, "hideWorld": 0, },113: { "worldId": 7, "name": "Bog", "display": "Bog", "areaId": 12, "hideWorld": 0, },114: { "worldId": 7, "name": "LanesBetween", "display": "The Lanes Between", "areaId": 50, "hideWorld": 0, },115: { "worldId": 7, "name": "Blank", "display": "Blank", "areaId": 51, "hideWorld": 0, },116: { "worldId": 7, "name": "Realm of Darkness", "display": "The Realm of Darkness", "areaId": 52, "hideWorld": 1, },117: { "worldId": 8, "name": "OlympusGates", "display": "Coliseum Gates", "areaId": 1, "hideWorld": 0, },118: { "worldId": 8, "name": "OlympusVestibule", "display": "Vestibule", "areaId": 2, "hideWorld": 0, },119: { "worldId": 8, "name": "OlympusWest", "display": "West Bracket", "areaId": 3, "hideWorld": 0, },120: { "worldId": 8, "name": "OlympusEast", "display": "East Bracket", "areaId": 4, "hideWorld": 0, },121: { "worldId": 8, "name": "OlympusTown", "display": "Town Near Thebes", "areaId": 5, "hideWorld": 0, },122: { "worldId": 8, "name": "OlympusEastNight", "display": "East Bracket", "areaId": 6, "hideWorld": 0, },123: { "worldId": 9, "name": "SpaceTuroBlock", "display": "Turo Prison Block", "areaId": 1, "hideWorld": 0, },124: { "worldId": 9, "name": "SpaceTuroTransporter", "display": "Turo Transporter", "areaId": 2, "hideWorld": 0, },125: { "worldId": 9, "name": "SpaceDurgonTransporter", "display": "Durgon Transporter", "areaId": 3, "hideWorld": 0, },126: { "worldId": 9, "name": "SpaceCorridor", "display": "Ship Corridor", "areaId": 4, "hideWorld": 0, },127: { "worldId": 9, "name": "SpaceControl", "display": "Control Room", "areaId": 5, "hideWorld": 0, },128: { "worldId": 9, "name": "SpacePod", "display": "Containment Pod", "areaId": 6, "hideWorld": 0, },129: { "worldId": 9, "name": "SpaceHub", "display": "Ship Hub", "areaId": 7, "hideWorld": 0, },130: { "worldId": 9, "name": "SpaceMachineryBay", "display": "Machinery Bay", "areaId": 8, "hideWorld": 0, },131: { "worldId": 9, "name": "SpaceLaunch", "display": "Launch Deck", "areaId": 9, "hideWorld": 0, },132: { "worldId": 9, "name": "SpaceExterior", "display": "Ship Exterior", "areaId": 10, "hideWorld": 0, },133: { "worldId": 9, "name": "SpaceOuter", "display": "Outer Space", "areaId": 11, "hideWorld": 0, },134: { "worldId": 9, "name": "SpaceCorridor2", "display": "Ship Corridor", "areaId": 12, "hideWorld": 0, },135: { "worldId": 9, "name": "SpaceLanesBetween", "display": "The Lanes Between", "areaId": 13, "hideWorld": 0, },136: { "worldId": 9, "name": "SpaceMachineryBayAccess", "display": "Machinery Bay Access", "areaId": 14, "hideWorld": 0, },137: { "worldId": 10, "name": "DestinyBeachDay", "display": "Island Beach", "areaId": 1, "hideWorld": 0, },138: { "worldId": 10, "name": "DestinyBeachSunset", "display": "Island Beach", "areaId": 2, "hideWorld": 0, },139: { "worldId": 10, "name": "DestinyBeachNight", "display": "Island Beach", "areaId": 3, "hideWorld": 0, },140: { "worldId": 10, "name": "DestinyMainIsland", "display": "Main Island Beach", "areaId": 4, "hideWorld": 0, },141: { "worldId": 11, "name": "NeverlandCove", "display": "Cove", "areaId": 1, "hideWorld": 0, },142: { "worldId": 11, "name": "NeverlandCliff", "display": "Cliff Path", "areaId": 2, "hideWorld": 0, },143: { "worldId": 11, "name": "NeverlandLagoon", "display": "Mermaid Lagoon", "areaId": 3, "hideWorld": 0, },144: { "worldId": 11, "name": "NeverlandSeacoast", "display": "Seacoast", "areaId": 4, "hideWorld": 0, },145: { "worldId": 11, "name": "NeverlandClearing", "display": "Jungle Clearing", "areaId": 5, "hideWorld": 0, },146: { "worldId": 11, "name": "NeverlandHideout", "display": "Peter’s Hideout", "areaId": 6, "hideWorld": 0, },147: { "worldId": 11, "name": "NeverlandGully", "display": "Gully", "areaId": 7, "hideWorld": 0, },148: { "worldId": 11, "name": "NeverlandCamp", "display": "Indian Camp", "areaId": 8, "hideWorld": 0, },149: { "worldId": 11, "name": "NeverlandBase", "display": "Rainbow Falls: Base", "areaId": 9, "hideWorld": 0, },150: { "worldId": 11, "name": "NeverlandAscent", "display": "Rainbow Falls: Ascent", "areaId": 10, "hideWorld": 0, },151: { "worldId": 11, "name": "NeverlandCrest", "display": "Rainbow Falls: Crest", "areaId": 11, "hideWorld": 0, },152: { "worldId": 11, "name": "NeverlandSkullEntrance", "display": "Skull Rock: Entrance", "areaId": 12, "hideWorld": 0, },153: { "worldId": 11, "name": "NeverlandSkullCavern", "display": "Skull Rock: Cavern", "areaId": 13, "hideWorld": 0, },154: { "worldId": 11, "name": "NeverlandSky", "display": "Night Sky", "areaId": 14, "hideWorld": 0, },155: { "worldId": 12, "name": "DisneyLibrary", "display": "Library", "areaId": 1, "hideWorld": 0, },156: { "worldId": 12, "name": "DisneyPlaza", "display": "Main Plaza", "areaId": 2, "hideWorld": 0, },157: { "worldId": 12, "name": "DisneyFruitballCourt", "display": "Fruitball Course", "areaId": 3, "hideWorld": 0, },158: { "worldId": 12, "name": "DisneyCountryChase", "display": "Country Chase", "areaId": 4, "hideWorld": 0, },159: { "worldId": 12, "name": "DisneyRaceway", "display": "Raceway", "areaId": 5, "hideWorld": 0, },160: { "worldId": 12, "name": "DisneyGizmo", "display": "Gizmo Gallery", "areaId": 6, "hideWorld": 0, },161: { "worldId": 12, "name": "DisneyRecRoom", "display": "Pete’s Rec Room", "areaId": 7, "hideWorld": 0, },162: { "worldId": 12, "name": "DisneyDrive", "display": "Disney Drive", "areaId": 8, "hideWorld": 0, },163: { "worldId": 12, "name": "DisneySpree", "display": "Grand Spree", "areaId": 9, "hideWorld": 0, },164: { "worldId": 12, "name": "DisneyCastle", "display": "Castle Circuit", "areaId": 10, "hideWorld": 0, },165: { "worldId": 12, "name": "DisneyLanesBetween", "display": "The Lanes Between", "areaId": 11, "hideWorld": 0, },166: { "worldId": 12, "name": "DisneyRegistration", "display": "Raceway Registration", "areaId": 12, "hideWorld": 0, },167: { "worldId": 12, "name": "DisneyIceCream", "display": "Ice Cream", "areaId": 13, "hideWorld": 0, },168: { "worldId": 12, "name": "DisneyFruitball", "display": "Fruitball", "areaId": 14, "hideWorld": 0, },169: { "worldId": 12, "name": "DisneyCourseCastle", "display": "Race: Castle Course", "areaId": 15, "hideWorld": 0, },170: { "worldId": 13, "name": "GraveyardBadlands", "display": "Badlands", "areaId": 1, "hideWorld": 0, },171: { "worldId": 13, "name": "GraveyardWar", "display": "Seat of War", "areaId": 2, "hideWorld": 0, },172: { "worldId": 13, "name": "GraveyardTwister", "display": "Twister Trench", "areaId": 3, "hideWorld": 0, },173: { "worldId": 13, "name": "GraveyardEye1", "display": "Eye of the Storm", "areaId": 4, "hideWorld": 0, },174: { "worldId": 13, "name": "GraveyardEye2", "display": "Eye of the Storm", "areaId": 5, "hideWorld": 0, },175: { "worldId": 13, "name": "GraveyardEye3", "display": "Eye of the Storm", "areaId": 6, "hideWorld": 0, },176: { "worldId": 13, "name": "GraveyardFissure", "display": "Fissure", "areaId": 7, "hideWorld": 0, },177: { "worldId": 13, "name": "Graveyard1", "display": "Keyblade Graveyard", "areaId": 8, "hideWorld": 1, },178: { "worldId": 13, "name": "Graveyard2", "display": "Keyblade Graveyard", "areaId": 9, "hideWorld": 1, },179: { "worldId": 13, "name": "Graveyard3", "display": "Keyblade Graveyard", "areaId": 10, "hideWorld": 1, },180: { "worldId": 13, "name": "GraveyardCage", "display": "Will’s Cage", "areaId": 11, "hideWorld": 0, },181: { "worldId": 13, "name": "Graveyard4", "display": "Keyblade Graveyard", "areaId": 12, "hideWorld": 1, },182: { "worldId": 13, "name": "VentusHeart1", "display": "Ventus’s Heart", "areaId": 50, "hideWorld": 0, },183: { "worldId": 13, "name": "VentusHeart2", "display": "Ventus’s Heart", "areaId": 51, "hideWorld": 0, },184: { "worldId": 13, "name": "VentusHeart3", "display": "Ventus’s Heart", "areaId": 52, "hideWorld": 0, },185: { "worldId": 13, "name": "SoraHeart", "display": "Sora’s Heart", "areaId": 53, "hideWorld": 0, },186: { "worldId": 13, "name": "TerraHeart", "display": "Terra’s Heart", "areaId": 54, "hideWorld": 0, },187: { "worldId": 13, "name": "Graveyard5", "display": "Keyblade Graveyard", "areaId": 55, "hideWorld": 0, },188: { "worldId": 13, "name": "GraveyardBadlands2", "display": "Badlands", "areaId": 56, "hideWorld": 0, },189: { "worldId": 15, "name": "MirageHub", "display": "Hub", "areaId": 1, "hideWorld": 0, },190: { "worldId": 15, "name": "MirageColiseum", "display": "Coliseum", "areaId": 2, "hideWorld": 0, },191: { "worldId": 15, "name": "MirageArena1", "display": "Arena", "areaId": 3, "hideWorld": 0, },192: { "worldId": 15, "name": "MirageBadlands", "display": "Badlands", "areaId": 4, "hideWorld": 0, },193: { "worldId": 15, "name": "MiragePinball", "display": "Pinball", "areaId": 5, "hideWorld": 0, },194: { "worldId": 15, "name": "MirageShipHub", "display": "Ship Hub", "areaId": 6, "hideWorld": 0, },195: { "worldId": 15, "name": "MirageMousehole", "display": "Mousehole", "areaId": 7, "hideWorld": 0, },196: { "worldId": 15, "name": "MirageForest", "display": "Forest", "areaId": 8, "hideWorld": 0, },197: { "worldId": 15, "name": "MirageSkull", "display": "Skull Rock", "areaId": 9, "hideWorld": 0, },198: { "worldId": 15, "name": "MirageChamber", "display": "Audience Chamber", "areaId": 10, "hideWorld": 0, },199: { "worldId": 15, "name": "MirageForecourt", "display": "Forecourt", "areaId": 11, "hideWorld": 0, },200: { "worldId": 15, "name": "MirageSummit", "display": "Summit", "areaId": 12, "hideWorld": 0, },201: { "worldId": 15, "name": "MirageDeck", "display": "Launch Deck", "areaId": 13, "hideWorld": 0, },202: { "worldId": 15, "name": "MirageExterior", "display": "Ship Exterior", "areaId": 14, "hideWorld": 0, },203: { "worldId": 15, "name": "MirageArena2", "display": "Arena", "areaId": 15, "hideWorld": 0, },204: { "worldId": 16, "name": "CommandDeparture", "display": "The Land of Departure Command Board", "areaId": 1, "hideWorld": 1, },205: { "worldId": 16, "name": "CommandCinderella", "display": "Cinderella Command Board", "areaId": 3, "hideWorld": 1, },206: { "worldId": 16, "name": "CommandSitch", "display": "Lilo and Stitch Command Board", "areaId": 9, "hideWorld": 1, },207: { "worldId": 16, "name": "CommandPan", "display": "Peter Pan Command Board", "areaId": 11, "hideWorld": 1, },208: { "worldId": 16, "name": "CommandDisney", "display": "Disney Castle Command Board", "areaId": 12, "hideWorld": 1, },209: { "worldId": 16, "name": "CommandPooh", "display": "Winnie the Pooh Command Board", "areaId": 18, "hideWorld": 1, },210: { "worldId": 16, "name": "CommandPan2", "display": "Peter Pan Command Board", "areaId": 19, "hideWorld": 1, },211: { "worldId": 17, "name": "WorldMap", "display": "World Map", "areaId": 1, "hideWorld": 1, },212: { "worldId": 15, "name": "MirageMonstro", "display": "Prankster’s Paradise", "areaId": 17, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3789,7 +3789,7 @@
       </c>
       <c r="G31" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A31,": { ""worldId"": ",C31,", ""name"": """,D31,""", ""display"": """,E31,""", ""areaId"": ",B31,", ""hideWorld"": ",F31,", },")</f>
-        <v>30: { "worldId": 3, "name": "CastleHouse", "display": "Cinderella’s House", "areaId": 1, "hideWorld": 0, },</v>
+        <v>30: { "worldId": 3, "name": "CastleRoom", "display": "Cinderella’s Room", "areaId": 1, "hideWorld": 0, },</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8178,13 +8178,13 @@
   </sheetPr>
   <dimension ref="A1:N227"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="K229" activeCellId="0" sqref="K229"/>
+      <selection pane="bottomLeft" activeCell="J229" activeCellId="0" sqref="J229"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.12109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -16644,7 +16644,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C108"/>
+  <autoFilter ref="C1:C108"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added achievements up until the end of Enchanted Dominion in Ven's story
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1822" uniqueCount="864">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="866">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -2618,6 +2618,12 @@
   </si>
   <si>
     <t xml:space="preserve">Situational</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x145</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Joint Force</t>
   </si>
 </sst>
 </file>
@@ -2739,7 +2745,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3031,11 +3037,11 @@
   </sheetPr>
   <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A17" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.47265625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8176,15 +8182,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N227"/>
+  <dimension ref="A1:N228"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="J229" activeCellId="0" sqref="J229"/>
+      <selection pane="bottomLeft" activeCell="L228" activeCellId="0" sqref="L228"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -8237,7 +8243,7 @@
       </c>
       <c r="N1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L2:L1013)</f>
-        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16643,8 +16649,47 @@
         <v>0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
+    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A228" s="0" t="s">
+        <v>864</v>
+      </c>
+      <c r="B228" s="0" t="s">
+        <v>865</v>
+      </c>
+      <c r="C228" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="D228" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="E228" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F228" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="G228" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="H228" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I228" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J228" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K228" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L228" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A228,": { ""id"": ",A228,", ""name"": """,B228,""", ""category"": """,C228,""", ""slots"": ",E228,", ""type"": """,G228,""", ""tier"": ",I228,", ""healsHp"": ",J228,", ""equippableBattleCommand"": ",K228,", ""supercategory"": """,D228,""", ""element"": """,F228,""" },")</f>
+        <v>0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="C1:C108"/>
+  <autoFilter ref="A1:C108"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added achievements up to the end of Olympus Coliseum in Ven's story
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1828" uniqueCount="866">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="868">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -2618,6 +2618,12 @@
   </si>
   <si>
     <t xml:space="preserve">Situational</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x13e</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Swing Slash</t>
   </si>
   <si>
     <t xml:space="preserve">0x145</t>
@@ -2745,7 +2751,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.89453125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3041,7 +3047,7 @@
       <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.48828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8182,7 +8188,7 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N228"/>
+  <dimension ref="A1:N229"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
@@ -8190,7 +8196,7 @@
       <selection pane="bottomLeft" activeCell="L228" activeCellId="0" sqref="L228"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -8242,8 +8248,8 @@
         <v>24</v>
       </c>
       <c r="N1" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(L2:L1013)</f>
-        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+        <f aca="false">_xlfn.CONCAT(L2:L1014)</f>
+        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13e: { "id": 0x13e, "name": "Swing Slash", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16685,11 +16691,50 @@
       </c>
       <c r="L228" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A228,": { ""id"": ",A228,", ""name"": """,B228,""", ""category"": """,C228,""", ""slots"": ",E228,", ""type"": """,G228,""", ""tier"": ",I228,", ""healsHp"": ",J228,", ""equippableBattleCommand"": ",K228,", ""supercategory"": """,D228,""", ""element"": """,F228,""" },")</f>
+        <v>0x13e: { "id": 0x13e, "name": "Swing Slash", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+      </c>
+    </row>
+    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A229" s="0" t="s">
+        <v>866</v>
+      </c>
+      <c r="B229" s="0" t="s">
+        <v>867</v>
+      </c>
+      <c r="C229" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="D229" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="E229" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F229" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="G229" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="H229" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I229" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J229" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K229" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L229" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A229,": { ""id"": ",A229,", ""name"": """,B229,""", ""category"": """,C229,""", ""slots"": ",E229,", ""type"": """,G229,""", ""tier"": ",I229,", ""healsHp"": ",J229,", ""equippableBattleCommand"": ",K229,", ""supercategory"": """,D229,""", ""element"": """,F229,""" },")</f>
         <v>0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C108"/>
+  <autoFilter ref="C1:C108"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added achievements up to the end of Deep Space for Ven's story
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$108</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$108</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1834" uniqueCount="868">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1840" uniqueCount="870">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -2624,6 +2624,12 @@
   </si>
   <si>
     <t xml:space="preserve">Swing Slash</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x140</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Astro Strike</t>
   </si>
   <si>
     <t xml:space="preserve">0x145</t>
@@ -2751,7 +2757,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9296875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3044,10 +3050,10 @@
   <dimension ref="A1:I213"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D32" activeCellId="0" sqref="D32"/>
+      <selection pane="topLeft" activeCell="R166" activeCellId="0" sqref="R166"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.5078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.5234375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8188,15 +8194,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N229"/>
+  <dimension ref="A1:N230"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A203" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L228" activeCellId="0" sqref="L228"/>
+      <selection pane="bottomLeft" activeCell="K231" activeCellId="0" sqref="K231"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.171875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.19140625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -8248,8 +8254,8 @@
         <v>24</v>
       </c>
       <c r="N1" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(L2:L1014)</f>
-        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13e: { "id": 0x13e, "name": "Swing Slash", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+        <f aca="false">_xlfn.CONCAT(L2:L1015)</f>
+        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13e: { "id": 0x13e, "name": "Swing Slash", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x140: { "id": 0x140, "name": "Astro Strike", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -16730,11 +16736,50 @@
       </c>
       <c r="L229" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A229,": { ""id"": ",A229,", ""name"": """,B229,""", ""category"": """,C229,""", ""slots"": ",E229,", ""type"": """,G229,""", ""tier"": ",I229,", ""healsHp"": ",J229,", ""equippableBattleCommand"": ",K229,", ""supercategory"": """,D229,""", ""element"": """,F229,""" },")</f>
+        <v>0x140: { "id": 0x140, "name": "Astro Strike", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+      </c>
+    </row>
+    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A230" s="0" t="s">
+        <v>868</v>
+      </c>
+      <c r="B230" s="0" t="s">
+        <v>869</v>
+      </c>
+      <c r="C230" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="D230" s="0" t="s">
+        <v>863</v>
+      </c>
+      <c r="E230" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F230" s="0" t="s">
+        <v>547</v>
+      </c>
+      <c r="G230" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="H230" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I230" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J230" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K230" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L230" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A230,": { ""id"": ",A230,", ""name"": """,B230,""", ""category"": """,C230,""", ""slots"": ",E230,", ""type"": """,G230,""", ""tier"": ",I230,", ""healsHp"": ",J230,", ""equippableBattleCommand"": ",K230,", ""supercategory"": """,D230,""", ""element"": """,F230,""" },")</f>
         <v>0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C108"/>
+  <autoFilter ref="A1:C108"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Added achievements up to the end of Radiant Garden in Aqua's story
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$119</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$119</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$119</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$119</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1918" uniqueCount="896">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1924" uniqueCount="898">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -2708,6 +2708,12 @@
   </si>
   <si>
     <t xml:space="preserve">Astro Strike</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0x141</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Holy Burst</t>
   </si>
   <si>
     <t xml:space="preserve">0x145</t>
@@ -2835,7 +2841,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.9765625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.9921875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3127,11 +3133,11 @@
   </sheetPr>
   <dimension ref="A1:I213"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A131" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="R166" activeCellId="0" sqref="R166"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A70" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="X82" activeCellId="0" sqref="X82"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="4.76"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8272,15 +8278,15 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:N243"/>
+  <dimension ref="A1:N244"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <pane xSplit="0" ySplit="1" topLeftCell="A209" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="L4" activeCellId="0" sqref="L4"/>
+      <selection pane="bottomLeft" activeCell="G246" activeCellId="0" sqref="G246"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.23828125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.25390625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -8332,8 +8338,8 @@
         <v>24</v>
       </c>
       <c r="N1" s="0" t="str">
-        <f aca="false">_xlfn.CONCAT(L2:L1028)</f>
-        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x13: { "id": 0x13, "name": "Spellweaver", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x17: { "id": 0x17, "name": "Thunderbolt", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x2f: { "id": 0x2f, "name": "Last Charge", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x3d: { "id": 0x3d, "name": "Finish (Ventus)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x40: { "id": 0x40, "name": "Air Flair 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x43: { "id": 0x43, "name": "Heat Slash 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Fire" },0x45: { "id": 0x45, "name": "Air Flair 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4c: { "id": 0x4c, "name": "Air Flair 3", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x52: { "id": 0x52, "name": "Air Flair 4", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x57: { "id": 0x57, "name": "Celebration", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x58: { "id": 0x58, "name": "Stratosphere", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x139: { "id": 0x139, "name": "Saber Counter", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13d: { "id": 0x13d, "name": "Selfless Prince", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "N/A" },0x13e: { "id": 0x13e, "name": "Swing Slash", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x140: { "id": 0x140, "name": "Astro Strike", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+        <f aca="false">_xlfn.CONCAT(L2:L1029)</f>
+        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x13: { "id": 0x13, "name": "Spellweaver", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x17: { "id": 0x17, "name": "Thunderbolt", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x2f: { "id": 0x2f, "name": "Last Charge", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x3d: { "id": 0x3d, "name": "Finish (Ventus)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x40: { "id": 0x40, "name": "Air Flair 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x43: { "id": 0x43, "name": "Heat Slash 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Fire" },0x45: { "id": 0x45, "name": "Air Flair 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4c: { "id": 0x4c, "name": "Air Flair 3", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x52: { "id": 0x52, "name": "Air Flair 4", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x57: { "id": 0x57, "name": "Celebration", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x58: { "id": 0x58, "name": "Stratosphere", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Guard", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x139: { "id": 0x139, "name": "Saber Counter", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13d: { "id": 0x13d, "name": "Selfless Prince", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "N/A" },0x13e: { "id": 0x13e, "name": "Swing Slash", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x140: { "id": 0x140, "name": "Astro Strike", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x141: { "id": 0x141, "name": "Holy Burst", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -17360,11 +17366,50 @@
       </c>
       <c r="L243" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A243,": { ""id"": ",A243,", ""name"": """,B243,""", ""category"": """,C243,""", ""slots"": ",E243,", ""type"": """,G243,""", ""tier"": ",I243,", ""healsHp"": ",J243,", ""equippableBattleCommand"": ",K243,", ""supercategory"": """,D243,""", ""element"": """,F243,""" },")</f>
+        <v>0x141: { "id": 0x141, "name": "Holy Burst", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+      </c>
+    </row>
+    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A244" s="0" t="s">
+        <v>896</v>
+      </c>
+      <c r="B244" s="0" t="s">
+        <v>897</v>
+      </c>
+      <c r="C244" s="0" t="s">
+        <v>885</v>
+      </c>
+      <c r="D244" s="0" t="s">
+        <v>885</v>
+      </c>
+      <c r="E244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="F244" s="0" t="s">
+        <v>394</v>
+      </c>
+      <c r="G244" s="0" t="s">
+        <v>384</v>
+      </c>
+      <c r="H244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="I244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="J244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="K244" s="0" t="n">
+        <v>0</v>
+      </c>
+      <c r="L244" s="0" t="str">
+        <f aca="false">_xlfn.CONCAT( ,A244,": { ""id"": ",A244,", ""name"": """,B244,""", ""category"": """,C244,""", ""slots"": ",E244,", ""type"": """,G244,""", ""tier"": ",I244,", ""healsHp"": ",J244,", ""equippableBattleCommand"": ",K244,", ""supercategory"": """,D244,""", ""element"": """,F244,""" },")</f>
         <v>0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C119"/>
+  <autoFilter ref="A1:C119"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Certain command issues resolved
* * "Ribbon of Terracotta" and "Severe Frostbite": Illusion commands were incorrectly categorized as non-equippable battle commands. This has been corrected.
* "Prime Sacrifice": Updated the description to clarify that only non-Illusion battle commands are considered. The current toolset is not robust enough to check for multiple clusters of commands  resulting from the above fix (Illusion commands are the only equippable battle commands in their own cluster, and this cannot be worked around).
* "Rainbow Loom": Fixed an issue where multi-slot commands would count as duplicates.
* A missed syntax error was corrected.
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -13,8 +13,8 @@
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$127</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$127</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$127</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$127</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -2931,7 +2931,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.07421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3223,11 +3223,11 @@
   </sheetPr>
   <dimension ref="A1:I220"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A19" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6796875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8757,13 +8757,13 @@
   </sheetPr>
   <dimension ref="A1:N253"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A186" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="B212" activeCellId="0" sqref="B212"/>
+      <selection pane="bottomLeft" activeCell="I172" activeCellId="0" sqref="I172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.3359375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -8816,7 +8816,7 @@
       </c>
       <c r="N1" s="0" t="str">
         <f aca="false">_xlfn.CONCAT(L2:L1038)</f>
-        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x13: { "id": 0x13, "name": "Spellweaver", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x17: { "id": 0x17, "name": "Thunderbolt", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x2f: { "id": 0x2f, "name": "Last Charge", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x3d: { "id": 0x3d, "name": "Finish (Ventus)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x3e: { "id": 0x3e, "name": "Finish (Aqua)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x40: { "id": 0x40, "name": "Air Flair 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x41: { "id": 0x41, "name": "Magic Pulse 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x43: { "id": 0x43, "name": "Heat Slash 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Fire" },0x45: { "id": 0x45, "name": "Air Flair 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x46: { "id": 0x46, "name": "Magic Pulse 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x48: { "id": 0x48, "name": "Heat Slash 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Fire" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4c: { "id": 0x4c, "name": "Air Flair 3", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x4d: { "id": 0x4d, "name": "Magic Pulse 3", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x52: { "id": 0x52, "name": "Air Flair 4", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x53: { "id": 0x53, "name": "Magic Pulse 4", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x56: { "id": 0x56, "name": "Ice Burst", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Blizzard" },0x57: { "id": 0x57, "name": "Celebration", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x58: { "id": 0x58, "name": "Stratosphere", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x59: { "id": 0x59, "name": "Teleport Spike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x139: { "id": 0x139, "name": "Saber Counter", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13d: { "id": 0x13d, "name": "Selfless Prince", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "N/A" },0x13e: { "id": 0x13e, "name": "Swing Slash", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x140: { "id": 0x140, "name": "Astro Strike", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x141: { "id": 0x141, "name": "Holy Burst", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x142: { "id": 0x142, "name": "Dual Limit", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
+        <v>0xFFFF: { "id": 0xFFFF, "name": "N/A", "category": "N/A", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "N/A", "element": "N/A" },0x13: { "id": 0x13, "name": "Spellweaver", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x17: { "id": 0x17, "name": "Thunderbolt", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x2f: { "id": 0x2f, "name": "Last Charge", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x3d: { "id": 0x3d, "name": "Finish (Ventus)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x3e: { "id": 0x3e, "name": "Finish (Aqua)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x3f: { "id": 0x3f, "name": "Finish (Terra)", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x40: { "id": 0x40, "name": "Air Flair 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x41: { "id": 0x41, "name": "Magic Pulse 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x42: { "id": 0x42, "name": "Rising Rock 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x43: { "id": 0x43, "name": "Heat Slash 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Fire" },0x45: { "id": 0x45, "name": "Air Flair 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x46: { "id": 0x46, "name": "Magic Pulse 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x47: { "id": 0x47, "name": "Rising Rock 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x48: { "id": 0x48, "name": "Heat Slash 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Fire" },0x49: { "id": 0x49, "name": "Ramuh’s Judgment", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Thunder" },0x4a: { "id": 0x4a, "name": "Twisted Hours", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4b: { "id": 0x4b, "name": "Surprise! 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4c: { "id": 0x4c, "name": "Air Flair 3", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x4d: { "id": 0x4d, "name": "Magic Pulse 3", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x4e: { "id": 0x4e, "name": "Dark Star 1", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x4f: { "id": 0x4f, "name": "Heal Strike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x50: { "id": 0x50, "name": "Random End", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x51: { "id": 0x51, "name": "Surprise! 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x52: { "id": 0x52, "name": "Air Flair 4", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x53: { "id": 0x53, "name": "Magic Pulse 4", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x54: { "id": 0x54, "name": "Dark Star 2", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x55: { "id": 0x55, "name": "Explosion", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x56: { "id": 0x56, "name": "Ice Burst", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Blizzard" },0x57: { "id": 0x57, "name": "Celebration", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x58: { "id": 0x58, "name": "Stratosphere", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x59: { "id": 0x59, "name": "Teleport Spike", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Null" },0x5a: { "id": 0x5a, "name": "Demolition", "category": "Finish", "slots": 0, "type": "Finish", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Finish", "element": "Physical" },0x5b: { "id": 0x5b, "name": "Quick Blitz", "category": "Attack", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5c: { "id": 0x5c, "name": "Blitz", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5d: { "id": 0x5d, "name": "Magic Hour", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5e: { "id": 0x5e, "name": "Meteor Crash", "category": "Ranged", "slots": 2, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x5f: { "id": 0x5f, "name": "Sliding Dash", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x60: { "id": 0x60, "name": "Fire Dash", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x61: { "id": 0x61, "name": "Dark Haze", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x62: { "id": 0x62, "name": "Sonic Blade", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x63: { "id": 0x63, "name": "Chaos Blade", "category": "Melee", "slots": 2, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Dark" },0x64: { "id": 0x64, "name": "Zantetsuken", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x65: { "id": 0x65, "name": "Strike Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x66: { "id": 0x66, "name": "Freeze Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x67: { "id": 0x67, "name": "Treasure Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x68: { "id": 0x68, "name": "Spark Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x69: { "id": 0x69, "name": "Wind Raid", "category": "Ranged", "slots": 1, "type": "Raid", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6a: { "id": 0x6a, "name": "Fire Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x6b: { "id": 0x6b, "name": "Barrier Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6c: { "id": 0x6c, "name": "Thunder Surge", "category": "Melee", "slots": 1, "type": "Rush", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Thunder" },0x6d: { "id": 0x6d, "name": "Aerial Slam", "category": "Melee", "slots": 1, "type": "Jump", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6e: { "id": 0x6e, "name": "Ars Solum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x6f: { "id": 0x6f, "name": "Ars Arcanum", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x70: { "id": 0x70, "name": "Time Splicer", "category": "Melee", "slots": 2, "type": "Chain Hit", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x71: { "id": 0x71, "name": "Poison Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x72: { "id": 0x72, "name": "Wishing Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x73: { "id": 0x73, "name": "Blizzard Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Blizzard" },0x74: { "id": 0x74, "name": "Stun Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x75: { "id": 0x75, "name": "Slot Edge", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x76: { "id": 0x76, "name": "Fire Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Fire" },0x77: { "id": 0x77, "name": "Confuse Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x78: { "id": 0x78, "name": "Binding Strike", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x79: { "id": 0x79, "name": "Tornado Strike", "category": "Melee", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7a: { "id": 0x7a, "name": "Brutal Blast", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7b: { "id": 0x7b, "name": "Magnet Spiral", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7c: { "id": 0x7c, "name": "Salvation", "category": "Ranged", "slots": 2, "type": "Strike", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7d: { "id": 0x7d, "name": "Wind Cutter", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7e: { "id": 0x7e, "name": "Limit Storm", "category": "Melee", "slots": 1, "type": "Strike", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x7f: { "id": 0x7f, "name": "Collision Magnet", "category": "Hybrid", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x80: { "id": 0x80, "name": "Geo Impact", "category": "Melee", "slots": 2, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x81: { "id": 0x81, "name": "Sacrifice", "category": "Melee", "slots": 1, "type": "Blade", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "Physical" },0x82: { "id": 0x82, "name": "Break Time", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Attack", "element": "N/A" },0x83: { "id": 0x83, "name": "Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x84: { "id": 0x84, "name": "Fira", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x85: { "id": 0x85, "name": "Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x86: { "id": 0x86, "name": "Dark Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Dark" },0x87: { "id": 0x87, "name": "Fission Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x88: { "id": 0x88, "name": "Triple Firaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x89: { "id": 0x89, "name": "Crawling Fire", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0x8a: { "id": 0x8a, "name": "Blizzard", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8b: { "id": 0x8b, "name": "Blizzara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8c: { "id": 0x8c, "name": "Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8d: { "id": 0x8d, "name": "Triple Blizzaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0x8e: { "id": 0x8e, "name": "Thunder", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x8f: { "id": 0x8f, "name": "Thundara", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x90: { "id": 0x90, "name": "Thundaga", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x91: { "id": 0x91, "name": "Thundaga Shot", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Thunder" },0x92: { "id": 0x92, "name": "Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x93: { "id": 0x93, "name": "Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x94: { "id": 0x94, "name": "Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x95: { "id": 0x95, "name": "Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "N/A" },0x96: { "id": 0x96, "name": "Mine Shield", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x97: { "id": 0x97, "name": "Mine Square", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x98: { "id": 0x98, "name": "Seeker Mine", "category": "Mine", "slots": 1, "type": "Detonate", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x99: { "id": 0x99, "name": "Zero Gravity", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9a: { "id": 0x9a, "name": "Zero Gravira", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9b: { "id": 0x9b, "name": "Zero Graviga", "category": "Ranged", "slots": 1, "type": "Zero Gravity", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9c: { "id": 0x9c, "name": "Magnet", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9d: { "id": 0x9d, "name": "Magnera", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9e: { "id": 0x9e, "name": "Magnega", "category": "Ranged", "slots": 1, "type": "Magnet", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0x9f: { "id": 0x9f, "name": "Munny Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa0: { "id": 0xa0, "name": "Energy Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa1: { "id": 0xa1, "name": "D-Link Magnet", "category": "Support", "slots": 1, "type": "Magnet", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa2: { "id": 0xa2, "name": "Aero", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa3: { "id": 0xa3, "name": "Aerora", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa4: { "id": 0xa4, "name": "Aeroga", "category": "Ranged", "slots": 1, "type": "Aero", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa5: { "id": 0xa5, "name": "Warp", "category": "Ranged", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa6: { "id": 0xa6, "name": "Faith", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xa7: { "id": 0xa7, "name": "Deep Freeze", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa8: { "id": 0xa8, "name": "Glacier", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xa9: { "id": 0xa9, "name": "Ice Barrage", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Blizzard" },0xaa: { "id": 0xaa, "name": "Firaga Burst", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xab: { "id": 0xab, "name": "Raging Storm", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xac: { "id": 0xac, "name": "Mega Flare", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xad: { "id": 0xad, "name": "Quake", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xae: { "id": 0xae, "name": "Tornado", "category": "Ranged", "slots": 2, "type": "Aero", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xaf: { "id": 0xaf, "name": "Meteor", "category": "Ranged", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb0: { "id": 0xb0, "name": "Transcendence", "category": "Ranged", "slots": 2, "type": "Zero Gravity", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb1: { "id": 0xb1, "name": "Mini", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb2: { "id": 0xb2, "name": "Blackout", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb3: { "id": 0xb3, "name": "Ignite", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Fire" },0xb4: { "id": 0xb4, "name": "Confuse", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb5: { "id": 0xb5, "name": "Bind", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb6: { "id": 0xb6, "name": "Poison", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb7: { "id": 0xb7, "name": "Slow", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb8: { "id": 0xb8, "name": "Stop", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xb9: { "id": 0xb9, "name": "Stopra", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 2, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xba: { "id": 0xba, "name": "Stopga", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 3, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbb: { "id": 0xbb, "name": "Sleep", "category": "Status", "slots": 1, "type": "Status Effect", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Magic", "element": "Null" },0xbc: { "id": 0xbc, "name": "Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbd: { "id": 0xbd, "name": "Hi-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbe: { "id": 0xbe, "name": "Mega-Potion", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xbf: { "id": 0xbf, "name": "Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc0: { "id": 0xc0, "name": "Mega-Ether", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc1: { "id": 0xc1, "name": "Panacea", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc2: { "id": 0xc2, "name": "Elixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc3: { "id": 0xc3, "name": "Megalixir", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc4: { "id": 0xc4, "name": "Balloon Letter", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc5: { "id": 0xc5, "name": "Vanilla Glitz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc6: { "id": 0xc6, "name": "Fabracadabra", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc7: { "id": 0xc7, "name": "Honeybunny", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc8: { "id": 0xc8, "name": "Bueno Volcano", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xc9: { "id": 0xc9, "name": "Snow Bear", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xca: { "id": 0xca, "name": "Spark Lemon", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcb: { "id": 0xcb, "name": "Goofy Parfait", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcc: { "id": 0xcc, "name": "Royalberry", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcd: { "id": 0xcd, "name": "Milky Way", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xce: { "id": 0xce, "name": "Rockin’ Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xcf: { "id": 0xcf, "name": "Donald Fizz", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd0: { "id": 0xd0, "name": "Space Mint", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd1: { "id": 0xd1, "name": "Big Bad Pete", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd2: { "id": 0xd2, "name": "Double Crunch", "category": "Item", "slots": 1, "type": "Item", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Item", "element": "N/A" },0xd3: { "id": 0xd3, "name": "Group Cure", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd4: { "id": 0xd4, "name": "Group Cura", "category": "Support", "slots": 1, "type": "Cure", "tier": 2, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd5: { "id": 0xd5, "name": "Group Curaga", "category": "Support", "slots": 1, "type": "Cure", "tier": 3, "healsHp": 1, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd6: { "id": 0xd6, "name": "Group Esuna", "category": "Support", "slots": 1, "type": "Cure", "tier": 1, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd7: { "id": 0xd7, "name": "Confetti", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd8: { "id": 0xd8, "name": "Fireworks", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xd9: { "id": 0xd9, "name": "Taunt", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xda: { "id": 0xda, "name": "Victory Pose", "category": "Friendship", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdb: { "id": 0xdb, "name": "Deck Scramble", "category": "Melee", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdc: { "id": 0xdc, "name": "Vanish", "category": "Support", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdd: { "id": 0xdd, "name": "Unison Rush", "category": "Melee", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xde: { "id": 0xde, "name": "Voltage Stack", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xdf: { "id": 0xdf, "name": "Trinity Limit", "category": "Ranged", "slots": 3, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xe0: { "id": 0xe0, "name": "Gold", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe1: { "id": 0xe1, "name": "Black", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe2: { "id": 0xe2, "name": "Finish (Dummy)", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe3: { "id": 0xe3, "name": "Wrath of Darkness", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe4: { "id": 0xe4, "name": "Sign of Faith", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xe5: { "id": 0xe5, "name": "Wish Circle", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe6: { "id": 0xe6, "name": "Enchanted Step", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe7: { "id": 0xe7, "name": "Wish Shot", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe8: { "id": 0xe8, "name": "Magic Mending", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xe9: { "id": 0xe9, "name": "Doc", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xea: { "id": 0xea, "name": "Grumpy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xeb: { "id": 0xeb, "name": "Sneezy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xec: { "id": 0xec, "name": "Happy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xed: { "id": 0xed, "name": "Sleepy", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xee: { "id": 0xee, "name": "Bashful", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xef: { "id": 0xef, "name": "Dopey", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf0: { "id": 0xf0, "name": "Dark Spiral", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf1: { "id": 0xf1, "name": "Dark Splicer", "category": "D-Link", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "D-Link", "element": "N/A" },0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },0xf7: { "id": 0xf7, "name": "Dummy", "category": "Dummy", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0xf8: { "id": 0xf8, "name": "Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xf9: { "id": 0xf9, "name": "Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfa: { "id": 0xfa, "name": "High Jump", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfb: { "id": 0xfb, "name": "Dodge Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfc: { "id": 0xfc, "name": "Thunder Roll", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Thunder" },0xfd: { "id": 0xfd, "name": "Cartwheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0xfe: { "id": 0xfe, "name": "Firewheel", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0xff: { "id": 0xff, "name": "Air Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x100: { "id": 0x100, "name": "Ice Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x101: { "id": 0x101, "name": "Reversal", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x102: { "id": 0x102, "name": "Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x103: { "id": 0x103, "name": "Superglide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x104: { "id": 0x104, "name": "Fire Glide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Fire" },0x105: { "id": 0x105, "name": "Homing Slide", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x106: { "id": 0x106, "name": "Teleport", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x107: { "id": 0x107, "name": "Sonic Impact", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "Physical" },0x108: { "id": 0x108, "name": "Doubleflight", "category": "Movement", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Movement", "element": "N/A" },0x109: { "id": 0x109, "name": "Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10a: { "id": 0x10a, "name": "Renewal Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10b: { "id": 0x10b, "name": "Focus Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10c: { "id": 0x10c, "name": "Stun Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10d: { "id": 0x10d, "name": "Poison Block", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10e: { "id": 0x10e, "name": "Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x10f: { "id": 0x10f, "name": "Renewal Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 1, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x110: { "id": 0x110, "name": "Focus Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x111: { "id": 0x111, "name": "Confuse Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x112: { "id": 0x112, "name": "Stop Barrier", "category": "Defense", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Defense", "element": "N/A" },0x113: { "id": 0x113, "name": "Counter Rush", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x114: { "id": 0x114, "name": "Counter Hammer", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x115: { "id": 0x115, "name": "Reversal Slash", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x116: { "id": 0x116, "name": "Counter Barrier", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x117: { "id": 0x117, "name": "Payback Raid", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x118: { "id": 0x118, "name": "Payback Surge", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x119: { "id": 0x119, "name": "Payback Fang", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11a: { "id": 0x11a, "name": "Aerial Recovery", "category": "Reprisal", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Reprisal", "element": "N/A" },0x11b: { "id": 0x11b, "name": "Shotlock", "category": "Dummy", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Dummy", "element": "N/A" },0x11c: { "id": 0x11c, "name": "Meteor Shower", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11d: { "id": 0x11d, "name": "Flame Salvo", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Fire" },0x11e: { "id": 0x11e, "name": "Chaos Snake", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x11f: { "id": 0x11f, "name": "Bubble Blaster", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x120: { "id": 0x120, "name": "Dark Volley", "category": "Shotlock", "slots": 1, "type": "Blaster", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Dark" },0x121: { "id": 0x121, "name": "Ragnarok", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x122: { "id": 0x122, "name": "Thunderstorm", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x123: { "id": 0x123, "name": "Bio Barrage", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x124: { "id": 0x124, "name": "Prism Rain", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x125: { "id": 0x125, "name": "Pulse Bomb", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Thunder" },0x126: { "id": 0x126, "name": "Photon Charge", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x127: { "id": 0x127, "name": "Absolute Zero", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Blizzard" },0x128: { "id": 0x128, "name": "Lightning Ray", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x129: { "id": 0x129, "name": "Sonic Shadow", "category": "Shotlock", "slots": 1, "type": "Rave", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12a: { "id": 0x12a, "name": "Dark Link", "category": "Shotlock", "slots": 1, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "N/A" },0x12b: { "id": 0x12b, "name": "Ultima Cannon", "category": "Shotlock", "slots": 1, "type": "Ragnarok", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12c: { "id": 0x12c, "name": "Lightbloom", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x12d: { "id": 0x12d, "name": "Multivortex", "category": "Shotlock", "slots": 1, "type": "Spin", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Shotlock", "element": "Null" },0x139: { "id": 0x139, "name": "Saber Counter", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13c: { "id": 0x13c, "name": "White Calm", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x13d: { "id": 0x13d, "name": "Selfless Prince", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "N/A" },0x13e: { "id": 0x13e, "name": "Swing Slash", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x140: { "id": 0x140, "name": "Astro Strike", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x141: { "id": 0x141, "name": "Holy Burst", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x142: { "id": 0x142, "name": "Dual Limit", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },0x145: { "id": 0x145, "name": "Joint Force", "category": "Situational", "slots": 0, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Situational", "element": "Null" },</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15793,11 +15793,11 @@
         <v>0</v>
       </c>
       <c r="K186" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L186" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A186,": { ""id"": ",A186,", ""name"": """,B186,""", ""category"": """,C186,""", ""slots"": ",E186,", ""type"": """,G186,""", ""tier"": ",I186,", ""healsHp"": ",J186,", ""equippableBattleCommand"": ",K186,", ""supercategory"": """,D186,""", ""element"": """,F186,""" },")</f>
-        <v>0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
+        <v>0xf2: { "id": 0xf2, "name": "Illusion-L", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15829,11 +15829,11 @@
         <v>0</v>
       </c>
       <c r="K187" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L187" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A187,": { ""id"": ",A187,", ""name"": """,B187,""", ""category"": """,C187,""", ""slots"": ",E187,", ""type"": """,G187,""", ""tier"": ",I187,", ""healsHp"": ",J187,", ""equippableBattleCommand"": ",K187,", ""supercategory"": """,D187,""", ""element"": """,F187,""" },")</f>
-        <v>0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
+        <v>0xf3: { "id": 0xf3, "name": "Illusion-F", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15865,11 +15865,11 @@
         <v>0</v>
       </c>
       <c r="K188" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L188" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A188,": { ""id"": ",A188,", ""name"": """,B188,""", ""category"": """,C188,""", ""slots"": ",E188,", ""type"": """,G188,""", ""tier"": ",I188,", ""healsHp"": ",J188,", ""equippableBattleCommand"": ",K188,", ""supercategory"": """,D188,""", ""element"": """,F188,""" },")</f>
-        <v>0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
+        <v>0xf4: { "id": 0xf4, "name": "Illusion-V", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15901,11 +15901,11 @@
         <v>0</v>
       </c>
       <c r="K189" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L189" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A189,": { ""id"": ",A189,", ""name"": """,B189,""", ""category"": """,C189,""", ""slots"": ",E189,", ""type"": """,G189,""", ""tier"": ",I189,", ""healsHp"": ",J189,", ""equippableBattleCommand"": ",K189,", ""supercategory"": """,D189,""", ""element"": """,F189,""" },")</f>
-        <v>0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
+        <v>0xf5: { "id": 0xf5, "name": "Illusion-R", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -15937,11 +15937,11 @@
         <v>0</v>
       </c>
       <c r="K190" s="0" t="n">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="L190" s="0" t="str">
         <f aca="false">_xlfn.CONCAT( ,A190,": { ""id"": ",A190,", ""name"": """,B190,""", ""category"": """,C190,""", ""slots"": ",E190,", ""type"": """,G190,""", ""tier"": ",I190,", ""healsHp"": ",J190,", ""equippableBattleCommand"": ",K190,", ""supercategory"": """,D190,""", ""element"": """,F190,""" },")</f>
-        <v>0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 0, "supercategory": "Friendship", "element": "N/A" },</v>
+        <v>0xf6: { "id": 0xf6, "name": "Illusion-B", "category": "Friendship", "slots": 2, "type": "N/A", "tier": 0, "healsHp": 0, "equippableBattleCommand": 1, "supercategory": "Friendship", "element": "N/A" },</v>
       </c>
     </row>
     <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18237,7 +18237,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C127"/>
+  <autoFilter ref="A1:C127"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>

</xml_diff>

<commit_message>
Balanced two of Terra's endgame achievements and the Coliseum achievements
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -5,16 +5,17 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Locations" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
+    <sheet name="Stats - Terra" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$127</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$127</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$127</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$127</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -26,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1992" uniqueCount="928">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="941">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -2810,14 +2811,54 @@
   </si>
   <si>
     <t xml:space="preserve">Joint Force</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Level</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulated LV</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Strength Mod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Magic Mod</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulated STR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulated MAG</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Simulated DEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enemy HP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Enemy DEF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damage Taken per Physical Hit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Damage Taken per Magical Hit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Total Hits</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="164" formatCode="General"/>
+    <numFmt numFmtId="165" formatCode="General"/>
   </numFmts>
   <fonts count="5">
     <font>
@@ -2891,7 +2932,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -2902,6 +2943,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -2931,7 +2976,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.09375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3227,7 +3272,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.6953125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8757,13 +8802,13 @@
   </sheetPr>
   <dimension ref="A1:N253"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="I172" activeCellId="0" sqref="I172"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.35546875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -18237,7 +18282,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:C127"/>
+  <autoFilter ref="C1:C127"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -18247,4 +18292,930 @@
   </headerFooter>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I100"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.55"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <f aca="true">INDIRECT(ADDRESS(F2 + 1, 2)) + G2</f>
+        <v>21</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <f aca="true">INDIRECT(ADDRESS(F2 + 1, 3)) + H2</f>
+        <v>7</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <f aca="true">INDIRECT(ADDRESS(F2 + 1, 4))</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>700</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">MAX(MIN(F5-G8, 25), 1)</f>
+        <v>7</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">MAX(MIN(G5-G8, 25), 1)</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">MIN(F8/H8, F8/I8)</f>
+        <v>100</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Additional rebalancing to most of the rest of Terra's challenge achievements
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
@@ -14,8 +14,9 @@
     <sheet name="Stats - Terra" sheetId="4" state="visible" r:id="rId5"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$C$1:$C$127</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$D$1:$D$253</definedName>
     <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$127</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Commands!$C$1:$C$127</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -2976,7 +2977,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3272,7 +3273,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.71484375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8802,13 +8803,13 @@
   </sheetPr>
   <dimension ref="A1:N253"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <pane xSplit="0" ySplit="1" topLeftCell="A155" activePane="bottomLeft" state="frozen"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
-      <selection pane="bottomLeft" activeCell="I172" activeCellId="0" sqref="I172"/>
+      <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.37109375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -18282,7 +18283,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="C1:C127"/>
+  <autoFilter ref="D1:D253"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -18301,13 +18302,17 @@
   </sheetPr>
   <dimension ref="A1:I100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.8"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.35"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.25"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.55"/>
@@ -18350,13 +18355,13 @@
         <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>15</v>
+        <v>7</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>10</v>
+        <v>1</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>-2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18411,7 +18416,7 @@
       </c>
       <c r="F5" s="3" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 2)) + G2</f>
-        <v>21</v>
+        <v>8</v>
       </c>
       <c r="G5" s="3" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 3)) + H2</f>
@@ -18419,7 +18424,7 @@
       </c>
       <c r="H5" s="3" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 4))</f>
-        <v>11</v>
+        <v>7</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18476,18 +18481,18 @@
         <v>7</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>700</v>
+        <v>300</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>14</v>
+        <v>4</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">MAX(MIN(F5-G8, 25), 1)</f>
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">MAX(MIN(G5-G8, 25), 1)</f>
-        <v>1</v>
+        <v>3</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18536,7 +18541,7 @@
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">MIN(F8/H8, F8/I8)</f>
-        <v>100</v>
+        <v>75</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Rebalanced more of Ven's late-game achievements
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -5,18 +5,19 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="4"/>
   </bookViews>
   <sheets>
     <sheet name="Worlds" sheetId="1" state="visible" r:id="rId2"/>
     <sheet name="Locations" sheetId="2" state="visible" r:id="rId3"/>
     <sheet name="Commands" sheetId="3" state="visible" r:id="rId4"/>
     <sheet name="Stats - Terra" sheetId="4" state="visible" r:id="rId5"/>
+    <sheet name="Stats - Ven" sheetId="5" state="visible" r:id="rId6"/>
   </sheets>
   <definedNames>
-    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$D$1:$D$253</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$127</definedName>
-    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0" vbProcedure="false">Commands!$C$1:$C$127</definedName>
+    <definedName function="false" hidden="true" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$A$1:$C$127</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase" vbProcedure="false">Commands!$D$1:$D$253</definedName>
+    <definedName function="false" hidden="false" localSheetId="2" name="_xlnm._FilterDatabase_0_0" vbProcedure="false">Commands!$C$1:$C$127</definedName>
   </definedNames>
   <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
   <extLst>
@@ -28,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2007" uniqueCount="941">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2022" uniqueCount="941">
   <si>
     <t xml:space="preserve">World ID</t>
   </si>
@@ -2977,7 +2978,7 @@
       <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.13671875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.15625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="20.01"/>
   </cols>
@@ -3273,7 +3274,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.7421875" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.7578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="5.88"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="25.56"/>
@@ -8803,13 +8804,13 @@
   </sheetPr>
   <dimension ref="A1:N253"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <pane xSplit="0" ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
       <selection pane="bottomLeft" activeCell="F24" activeCellId="0" sqref="F24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="12.40625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="12.42578125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="7.95"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="14.77"/>
@@ -18283,7 +18284,7 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="D1:D253"/>
+  <autoFilter ref="A1:C127"/>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
   <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
@@ -18303,10 +18304,10 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H21" activeCellId="0" sqref="H21"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.16"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
@@ -18355,7 +18356,7 @@
         <v>2</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="G2" s="0" t="n">
         <v>1</v>
@@ -18416,15 +18417,15 @@
       </c>
       <c r="F5" s="3" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 2)) + G2</f>
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="G5" s="3" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 3)) + H2</f>
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="H5" s="3" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 4))</f>
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18481,18 +18482,18 @@
         <v>7</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>300</v>
+        <v>400</v>
       </c>
       <c r="G8" s="0" t="n">
         <v>4</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">MAX(MIN(F5-G8, 25), 1)</f>
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">MAX(MIN(G5-G8, 25), 1)</f>
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18541,7 +18542,7 @@
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">MIN(F8/H8, F8/I8)</f>
-        <v>75</v>
+        <v>133.333333333333</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -18917,6 +18918,981 @@
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="n">
         <v>40</v>
+      </c>
+    </row>
+    <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A42" s="0" t="n">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A43" s="0" t="n">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A44" s="0" t="n">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A45" s="0" t="n">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A46" s="0" t="n">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A47" s="0" t="n">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A48" s="0" t="n">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A49" s="0" t="n">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A50" s="0" t="n">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A51" s="0" t="n">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A52" s="0" t="n">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A53" s="0" t="n">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A54" s="0" t="n">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A55" s="0" t="n">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A56" s="0" t="n">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A57" s="0" t="n">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A58" s="0" t="n">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A59" s="0" t="n">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A60" s="0" t="n">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A61" s="0" t="n">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A62" s="0" t="n">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A63" s="0" t="n">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A64" s="0" t="n">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A65" s="0" t="n">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="66" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A66" s="0" t="n">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="67" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A67" s="0" t="n">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="68" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A68" s="0" t="n">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="69" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A69" s="0" t="n">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="70" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A70" s="0" t="n">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="71" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A71" s="0" t="n">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="n">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="n">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="n">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="n">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="n">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="n">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="n">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="n">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="n">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="n">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="n">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="n">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="n">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="n">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A86" s="0" t="n">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A87" s="0" t="n">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A88" s="0" t="n">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A89" s="0" t="n">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="90" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A90" s="0" t="n">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="91" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A91" s="0" t="n">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="92" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A92" s="0" t="n">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="93" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A93" s="0" t="n">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A94" s="0" t="n">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="95" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A95" s="0" t="n">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="96" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A96" s="0" t="n">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="97" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A97" s="0" t="n">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="98" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A98" s="0" t="n">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="99" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A99" s="0" t="n">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="100" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A100" s="0" t="n">
+        <v>99</v>
+      </c>
+    </row>
+  </sheetData>
+  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
+  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <headerFooter differentFirst="false" differentOddEven="false">
+    <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
+    <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
+  </headerFooter>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+  <sheetPr filterMode="false">
+    <pageSetUpPr fitToPage="false"/>
+  </sheetPr>
+  <dimension ref="A1:I100"/>
+  <sheetViews>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <cols>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.16"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="8.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="6.71"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="8.38"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="13.82"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="14.35"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="28.25"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="27.55"/>
+  </cols>
+  <sheetData>
+    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A1" s="1" t="s">
+        <v>928</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>929</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>560</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>834</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>930</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>931</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>932</v>
+      </c>
+    </row>
+    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A2" s="0" t="n">
+        <v>1</v>
+      </c>
+      <c r="B2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C2" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D2" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="F2" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="G2" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="H2" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A3" s="0" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="C3" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D3" s="0" t="n">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A4" s="0" t="n">
+        <v>3</v>
+      </c>
+      <c r="B4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C4" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="D4" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>933</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>934</v>
+      </c>
+      <c r="H4" s="1" t="s">
+        <v>935</v>
+      </c>
+    </row>
+    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="B5" s="0" t="n">
+        <v>4</v>
+      </c>
+      <c r="C5" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D5" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F5" s="3" t="n">
+        <f aca="true">INDIRECT(ADDRESS(F2 + 1, 2)) + G2</f>
+        <v>26</v>
+      </c>
+      <c r="G5" s="3" t="n">
+        <f aca="true">INDIRECT(ADDRESS(F2 + 1, 3)) + H2</f>
+        <v>25</v>
+      </c>
+      <c r="H5" s="3" t="n">
+        <f aca="true">INDIRECT(ADDRESS(F2 + 1, 4))</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="B6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C6" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="D6" s="0" t="n">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="B7" s="0" t="n">
+        <v>5</v>
+      </c>
+      <c r="C7" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D7" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>936</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>937</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>938</v>
+      </c>
+      <c r="I7" s="1" t="s">
+        <v>939</v>
+      </c>
+    </row>
+    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="B8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C8" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D8" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="F8" s="0" t="n">
+        <v>550</v>
+      </c>
+      <c r="G8" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="H8" s="0" t="n">
+        <f aca="false">MAX(MIN(F5-G8, 25), 1)</f>
+        <v>12</v>
+      </c>
+      <c r="I8" s="0" t="n">
+        <f aca="false">MAX(MIN(G5-G8, 25), 1)</f>
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A9" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="B9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C9" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="D9" s="0" t="n">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="B10" s="0" t="n">
+        <v>6</v>
+      </c>
+      <c r="C10" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D10" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F10" s="1" t="s">
+        <v>940</v>
+      </c>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A11" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="B11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C11" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="D11" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="F11" s="0" t="n">
+        <f aca="false">MIN(F8/H8, F8/I8)</f>
+        <v>45.8333333333333</v>
+      </c>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A12" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="B12" s="0" t="n">
+        <v>7</v>
+      </c>
+      <c r="C12" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D12" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A13" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="B13" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C13" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="D13" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A14" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="B14" s="0" t="n">
+        <v>8</v>
+      </c>
+      <c r="C14" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D14" s="0" t="n">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A15" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="B15" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C15" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="D15" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A16" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="B16" s="0" t="n">
+        <v>9</v>
+      </c>
+      <c r="C16" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D16" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A17" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="B17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C17" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="D17" s="0" t="n">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A18" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="B18" s="0" t="n">
+        <v>10</v>
+      </c>
+      <c r="C18" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D18" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A19" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="B19" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C19" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="D19" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A20" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="B20" s="0" t="n">
+        <v>11</v>
+      </c>
+      <c r="C20" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D20" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A21" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="B21" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C21" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D21" s="0" t="n">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A22" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="B22" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C22" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="D22" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A23" s="0" t="n">
+        <v>22</v>
+      </c>
+      <c r="B23" s="0" t="n">
+        <v>12</v>
+      </c>
+      <c r="C23" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D23" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A24" s="0" t="n">
+        <v>23</v>
+      </c>
+      <c r="B24" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C24" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D24" s="0" t="n">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A25" s="0" t="n">
+        <v>24</v>
+      </c>
+      <c r="B25" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C25" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="D25" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A26" s="0" t="n">
+        <v>25</v>
+      </c>
+      <c r="B26" s="0" t="n">
+        <v>13</v>
+      </c>
+      <c r="C26" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D26" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A27" s="0" t="n">
+        <v>26</v>
+      </c>
+      <c r="B27" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C27" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="D27" s="0" t="n">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A28" s="0" t="n">
+        <v>27</v>
+      </c>
+      <c r="B28" s="0" t="n">
+        <v>14</v>
+      </c>
+      <c r="C28" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D28" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A29" s="0" t="n">
+        <v>28</v>
+      </c>
+      <c r="B29" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C29" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="D29" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A30" s="0" t="n">
+        <v>29</v>
+      </c>
+      <c r="B30" s="0" t="n">
+        <v>15</v>
+      </c>
+      <c r="C30" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D30" s="0" t="n">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A31" s="0" t="n">
+        <v>30</v>
+      </c>
+      <c r="B31" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C31" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="D31" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A32" s="0" t="n">
+        <v>31</v>
+      </c>
+      <c r="B32" s="0" t="n">
+        <v>16</v>
+      </c>
+      <c r="C32" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D32" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A33" s="0" t="n">
+        <v>32</v>
+      </c>
+      <c r="B33" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C33" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="D33" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A34" s="0" t="n">
+        <v>33</v>
+      </c>
+      <c r="B34" s="0" t="n">
+        <v>17</v>
+      </c>
+      <c r="C34" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D34" s="0" t="n">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A35" s="0" t="n">
+        <v>34</v>
+      </c>
+      <c r="B35" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C35" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="D35" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A36" s="0" t="n">
+        <v>35</v>
+      </c>
+      <c r="B36" s="0" t="n">
+        <v>18</v>
+      </c>
+      <c r="C36" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D36" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A37" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B37" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C37" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="D37" s="0" t="n">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A38" s="0" t="n">
+        <v>37</v>
+      </c>
+      <c r="B38" s="0" t="n">
+        <v>19</v>
+      </c>
+      <c r="C38" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D38" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A39" s="0" t="n">
+        <v>38</v>
+      </c>
+      <c r="B39" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C39" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="D39" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A40" s="0" t="n">
+        <v>39</v>
+      </c>
+      <c r="B40" s="0" t="n">
+        <v>20</v>
+      </c>
+      <c r="C40" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D40" s="0" t="n">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A41" s="0" t="n">
+        <v>40</v>
+      </c>
+      <c r="B41" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="C41" s="0" t="n">
+        <v>21</v>
+      </c>
+      <c r="D41" s="0" t="n">
+        <v>22</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>

<commit_message>
Update Kingdom Hearts Birth by Sleep Final Mix.xlsx
</commit_message>
<xml_diff>
--- a/Kingdom Hearts Birth by Sleep Final Mix.xlsx
+++ b/Kingdom Hearts Birth by Sleep Final Mix.xlsx
@@ -19234,7 +19234,7 @@
   <dimension ref="A1:I100"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D42" activeCellId="0" sqref="D42"/>
+      <selection pane="topLeft" activeCell="F2" activeCellId="0" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -19286,13 +19286,13 @@
         <v>3</v>
       </c>
       <c r="F2" s="0" t="n">
-        <v>38</v>
+        <v>14</v>
       </c>
       <c r="G2" s="0" t="n">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="H2" s="0" t="n">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19347,15 +19347,15 @@
       </c>
       <c r="F5" s="3" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 2)) + G2</f>
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="G5" s="3" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 3)) + H2</f>
-        <v>25</v>
+        <v>12</v>
       </c>
       <c r="H5" s="3" t="n">
         <f aca="true">INDIRECT(ADDRESS(F2 + 1, 4))</f>
-        <v>22</v>
+        <v>12</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19412,18 +19412,18 @@
         <v>7</v>
       </c>
       <c r="F8" s="0" t="n">
-        <v>550</v>
+        <v>200</v>
       </c>
       <c r="G8" s="0" t="n">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="H8" s="0" t="n">
         <f aca="false">MAX(MIN(F5-G8, 25), 1)</f>
-        <v>12</v>
+        <v>1</v>
       </c>
       <c r="I8" s="0" t="n">
         <f aca="false">MAX(MIN(G5-G8, 25), 1)</f>
-        <v>11</v>
+        <v>1</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -19472,7 +19472,7 @@
       </c>
       <c r="F11" s="0" t="n">
         <f aca="false">MIN(F8/H8, F8/I8)</f>
-        <v>45.8333333333333</v>
+        <v>200</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">

</xml_diff>